<commit_message>
feat: Assembleur python qui permet de traduire lamoitié du tableau d'instruction en binaire
</commit_message>
<xml_diff>
--- a/Encodage_PARM.xlsx
+++ b/Encodage_PARM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\habib\PROJARCHI\Projet-P-ARM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monsi\Desktop\Ecole\Polytech_Nice\Architecture\Projet-P-ARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B571AEA2-73FE-467D-BDE0-8BBB461B9A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AE8A59-CFD7-4022-B5A2-838A677C4960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2184" yWindow="1848" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encodage PARM" sheetId="1" r:id="rId1"/>
@@ -1352,6 +1352,123 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
       <extLst>
@@ -1400,18 +1517,6 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1420,111 +1525,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1853,7 +1853,7 @@
   <dimension ref="A1:AP54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E11" sqref="E11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1872,54 +1872,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="47"/>
-      <c r="C1" s="104" t="s">
+      <c r="C1" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="106"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="94"/>
       <c r="G1" s="48"/>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
       <c r="X1" s="49"/>
-      <c r="Y1" s="104" t="s">
+      <c r="Y1" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="105"/>
-      <c r="AA1" s="105"/>
-      <c r="AB1" s="113"/>
+      <c r="Z1" s="72"/>
+      <c r="AA1" s="72"/>
+      <c r="AB1" s="73"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" s="103"/>
+      <c r="A2" s="93"/>
       <c r="B2" s="45"/>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="82"/>
-      <c r="F2" s="80"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="75"/>
       <c r="G2" s="38"/>
       <c r="H2" s="3">
         <v>15</v>
@@ -2016,23 +2016,23 @@
       <c r="L3" s="32">
         <v>0</v>
       </c>
-      <c r="M3" s="73" t="s">
+      <c r="M3" s="89" t="s">
         <v>102</v>
       </c>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="107" t="s">
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="S3" s="108"/>
-      <c r="T3" s="109"/>
-      <c r="U3" s="85" t="s">
+      <c r="S3" s="80"/>
+      <c r="T3" s="81"/>
+      <c r="U3" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="V3" s="86"/>
-      <c r="W3" s="86"/>
+      <c r="V3" s="88"/>
+      <c r="W3" s="88"/>
       <c r="X3" s="39"/>
       <c r="Y3" s="35" t="b">
         <v>1</v>
@@ -2080,23 +2080,23 @@
       <c r="L4" s="12">
         <v>1</v>
       </c>
-      <c r="M4" s="73" t="s">
+      <c r="M4" s="89" t="s">
         <v>102</v>
       </c>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="110"/>
-      <c r="R4" s="107" t="s">
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="S4" s="108"/>
-      <c r="T4" s="109"/>
-      <c r="U4" s="85" t="s">
+      <c r="S4" s="80"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="88"/>
       <c r="X4" s="39"/>
       <c r="Y4" s="36" t="b">
         <v>1</v>
@@ -2144,23 +2144,23 @@
       <c r="L5" s="32">
         <v>0</v>
       </c>
-      <c r="M5" s="73" t="s">
+      <c r="M5" s="89" t="s">
         <v>103</v>
       </c>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="110"/>
-      <c r="R5" s="107" t="s">
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="90"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="S5" s="108"/>
-      <c r="T5" s="109"/>
-      <c r="U5" s="85" t="s">
+      <c r="S5" s="80"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="V5" s="86"/>
-      <c r="W5" s="86"/>
+      <c r="V5" s="88"/>
+      <c r="W5" s="88"/>
       <c r="X5" s="39"/>
       <c r="Y5" s="35" t="b">
         <v>1</v>
@@ -2181,9 +2181,9 @@
       </c>
       <c r="B6" s="45"/>
       <c r="C6" s="34"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="80"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="38"/>
       <c r="H6" s="3">
         <v>0</v>
@@ -2191,27 +2191,27 @@
       <c r="I6" s="1">
         <v>0</v>
       </c>
-      <c r="J6" s="80" t="s">
+      <c r="J6" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="81"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="78"/>
+      <c r="V6" s="78"/>
+      <c r="W6" s="78"/>
       <c r="X6" s="38"/>
-      <c r="Y6" s="101"/>
-      <c r="Z6" s="82"/>
-      <c r="AA6" s="82"/>
-      <c r="AB6" s="114"/>
+      <c r="Y6" s="76"/>
+      <c r="Z6" s="74"/>
+      <c r="AA6" s="74"/>
+      <c r="AB6" s="77"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
@@ -2252,21 +2252,21 @@
       <c r="N7" s="32">
         <v>0</v>
       </c>
-      <c r="O7" s="83" t="s">
+      <c r="O7" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="P7" s="84"/>
-      <c r="Q7" s="93"/>
-      <c r="R7" s="107" t="s">
+      <c r="P7" s="83"/>
+      <c r="Q7" s="84"/>
+      <c r="R7" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="S7" s="108"/>
-      <c r="T7" s="109"/>
-      <c r="U7" s="85" t="s">
+      <c r="S7" s="80"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="V7" s="86"/>
-      <c r="W7" s="86"/>
+      <c r="V7" s="88"/>
+      <c r="W7" s="88"/>
       <c r="X7" s="39"/>
       <c r="Y7" s="35" t="b">
         <v>1</v>
@@ -2320,21 +2320,21 @@
       <c r="N8" s="12">
         <v>1</v>
       </c>
-      <c r="O8" s="83" t="s">
+      <c r="O8" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="P8" s="84"/>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="107" t="s">
+      <c r="P8" s="83"/>
+      <c r="Q8" s="84"/>
+      <c r="R8" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="S8" s="108"/>
-      <c r="T8" s="109"/>
-      <c r="U8" s="85" t="s">
+      <c r="S8" s="80"/>
+      <c r="T8" s="81"/>
+      <c r="U8" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="V8" s="86"/>
-      <c r="W8" s="86"/>
+      <c r="V8" s="88"/>
+      <c r="W8" s="88"/>
       <c r="X8" s="39"/>
       <c r="Y8" s="36" t="b">
         <v>1</v>
@@ -2388,21 +2388,21 @@
       <c r="N9" s="32">
         <v>0</v>
       </c>
-      <c r="O9" s="73" t="s">
+      <c r="O9" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="110"/>
-      <c r="R9" s="107" t="s">
+      <c r="P9" s="90"/>
+      <c r="Q9" s="91"/>
+      <c r="R9" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="S9" s="108"/>
-      <c r="T9" s="109"/>
-      <c r="U9" s="85" t="s">
+      <c r="S9" s="80"/>
+      <c r="T9" s="81"/>
+      <c r="U9" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="V9" s="86"/>
-      <c r="W9" s="86"/>
+      <c r="V9" s="88"/>
+      <c r="W9" s="88"/>
       <c r="X9" s="39"/>
       <c r="Y9" s="35" t="b">
         <v>1</v>
@@ -2456,21 +2456,21 @@
       <c r="N10" s="12">
         <v>1</v>
       </c>
-      <c r="O10" s="73" t="s">
+      <c r="O10" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="110"/>
-      <c r="R10" s="107" t="s">
+      <c r="P10" s="90"/>
+      <c r="Q10" s="91"/>
+      <c r="R10" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="S10" s="108"/>
-      <c r="T10" s="109"/>
-      <c r="U10" s="85" t="s">
+      <c r="S10" s="80"/>
+      <c r="T10" s="81"/>
+      <c r="U10" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="V10" s="86"/>
-      <c r="W10" s="86"/>
+      <c r="V10" s="88"/>
+      <c r="W10" s="88"/>
       <c r="X10" s="39"/>
       <c r="Y10" s="36" t="b">
         <v>1</v>
@@ -2496,10 +2496,10 @@
       <c r="D11" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="73" t="s">
+      <c r="E11" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="F11" s="74"/>
+      <c r="F11" s="90"/>
       <c r="G11" s="39"/>
       <c r="H11" s="13">
         <v>0</v>
@@ -2516,21 +2516,21 @@
       <c r="L11" s="32">
         <v>0</v>
       </c>
-      <c r="M11" s="85" t="s">
+      <c r="M11" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="N11" s="86"/>
-      <c r="O11" s="87"/>
-      <c r="P11" s="73" t="s">
+      <c r="N11" s="88"/>
+      <c r="O11" s="95"/>
+      <c r="P11" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="74"/>
-      <c r="T11" s="74"/>
-      <c r="U11" s="74"/>
-      <c r="V11" s="74"/>
-      <c r="W11" s="74"/>
+      <c r="Q11" s="90"/>
+      <c r="R11" s="90"/>
+      <c r="S11" s="90"/>
+      <c r="T11" s="90"/>
+      <c r="U11" s="90"/>
+      <c r="V11" s="90"/>
+      <c r="W11" s="90"/>
       <c r="X11" s="39"/>
       <c r="Y11" s="35" t="b">
         <v>0</v>
@@ -2556,10 +2556,10 @@
       <c r="D12" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="73" t="s">
+      <c r="E12" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="F12" s="74"/>
+      <c r="F12" s="90"/>
       <c r="G12" s="39"/>
       <c r="H12" s="13">
         <v>0</v>
@@ -2576,21 +2576,21 @@
       <c r="L12" s="12">
         <v>1</v>
       </c>
-      <c r="M12" s="85" t="s">
+      <c r="M12" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="N12" s="86"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="73" t="s">
+      <c r="N12" s="88"/>
+      <c r="O12" s="95"/>
+      <c r="P12" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="74"/>
-      <c r="T12" s="74"/>
-      <c r="U12" s="74"/>
-      <c r="V12" s="74"/>
-      <c r="W12" s="74"/>
+      <c r="Q12" s="90"/>
+      <c r="R12" s="90"/>
+      <c r="S12" s="90"/>
+      <c r="T12" s="90"/>
+      <c r="U12" s="90"/>
+      <c r="V12" s="90"/>
+      <c r="W12" s="90"/>
       <c r="X12" s="39"/>
       <c r="Y12" s="36" t="b">
         <v>0</v>
@@ -2616,10 +2616,10 @@
       <c r="D13" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="73" t="s">
+      <c r="E13" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="F13" s="74"/>
+      <c r="F13" s="90"/>
       <c r="G13" s="39"/>
       <c r="H13" s="13">
         <v>0</v>
@@ -2636,21 +2636,21 @@
       <c r="L13" s="32">
         <v>0</v>
       </c>
-      <c r="M13" s="85" t="s">
+      <c r="M13" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="N13" s="86"/>
-      <c r="O13" s="87"/>
-      <c r="P13" s="73" t="s">
+      <c r="N13" s="88"/>
+      <c r="O13" s="95"/>
+      <c r="P13" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="74"/>
-      <c r="S13" s="74"/>
-      <c r="T13" s="74"/>
-      <c r="U13" s="74"/>
-      <c r="V13" s="74"/>
-      <c r="W13" s="74"/>
+      <c r="Q13" s="90"/>
+      <c r="R13" s="90"/>
+      <c r="S13" s="90"/>
+      <c r="T13" s="90"/>
+      <c r="U13" s="90"/>
+      <c r="V13" s="90"/>
+      <c r="W13" s="90"/>
       <c r="X13" s="39"/>
       <c r="Y13" s="35" t="b">
         <v>1</v>
@@ -2676,10 +2676,10 @@
       <c r="D14" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="73" t="s">
+      <c r="E14" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="74"/>
+      <c r="F14" s="90"/>
       <c r="G14" s="39"/>
       <c r="H14" s="13">
         <v>0</v>
@@ -2696,21 +2696,21 @@
       <c r="L14" s="12">
         <v>1</v>
       </c>
-      <c r="M14" s="85" t="s">
+      <c r="M14" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="N14" s="86"/>
-      <c r="O14" s="87"/>
-      <c r="P14" s="73" t="s">
+      <c r="N14" s="88"/>
+      <c r="O14" s="95"/>
+      <c r="P14" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="74"/>
-      <c r="S14" s="74"/>
-      <c r="T14" s="74"/>
-      <c r="U14" s="74"/>
-      <c r="V14" s="74"/>
-      <c r="W14" s="74"/>
+      <c r="Q14" s="90"/>
+      <c r="R14" s="90"/>
+      <c r="S14" s="90"/>
+      <c r="T14" s="90"/>
+      <c r="U14" s="90"/>
+      <c r="V14" s="90"/>
+      <c r="W14" s="90"/>
       <c r="X14" s="39"/>
       <c r="Y14" s="36" t="b">
         <v>1</v>
@@ -2731,9 +2731,9 @@
       </c>
       <c r="B15" s="45"/>
       <c r="C15" s="34"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
       <c r="G15" s="38"/>
       <c r="H15" s="3">
         <v>0</v>
@@ -2753,18 +2753,18 @@
       <c r="M15" s="1">
         <v>0</v>
       </c>
-      <c r="N15" s="80" t="s">
+      <c r="N15" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="82"/>
-      <c r="S15" s="82"/>
-      <c r="T15" s="82"/>
-      <c r="U15" s="82"/>
-      <c r="V15" s="82"/>
-      <c r="W15" s="82"/>
+      <c r="O15" s="78"/>
+      <c r="P15" s="78"/>
+      <c r="Q15" s="78"/>
+      <c r="R15" s="74"/>
+      <c r="S15" s="74"/>
+      <c r="T15" s="74"/>
+      <c r="U15" s="74"/>
+      <c r="V15" s="74"/>
+      <c r="W15" s="74"/>
       <c r="X15" s="38"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="1"/>
@@ -2782,10 +2782,10 @@
       <c r="D16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="83" t="s">
+      <c r="E16" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="84"/>
+      <c r="F16" s="83"/>
       <c r="G16" s="39"/>
       <c r="H16" s="13">
         <v>0</v>
@@ -2817,16 +2817,16 @@
       <c r="Q16" s="12">
         <v>0</v>
       </c>
-      <c r="R16" s="83" t="s">
+      <c r="R16" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S16" s="84"/>
-      <c r="T16" s="93"/>
-      <c r="U16" s="94" t="s">
+      <c r="S16" s="83"/>
+      <c r="T16" s="84"/>
+      <c r="U16" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="V16" s="95"/>
-      <c r="W16" s="95"/>
+      <c r="V16" s="86"/>
+      <c r="W16" s="86"/>
       <c r="X16" s="39"/>
       <c r="Y16" s="36" t="b">
         <v>1</v>
@@ -2852,10 +2852,10 @@
       <c r="D17" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="83" t="s">
+      <c r="E17" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="84"/>
+      <c r="F17" s="83"/>
       <c r="G17" s="39"/>
       <c r="H17" s="41">
         <v>0</v>
@@ -2887,16 +2887,16 @@
       <c r="Q17" s="32">
         <v>1</v>
       </c>
-      <c r="R17" s="83" t="s">
+      <c r="R17" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S17" s="84"/>
-      <c r="T17" s="93"/>
-      <c r="U17" s="94" t="s">
+      <c r="S17" s="83"/>
+      <c r="T17" s="84"/>
+      <c r="U17" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="V17" s="95"/>
-      <c r="W17" s="95"/>
+      <c r="V17" s="86"/>
+      <c r="W17" s="86"/>
       <c r="X17" s="39"/>
       <c r="Y17" s="35" t="b">
         <v>1</v>
@@ -2922,10 +2922,10 @@
       <c r="D18" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="83" t="s">
+      <c r="E18" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="84"/>
+      <c r="F18" s="83"/>
       <c r="G18" s="39"/>
       <c r="H18" s="13">
         <v>0</v>
@@ -2957,16 +2957,16 @@
       <c r="Q18" s="12">
         <v>0</v>
       </c>
-      <c r="R18" s="83" t="s">
+      <c r="R18" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S18" s="84"/>
-      <c r="T18" s="93"/>
-      <c r="U18" s="94" t="s">
+      <c r="S18" s="83"/>
+      <c r="T18" s="84"/>
+      <c r="U18" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="V18" s="95"/>
-      <c r="W18" s="95"/>
+      <c r="V18" s="86"/>
+      <c r="W18" s="86"/>
       <c r="X18" s="39"/>
       <c r="Y18" s="36" t="b">
         <v>1</v>
@@ -2992,10 +2992,10 @@
       <c r="D19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="83" t="s">
+      <c r="E19" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="84"/>
+      <c r="F19" s="83"/>
       <c r="G19" s="39"/>
       <c r="H19" s="41">
         <v>0</v>
@@ -3027,16 +3027,16 @@
       <c r="Q19" s="32">
         <v>1</v>
       </c>
-      <c r="R19" s="83" t="s">
+      <c r="R19" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S19" s="84"/>
-      <c r="T19" s="93"/>
-      <c r="U19" s="94" t="s">
+      <c r="S19" s="83"/>
+      <c r="T19" s="84"/>
+      <c r="U19" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="V19" s="95"/>
-      <c r="W19" s="95"/>
+      <c r="V19" s="86"/>
+      <c r="W19" s="86"/>
       <c r="X19" s="39"/>
       <c r="Y19" s="35" t="b">
         <v>1</v>
@@ -3062,10 +3062,10 @@
       <c r="D20" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="83" t="s">
+      <c r="E20" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="84"/>
+      <c r="F20" s="83"/>
       <c r="G20" s="39"/>
       <c r="H20" s="13">
         <v>0</v>
@@ -3097,16 +3097,16 @@
       <c r="Q20" s="12">
         <v>0</v>
       </c>
-      <c r="R20" s="83" t="s">
+      <c r="R20" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S20" s="84"/>
-      <c r="T20" s="93"/>
-      <c r="U20" s="94" t="s">
+      <c r="S20" s="83"/>
+      <c r="T20" s="84"/>
+      <c r="U20" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="V20" s="95"/>
-      <c r="W20" s="95"/>
+      <c r="V20" s="86"/>
+      <c r="W20" s="86"/>
       <c r="X20" s="39"/>
       <c r="Y20" s="36" t="b">
         <v>1</v>
@@ -3132,10 +3132,10 @@
       <c r="D21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="83" t="s">
+      <c r="E21" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="84"/>
+      <c r="F21" s="83"/>
       <c r="G21" s="39"/>
       <c r="H21" s="41">
         <v>0</v>
@@ -3167,16 +3167,16 @@
       <c r="Q21" s="32">
         <v>1</v>
       </c>
-      <c r="R21" s="83" t="s">
+      <c r="R21" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S21" s="84"/>
-      <c r="T21" s="93"/>
-      <c r="U21" s="94" t="s">
+      <c r="S21" s="83"/>
+      <c r="T21" s="84"/>
+      <c r="U21" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="V21" s="95"/>
-      <c r="W21" s="95"/>
+      <c r="V21" s="86"/>
+      <c r="W21" s="86"/>
       <c r="X21" s="39"/>
       <c r="Y21" s="35" t="b">
         <v>1</v>
@@ -3202,10 +3202,10 @@
       <c r="D22" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="83" t="s">
+      <c r="E22" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="84"/>
+      <c r="F22" s="83"/>
       <c r="G22" s="39"/>
       <c r="H22" s="13">
         <v>0</v>
@@ -3237,16 +3237,16 @@
       <c r="Q22" s="12">
         <v>0</v>
       </c>
-      <c r="R22" s="83" t="s">
+      <c r="R22" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S22" s="84"/>
-      <c r="T22" s="93"/>
-      <c r="U22" s="94" t="s">
+      <c r="S22" s="83"/>
+      <c r="T22" s="84"/>
+      <c r="U22" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="V22" s="95"/>
-      <c r="W22" s="95"/>
+      <c r="V22" s="86"/>
+      <c r="W22" s="86"/>
       <c r="X22" s="39"/>
       <c r="Y22" s="36" t="b">
         <v>1</v>
@@ -3272,10 +3272,10 @@
       <c r="D23" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="83" t="s">
+      <c r="E23" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="84"/>
+      <c r="F23" s="83"/>
       <c r="G23" s="39"/>
       <c r="H23" s="41">
         <v>0</v>
@@ -3307,16 +3307,16 @@
       <c r="Q23" s="32">
         <v>1</v>
       </c>
-      <c r="R23" s="83" t="s">
+      <c r="R23" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S23" s="84"/>
-      <c r="T23" s="93"/>
-      <c r="U23" s="94" t="s">
+      <c r="S23" s="83"/>
+      <c r="T23" s="84"/>
+      <c r="U23" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="V23" s="95"/>
-      <c r="W23" s="95"/>
+      <c r="V23" s="86"/>
+      <c r="W23" s="86"/>
       <c r="X23" s="39"/>
       <c r="Y23" s="35" t="b">
         <v>1</v>
@@ -3342,10 +3342,10 @@
       <c r="D24" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="83" t="s">
+      <c r="E24" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="84"/>
+      <c r="F24" s="83"/>
       <c r="G24" s="39"/>
       <c r="H24" s="13">
         <v>0</v>
@@ -3377,16 +3377,16 @@
       <c r="Q24" s="12">
         <v>0</v>
       </c>
-      <c r="R24" s="83" t="s">
+      <c r="R24" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S24" s="84"/>
-      <c r="T24" s="93"/>
-      <c r="U24" s="94" t="s">
+      <c r="S24" s="83"/>
+      <c r="T24" s="84"/>
+      <c r="U24" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="V24" s="95"/>
-      <c r="W24" s="95"/>
+      <c r="V24" s="86"/>
+      <c r="W24" s="86"/>
       <c r="X24" s="39"/>
       <c r="Y24" s="36" t="b">
         <v>1</v>
@@ -3449,16 +3449,16 @@
       <c r="Q25" s="32">
         <v>1</v>
       </c>
-      <c r="R25" s="83" t="s">
+      <c r="R25" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S25" s="84"/>
-      <c r="T25" s="93"/>
-      <c r="U25" s="94" t="s">
+      <c r="S25" s="83"/>
+      <c r="T25" s="84"/>
+      <c r="U25" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="V25" s="95"/>
-      <c r="W25" s="95"/>
+      <c r="V25" s="86"/>
+      <c r="W25" s="86"/>
       <c r="X25" s="39"/>
       <c r="Y25" s="35" t="b">
         <v>1</v>
@@ -3484,10 +3484,10 @@
       <c r="D26" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="83" t="s">
+      <c r="E26" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="84"/>
+      <c r="F26" s="83"/>
       <c r="G26" s="39"/>
       <c r="H26" s="13">
         <v>0</v>
@@ -3519,16 +3519,16 @@
       <c r="Q26" s="12">
         <v>0</v>
       </c>
-      <c r="R26" s="83" t="s">
+      <c r="R26" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S26" s="84"/>
-      <c r="T26" s="93"/>
-      <c r="U26" s="94" t="s">
+      <c r="S26" s="83"/>
+      <c r="T26" s="84"/>
+      <c r="U26" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="V26" s="95"/>
-      <c r="W26" s="95"/>
+      <c r="V26" s="86"/>
+      <c r="W26" s="86"/>
       <c r="X26" s="39"/>
       <c r="Y26" s="36" t="b">
         <v>1</v>
@@ -3554,10 +3554,10 @@
       <c r="D27" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="83" t="s">
+      <c r="E27" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="84"/>
+      <c r="F27" s="83"/>
       <c r="G27" s="39"/>
       <c r="H27" s="41">
         <v>0</v>
@@ -3589,16 +3589,16 @@
       <c r="Q27" s="32">
         <v>1</v>
       </c>
-      <c r="R27" s="83" t="s">
+      <c r="R27" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S27" s="84"/>
-      <c r="T27" s="93"/>
-      <c r="U27" s="94" t="s">
+      <c r="S27" s="83"/>
+      <c r="T27" s="84"/>
+      <c r="U27" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="V27" s="95"/>
-      <c r="W27" s="95"/>
+      <c r="V27" s="86"/>
+      <c r="W27" s="86"/>
       <c r="X27" s="39"/>
       <c r="Y27" s="35" t="b">
         <v>1</v>
@@ -3624,10 +3624,10 @@
       <c r="D28" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="83" t="s">
+      <c r="E28" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="84"/>
+      <c r="F28" s="83"/>
       <c r="G28" s="39"/>
       <c r="H28" s="13">
         <v>0</v>
@@ -3659,16 +3659,16 @@
       <c r="Q28" s="12">
         <v>0</v>
       </c>
-      <c r="R28" s="83" t="s">
+      <c r="R28" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S28" s="84"/>
-      <c r="T28" s="93"/>
-      <c r="U28" s="94" t="s">
+      <c r="S28" s="83"/>
+      <c r="T28" s="84"/>
+      <c r="U28" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="V28" s="95"/>
-      <c r="W28" s="95"/>
+      <c r="V28" s="86"/>
+      <c r="W28" s="86"/>
       <c r="X28" s="39"/>
       <c r="Y28" s="36" t="b">
         <v>1</v>
@@ -3731,16 +3731,16 @@
       <c r="Q29" s="32">
         <v>1</v>
       </c>
-      <c r="R29" s="83" t="s">
+      <c r="R29" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="S29" s="84"/>
-      <c r="T29" s="93"/>
-      <c r="U29" s="96" t="s">
+      <c r="S29" s="83"/>
+      <c r="T29" s="84"/>
+      <c r="U29" s="102" t="s">
         <v>127</v>
       </c>
-      <c r="V29" s="97"/>
-      <c r="W29" s="97"/>
+      <c r="V29" s="103"/>
+      <c r="W29" s="103"/>
       <c r="X29" s="39"/>
       <c r="Y29" s="35" t="b">
         <v>0</v>
@@ -3766,10 +3766,10 @@
       <c r="D30" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="83" t="s">
+      <c r="E30" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="84"/>
+      <c r="F30" s="83"/>
       <c r="G30" s="39"/>
       <c r="H30" s="13">
         <v>0</v>
@@ -3801,16 +3801,16 @@
       <c r="Q30" s="12">
         <v>0</v>
       </c>
-      <c r="R30" s="83" t="s">
+      <c r="R30" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S30" s="84"/>
-      <c r="T30" s="93"/>
-      <c r="U30" s="94" t="s">
+      <c r="S30" s="83"/>
+      <c r="T30" s="84"/>
+      <c r="U30" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="V30" s="95"/>
-      <c r="W30" s="95"/>
+      <c r="V30" s="86"/>
+      <c r="W30" s="86"/>
       <c r="X30" s="39"/>
       <c r="Y30" s="36" t="b">
         <v>1</v>
@@ -3836,10 +3836,10 @@
       <c r="D31" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="83" t="s">
+      <c r="E31" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="84"/>
+      <c r="F31" s="83"/>
       <c r="G31" s="39"/>
       <c r="H31" s="41">
         <v>0</v>
@@ -3871,16 +3871,16 @@
       <c r="Q31" s="32">
         <v>1</v>
       </c>
-      <c r="R31" s="83" t="s">
+      <c r="R31" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="S31" s="84"/>
-      <c r="T31" s="93"/>
-      <c r="U31" s="94" t="s">
+      <c r="S31" s="83"/>
+      <c r="T31" s="84"/>
+      <c r="U31" s="85" t="s">
         <v>100</v>
       </c>
-      <c r="V31" s="95"/>
-      <c r="W31" s="95"/>
+      <c r="V31" s="86"/>
+      <c r="W31" s="86"/>
       <c r="X31" s="39"/>
       <c r="Y31" s="35" t="b">
         <v>1</v>
@@ -3901,9 +3901,9 @@
       </c>
       <c r="B32" s="45"/>
       <c r="C32" s="34"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
       <c r="G32" s="38"/>
       <c r="H32" s="15">
         <v>1</v>
@@ -3917,20 +3917,20 @@
       <c r="K32" s="4">
         <v>1</v>
       </c>
-      <c r="L32" s="80" t="s">
+      <c r="L32" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="M32" s="81"/>
-      <c r="N32" s="81"/>
-      <c r="O32" s="82"/>
-      <c r="P32" s="82"/>
-      <c r="Q32" s="82"/>
-      <c r="R32" s="82"/>
-      <c r="S32" s="82"/>
-      <c r="T32" s="82"/>
-      <c r="U32" s="82"/>
-      <c r="V32" s="82"/>
-      <c r="W32" s="82"/>
+      <c r="M32" s="78"/>
+      <c r="N32" s="78"/>
+      <c r="O32" s="74"/>
+      <c r="P32" s="74"/>
+      <c r="Q32" s="74"/>
+      <c r="R32" s="74"/>
+      <c r="S32" s="74"/>
+      <c r="T32" s="74"/>
+      <c r="U32" s="74"/>
+      <c r="V32" s="74"/>
+      <c r="W32" s="74"/>
       <c r="X32" s="38"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="1"/>
@@ -3948,10 +3948,10 @@
       <c r="D33" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E33" s="73" t="s">
+      <c r="E33" s="89" t="s">
         <v>117</v>
       </c>
-      <c r="F33" s="74"/>
+      <c r="F33" s="90"/>
       <c r="G33" s="39"/>
       <c r="H33" s="16">
         <v>1</v>
@@ -3968,21 +3968,21 @@
       <c r="L33" s="26">
         <v>0</v>
       </c>
-      <c r="M33" s="98" t="s">
+      <c r="M33" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="N33" s="99"/>
-      <c r="O33" s="100"/>
-      <c r="P33" s="73" t="s">
+      <c r="N33" s="97"/>
+      <c r="O33" s="98"/>
+      <c r="P33" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="74"/>
-      <c r="S33" s="74"/>
-      <c r="T33" s="74"/>
-      <c r="U33" s="74"/>
-      <c r="V33" s="74"/>
-      <c r="W33" s="74"/>
+      <c r="Q33" s="90"/>
+      <c r="R33" s="90"/>
+      <c r="S33" s="90"/>
+      <c r="T33" s="90"/>
+      <c r="U33" s="90"/>
+      <c r="V33" s="90"/>
+      <c r="W33" s="90"/>
       <c r="X33" s="39"/>
       <c r="Y33" s="35" t="b">
         <v>0</v>
@@ -4008,10 +4008,10 @@
       <c r="D34" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E34" s="73" t="s">
+      <c r="E34" s="89" t="s">
         <v>117</v>
       </c>
-      <c r="F34" s="74"/>
+      <c r="F34" s="90"/>
       <c r="G34" s="39"/>
       <c r="H34" s="16">
         <v>1</v>
@@ -4028,21 +4028,21 @@
       <c r="L34" s="5">
         <v>1</v>
       </c>
-      <c r="M34" s="98" t="s">
+      <c r="M34" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="N34" s="99"/>
-      <c r="O34" s="100"/>
-      <c r="P34" s="73" t="s">
+      <c r="N34" s="97"/>
+      <c r="O34" s="98"/>
+      <c r="P34" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q34" s="74"/>
-      <c r="R34" s="74"/>
-      <c r="S34" s="74"/>
-      <c r="T34" s="74"/>
-      <c r="U34" s="74"/>
-      <c r="V34" s="74"/>
-      <c r="W34" s="74"/>
+      <c r="Q34" s="90"/>
+      <c r="R34" s="90"/>
+      <c r="S34" s="90"/>
+      <c r="T34" s="90"/>
+      <c r="U34" s="90"/>
+      <c r="V34" s="90"/>
+      <c r="W34" s="90"/>
       <c r="X34" s="39"/>
       <c r="Y34" s="36" t="b">
         <v>0</v>
@@ -4064,8 +4064,8 @@
       <c r="B35" s="45"/>
       <c r="C35" s="34"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="80"/>
-      <c r="F35" s="81"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="78"/>
       <c r="G35" s="38"/>
       <c r="H35" s="15">
         <v>1</v>
@@ -4079,20 +4079,20 @@
       <c r="K35" s="4">
         <v>1</v>
       </c>
-      <c r="L35" s="80" t="s">
+      <c r="L35" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="M35" s="81"/>
-      <c r="N35" s="81"/>
-      <c r="O35" s="81"/>
-      <c r="P35" s="81"/>
-      <c r="Q35" s="81"/>
-      <c r="R35" s="101"/>
-      <c r="S35" s="82"/>
-      <c r="T35" s="82"/>
-      <c r="U35" s="82"/>
-      <c r="V35" s="82"/>
-      <c r="W35" s="82"/>
+      <c r="M35" s="78"/>
+      <c r="N35" s="78"/>
+      <c r="O35" s="78"/>
+      <c r="P35" s="78"/>
+      <c r="Q35" s="78"/>
+      <c r="R35" s="76"/>
+      <c r="S35" s="74"/>
+      <c r="T35" s="74"/>
+      <c r="U35" s="74"/>
+      <c r="V35" s="74"/>
+      <c r="W35" s="74"/>
       <c r="X35" s="38"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="1"/>
@@ -4110,10 +4110,10 @@
       <c r="D36" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E36" s="88" t="s">
+      <c r="E36" s="104" t="s">
         <v>118</v>
       </c>
-      <c r="F36" s="89"/>
+      <c r="F36" s="105"/>
       <c r="G36" s="39"/>
       <c r="H36" s="16">
         <v>1</v>
@@ -4142,15 +4142,15 @@
       <c r="P36" s="5">
         <v>0</v>
       </c>
-      <c r="Q36" s="73" t="s">
+      <c r="Q36" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="R36" s="74"/>
-      <c r="S36" s="74"/>
-      <c r="T36" s="74"/>
-      <c r="U36" s="74"/>
-      <c r="V36" s="74"/>
-      <c r="W36" s="74"/>
+      <c r="R36" s="90"/>
+      <c r="S36" s="90"/>
+      <c r="T36" s="90"/>
+      <c r="U36" s="90"/>
+      <c r="V36" s="90"/>
+      <c r="W36" s="90"/>
       <c r="X36" s="39"/>
       <c r="Y36" s="36" t="b">
         <v>0</v>
@@ -4176,10 +4176,10 @@
       <c r="D37" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E37" s="88" t="s">
+      <c r="E37" s="104" t="s">
         <v>118</v>
       </c>
-      <c r="F37" s="89"/>
+      <c r="F37" s="105"/>
       <c r="G37" s="39"/>
       <c r="H37" s="16">
         <v>1</v>
@@ -4208,15 +4208,15 @@
       <c r="P37" s="26">
         <v>1</v>
       </c>
-      <c r="Q37" s="73" t="s">
+      <c r="Q37" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="R37" s="74"/>
-      <c r="S37" s="74"/>
-      <c r="T37" s="74"/>
-      <c r="U37" s="74"/>
-      <c r="V37" s="74"/>
-      <c r="W37" s="74"/>
+      <c r="R37" s="90"/>
+      <c r="S37" s="90"/>
+      <c r="T37" s="90"/>
+      <c r="U37" s="90"/>
+      <c r="V37" s="90"/>
+      <c r="W37" s="90"/>
       <c r="X37" s="39"/>
       <c r="Y37" s="35" t="b">
         <v>0</v>
@@ -4237,9 +4237,9 @@
       </c>
       <c r="B38" s="45"/>
       <c r="C38" s="34"/>
-      <c r="D38" s="80"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
       <c r="G38" s="38"/>
       <c r="H38" s="42">
         <v>1</v>
@@ -4253,12 +4253,12 @@
       <c r="K38" s="21">
         <v>1</v>
       </c>
-      <c r="L38" s="82" t="s">
+      <c r="L38" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="M38" s="82"/>
-      <c r="N38" s="82"/>
-      <c r="O38" s="82"/>
+      <c r="M38" s="74"/>
+      <c r="N38" s="74"/>
+      <c r="O38" s="74"/>
       <c r="P38" s="66"/>
       <c r="Q38" s="66"/>
       <c r="R38" s="66"/>
@@ -4284,10 +4284,10 @@
       <c r="D39" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E39" s="75" t="s">
+      <c r="E39" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F39" s="76"/>
+      <c r="F39" s="68"/>
       <c r="G39" s="39"/>
       <c r="H39" s="16">
         <v>1</v>
@@ -4301,29 +4301,29 @@
       <c r="K39" s="10">
         <v>1</v>
       </c>
-      <c r="L39" s="90" t="s">
+      <c r="L39" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M39" s="91"/>
-      <c r="N39" s="91"/>
-      <c r="O39" s="92"/>
-      <c r="P39" s="73" t="s">
+      <c r="M39" s="100"/>
+      <c r="N39" s="100"/>
+      <c r="O39" s="101"/>
+      <c r="P39" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q39" s="74"/>
-      <c r="R39" s="74"/>
-      <c r="S39" s="74"/>
-      <c r="T39" s="74"/>
-      <c r="U39" s="74"/>
-      <c r="V39" s="74"/>
-      <c r="W39" s="74"/>
+      <c r="Q39" s="90"/>
+      <c r="R39" s="90"/>
+      <c r="S39" s="90"/>
+      <c r="T39" s="90"/>
+      <c r="U39" s="90"/>
+      <c r="V39" s="90"/>
+      <c r="W39" s="90"/>
       <c r="X39" s="39"/>
-      <c r="Y39" s="67" t="s">
+      <c r="Y39" s="106" t="s">
         <v>129</v>
       </c>
-      <c r="Z39" s="68"/>
-      <c r="AA39" s="68"/>
-      <c r="AB39" s="69"/>
+      <c r="Z39" s="107"/>
+      <c r="AA39" s="107"/>
+      <c r="AB39" s="108"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" s="51" t="s">
@@ -4336,10 +4336,10 @@
       <c r="D40" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E40" s="75" t="s">
+      <c r="E40" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F40" s="76"/>
+      <c r="F40" s="68"/>
       <c r="G40" s="39"/>
       <c r="H40" s="16">
         <v>1</v>
@@ -4353,29 +4353,29 @@
       <c r="K40" s="10">
         <v>1</v>
       </c>
-      <c r="L40" s="90" t="s">
+      <c r="L40" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M40" s="91"/>
-      <c r="N40" s="91"/>
-      <c r="O40" s="92"/>
-      <c r="P40" s="73" t="s">
+      <c r="M40" s="100"/>
+      <c r="N40" s="100"/>
+      <c r="O40" s="101"/>
+      <c r="P40" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q40" s="74"/>
-      <c r="R40" s="74"/>
-      <c r="S40" s="74"/>
-      <c r="T40" s="74"/>
-      <c r="U40" s="74"/>
-      <c r="V40" s="74"/>
-      <c r="W40" s="74"/>
+      <c r="Q40" s="90"/>
+      <c r="R40" s="90"/>
+      <c r="S40" s="90"/>
+      <c r="T40" s="90"/>
+      <c r="U40" s="90"/>
+      <c r="V40" s="90"/>
+      <c r="W40" s="90"/>
       <c r="X40" s="39"/>
-      <c r="Y40" s="70" t="s">
+      <c r="Y40" s="109" t="s">
         <v>130</v>
       </c>
-      <c r="Z40" s="71"/>
-      <c r="AA40" s="71"/>
-      <c r="AB40" s="72"/>
+      <c r="Z40" s="110"/>
+      <c r="AA40" s="110"/>
+      <c r="AB40" s="111"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" s="53" t="s">
@@ -4388,10 +4388,10 @@
       <c r="D41" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E41" s="75" t="s">
+      <c r="E41" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F41" s="76"/>
+      <c r="F41" s="68"/>
       <c r="G41" s="39"/>
       <c r="H41" s="16">
         <v>1</v>
@@ -4405,29 +4405,29 @@
       <c r="K41" s="10">
         <v>1</v>
       </c>
-      <c r="L41" s="90" t="s">
+      <c r="L41" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M41" s="91"/>
-      <c r="N41" s="91"/>
-      <c r="O41" s="92"/>
-      <c r="P41" s="73" t="s">
+      <c r="M41" s="100"/>
+      <c r="N41" s="100"/>
+      <c r="O41" s="101"/>
+      <c r="P41" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q41" s="74"/>
-      <c r="R41" s="74"/>
-      <c r="S41" s="74"/>
-      <c r="T41" s="74"/>
-      <c r="U41" s="74"/>
-      <c r="V41" s="74"/>
-      <c r="W41" s="74"/>
+      <c r="Q41" s="90"/>
+      <c r="R41" s="90"/>
+      <c r="S41" s="90"/>
+      <c r="T41" s="90"/>
+      <c r="U41" s="90"/>
+      <c r="V41" s="90"/>
+      <c r="W41" s="90"/>
       <c r="X41" s="39"/>
-      <c r="Y41" s="67" t="s">
+      <c r="Y41" s="106" t="s">
         <v>131</v>
       </c>
-      <c r="Z41" s="68"/>
-      <c r="AA41" s="68"/>
-      <c r="AB41" s="69"/>
+      <c r="Z41" s="107"/>
+      <c r="AA41" s="107"/>
+      <c r="AB41" s="108"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="51" t="s">
@@ -4440,10 +4440,10 @@
       <c r="D42" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E42" s="75" t="s">
+      <c r="E42" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F42" s="76"/>
+      <c r="F42" s="68"/>
       <c r="G42" s="39"/>
       <c r="H42" s="16">
         <v>1</v>
@@ -4457,29 +4457,29 @@
       <c r="K42" s="10">
         <v>1</v>
       </c>
-      <c r="L42" s="90" t="s">
+      <c r="L42" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M42" s="91"/>
-      <c r="N42" s="91"/>
-      <c r="O42" s="92"/>
-      <c r="P42" s="73" t="s">
+      <c r="M42" s="100"/>
+      <c r="N42" s="100"/>
+      <c r="O42" s="101"/>
+      <c r="P42" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q42" s="74"/>
-      <c r="R42" s="74"/>
-      <c r="S42" s="74"/>
-      <c r="T42" s="74"/>
-      <c r="U42" s="74"/>
-      <c r="V42" s="74"/>
-      <c r="W42" s="74"/>
+      <c r="Q42" s="90"/>
+      <c r="R42" s="90"/>
+      <c r="S42" s="90"/>
+      <c r="T42" s="90"/>
+      <c r="U42" s="90"/>
+      <c r="V42" s="90"/>
+      <c r="W42" s="90"/>
       <c r="X42" s="39"/>
-      <c r="Y42" s="70" t="s">
+      <c r="Y42" s="109" t="s">
         <v>132</v>
       </c>
-      <c r="Z42" s="71"/>
-      <c r="AA42" s="71"/>
-      <c r="AB42" s="72"/>
+      <c r="Z42" s="110"/>
+      <c r="AA42" s="110"/>
+      <c r="AB42" s="111"/>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" s="53" t="s">
@@ -4492,10 +4492,10 @@
       <c r="D43" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E43" s="75" t="s">
+      <c r="E43" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F43" s="76"/>
+      <c r="F43" s="68"/>
       <c r="G43" s="39"/>
       <c r="H43" s="16">
         <v>1</v>
@@ -4509,29 +4509,29 @@
       <c r="K43" s="10">
         <v>1</v>
       </c>
-      <c r="L43" s="90" t="s">
+      <c r="L43" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M43" s="91"/>
-      <c r="N43" s="91"/>
-      <c r="O43" s="92"/>
-      <c r="P43" s="73" t="s">
+      <c r="M43" s="100"/>
+      <c r="N43" s="100"/>
+      <c r="O43" s="101"/>
+      <c r="P43" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q43" s="74"/>
-      <c r="R43" s="74"/>
-      <c r="S43" s="74"/>
-      <c r="T43" s="74"/>
-      <c r="U43" s="74"/>
-      <c r="V43" s="74"/>
-      <c r="W43" s="74"/>
+      <c r="Q43" s="90"/>
+      <c r="R43" s="90"/>
+      <c r="S43" s="90"/>
+      <c r="T43" s="90"/>
+      <c r="U43" s="90"/>
+      <c r="V43" s="90"/>
+      <c r="W43" s="90"/>
       <c r="X43" s="39"/>
-      <c r="Y43" s="67" t="s">
+      <c r="Y43" s="106" t="s">
         <v>133</v>
       </c>
-      <c r="Z43" s="68"/>
-      <c r="AA43" s="68"/>
-      <c r="AB43" s="69"/>
+      <c r="Z43" s="107"/>
+      <c r="AA43" s="107"/>
+      <c r="AB43" s="108"/>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" s="51" t="s">
@@ -4544,10 +4544,10 @@
       <c r="D44" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E44" s="75" t="s">
+      <c r="E44" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F44" s="76"/>
+      <c r="F44" s="68"/>
       <c r="G44" s="39"/>
       <c r="H44" s="16">
         <v>1</v>
@@ -4561,29 +4561,29 @@
       <c r="K44" s="10">
         <v>1</v>
       </c>
-      <c r="L44" s="90" t="s">
+      <c r="L44" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M44" s="91"/>
-      <c r="N44" s="91"/>
-      <c r="O44" s="92"/>
-      <c r="P44" s="73" t="s">
+      <c r="M44" s="100"/>
+      <c r="N44" s="100"/>
+      <c r="O44" s="101"/>
+      <c r="P44" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q44" s="74"/>
-      <c r="R44" s="74"/>
-      <c r="S44" s="74"/>
-      <c r="T44" s="74"/>
-      <c r="U44" s="74"/>
-      <c r="V44" s="74"/>
-      <c r="W44" s="74"/>
+      <c r="Q44" s="90"/>
+      <c r="R44" s="90"/>
+      <c r="S44" s="90"/>
+      <c r="T44" s="90"/>
+      <c r="U44" s="90"/>
+      <c r="V44" s="90"/>
+      <c r="W44" s="90"/>
       <c r="X44" s="39"/>
-      <c r="Y44" s="70" t="s">
+      <c r="Y44" s="109" t="s">
         <v>134</v>
       </c>
-      <c r="Z44" s="71"/>
-      <c r="AA44" s="71"/>
-      <c r="AB44" s="72"/>
+      <c r="Z44" s="110"/>
+      <c r="AA44" s="110"/>
+      <c r="AB44" s="111"/>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" s="53" t="s">
@@ -4596,10 +4596,10 @@
       <c r="D45" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E45" s="75" t="s">
+      <c r="E45" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F45" s="76"/>
+      <c r="F45" s="68"/>
       <c r="G45" s="39"/>
       <c r="H45" s="16">
         <v>1</v>
@@ -4613,29 +4613,29 @@
       <c r="K45" s="10">
         <v>1</v>
       </c>
-      <c r="L45" s="90" t="s">
+      <c r="L45" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M45" s="91"/>
-      <c r="N45" s="91"/>
-      <c r="O45" s="92"/>
-      <c r="P45" s="73" t="s">
+      <c r="M45" s="100"/>
+      <c r="N45" s="100"/>
+      <c r="O45" s="101"/>
+      <c r="P45" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q45" s="74"/>
-      <c r="R45" s="74"/>
-      <c r="S45" s="74"/>
-      <c r="T45" s="74"/>
-      <c r="U45" s="74"/>
-      <c r="V45" s="74"/>
-      <c r="W45" s="74"/>
+      <c r="Q45" s="90"/>
+      <c r="R45" s="90"/>
+      <c r="S45" s="90"/>
+      <c r="T45" s="90"/>
+      <c r="U45" s="90"/>
+      <c r="V45" s="90"/>
+      <c r="W45" s="90"/>
       <c r="X45" s="39"/>
-      <c r="Y45" s="67" t="s">
+      <c r="Y45" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="Z45" s="68"/>
-      <c r="AA45" s="68"/>
-      <c r="AB45" s="69"/>
+      <c r="Z45" s="107"/>
+      <c r="AA45" s="107"/>
+      <c r="AB45" s="108"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" s="51" t="s">
@@ -4648,10 +4648,10 @@
       <c r="D46" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E46" s="75" t="s">
+      <c r="E46" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F46" s="76"/>
+      <c r="F46" s="68"/>
       <c r="G46" s="39"/>
       <c r="H46" s="16">
         <v>1</v>
@@ -4665,29 +4665,29 @@
       <c r="K46" s="10">
         <v>1</v>
       </c>
-      <c r="L46" s="90" t="s">
+      <c r="L46" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M46" s="91"/>
-      <c r="N46" s="91"/>
-      <c r="O46" s="92"/>
-      <c r="P46" s="73" t="s">
+      <c r="M46" s="100"/>
+      <c r="N46" s="100"/>
+      <c r="O46" s="101"/>
+      <c r="P46" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q46" s="74"/>
-      <c r="R46" s="74"/>
-      <c r="S46" s="74"/>
-      <c r="T46" s="74"/>
-      <c r="U46" s="74"/>
-      <c r="V46" s="74"/>
-      <c r="W46" s="74"/>
+      <c r="Q46" s="90"/>
+      <c r="R46" s="90"/>
+      <c r="S46" s="90"/>
+      <c r="T46" s="90"/>
+      <c r="U46" s="90"/>
+      <c r="V46" s="90"/>
+      <c r="W46" s="90"/>
       <c r="X46" s="39"/>
-      <c r="Y46" s="70" t="s">
+      <c r="Y46" s="109" t="s">
         <v>136</v>
       </c>
-      <c r="Z46" s="71"/>
-      <c r="AA46" s="71"/>
-      <c r="AB46" s="72"/>
+      <c r="Z46" s="110"/>
+      <c r="AA46" s="110"/>
+      <c r="AB46" s="111"/>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" s="53" t="s">
@@ -4700,10 +4700,10 @@
       <c r="D47" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E47" s="75" t="s">
+      <c r="E47" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F47" s="76"/>
+      <c r="F47" s="68"/>
       <c r="G47" s="39"/>
       <c r="H47" s="16">
         <v>1</v>
@@ -4717,29 +4717,29 @@
       <c r="K47" s="10">
         <v>1</v>
       </c>
-      <c r="L47" s="90" t="s">
+      <c r="L47" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M47" s="91"/>
-      <c r="N47" s="91"/>
-      <c r="O47" s="92"/>
-      <c r="P47" s="73" t="s">
+      <c r="M47" s="100"/>
+      <c r="N47" s="100"/>
+      <c r="O47" s="101"/>
+      <c r="P47" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q47" s="74"/>
-      <c r="R47" s="74"/>
-      <c r="S47" s="74"/>
-      <c r="T47" s="74"/>
-      <c r="U47" s="74"/>
-      <c r="V47" s="74"/>
-      <c r="W47" s="74"/>
+      <c r="Q47" s="90"/>
+      <c r="R47" s="90"/>
+      <c r="S47" s="90"/>
+      <c r="T47" s="90"/>
+      <c r="U47" s="90"/>
+      <c r="V47" s="90"/>
+      <c r="W47" s="90"/>
       <c r="X47" s="39"/>
-      <c r="Y47" s="67" t="s">
+      <c r="Y47" s="106" t="s">
         <v>137</v>
       </c>
-      <c r="Z47" s="68"/>
-      <c r="AA47" s="68"/>
-      <c r="AB47" s="69"/>
+      <c r="Z47" s="107"/>
+      <c r="AA47" s="107"/>
+      <c r="AB47" s="108"/>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A48" s="51" t="s">
@@ -4752,10 +4752,10 @@
       <c r="D48" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E48" s="75" t="s">
+      <c r="E48" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F48" s="76"/>
+      <c r="F48" s="68"/>
       <c r="G48" s="39"/>
       <c r="H48" s="16">
         <v>1</v>
@@ -4769,29 +4769,29 @@
       <c r="K48" s="10">
         <v>1</v>
       </c>
-      <c r="L48" s="90" t="s">
+      <c r="L48" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M48" s="91"/>
-      <c r="N48" s="91"/>
-      <c r="O48" s="92"/>
-      <c r="P48" s="73" t="s">
+      <c r="M48" s="100"/>
+      <c r="N48" s="100"/>
+      <c r="O48" s="101"/>
+      <c r="P48" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q48" s="74"/>
-      <c r="R48" s="74"/>
-      <c r="S48" s="74"/>
-      <c r="T48" s="74"/>
-      <c r="U48" s="74"/>
-      <c r="V48" s="74"/>
-      <c r="W48" s="74"/>
+      <c r="Q48" s="90"/>
+      <c r="R48" s="90"/>
+      <c r="S48" s="90"/>
+      <c r="T48" s="90"/>
+      <c r="U48" s="90"/>
+      <c r="V48" s="90"/>
+      <c r="W48" s="90"/>
       <c r="X48" s="39"/>
-      <c r="Y48" s="70" t="s">
+      <c r="Y48" s="109" t="s">
         <v>138</v>
       </c>
-      <c r="Z48" s="71"/>
-      <c r="AA48" s="71"/>
-      <c r="AB48" s="72"/>
+      <c r="Z48" s="110"/>
+      <c r="AA48" s="110"/>
+      <c r="AB48" s="111"/>
     </row>
     <row r="49" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A49" s="53" t="s">
@@ -4804,10 +4804,10 @@
       <c r="D49" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E49" s="75" t="s">
+      <c r="E49" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F49" s="76"/>
+      <c r="F49" s="68"/>
       <c r="G49" s="39"/>
       <c r="H49" s="16">
         <v>1</v>
@@ -4821,29 +4821,29 @@
       <c r="K49" s="10">
         <v>1</v>
       </c>
-      <c r="L49" s="90" t="s">
+      <c r="L49" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M49" s="91"/>
-      <c r="N49" s="91"/>
-      <c r="O49" s="92"/>
-      <c r="P49" s="73" t="s">
+      <c r="M49" s="100"/>
+      <c r="N49" s="100"/>
+      <c r="O49" s="101"/>
+      <c r="P49" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q49" s="74"/>
-      <c r="R49" s="74"/>
-      <c r="S49" s="74"/>
-      <c r="T49" s="74"/>
-      <c r="U49" s="74"/>
-      <c r="V49" s="74"/>
-      <c r="W49" s="74"/>
+      <c r="Q49" s="90"/>
+      <c r="R49" s="90"/>
+      <c r="S49" s="90"/>
+      <c r="T49" s="90"/>
+      <c r="U49" s="90"/>
+      <c r="V49" s="90"/>
+      <c r="W49" s="90"/>
       <c r="X49" s="39"/>
-      <c r="Y49" s="67" t="s">
+      <c r="Y49" s="106" t="s">
         <v>139</v>
       </c>
-      <c r="Z49" s="68"/>
-      <c r="AA49" s="68"/>
-      <c r="AB49" s="69"/>
+      <c r="Z49" s="107"/>
+      <c r="AA49" s="107"/>
+      <c r="AB49" s="108"/>
       <c r="AP49" s="9" t="s">
         <v>128</v>
       </c>
@@ -4859,10 +4859,10 @@
       <c r="D50" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E50" s="75" t="s">
+      <c r="E50" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F50" s="76"/>
+      <c r="F50" s="68"/>
       <c r="G50" s="39"/>
       <c r="H50" s="16">
         <v>1</v>
@@ -4876,29 +4876,29 @@
       <c r="K50" s="10">
         <v>1</v>
       </c>
-      <c r="L50" s="90" t="s">
+      <c r="L50" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M50" s="91"/>
-      <c r="N50" s="91"/>
-      <c r="O50" s="92"/>
-      <c r="P50" s="73" t="s">
+      <c r="M50" s="100"/>
+      <c r="N50" s="100"/>
+      <c r="O50" s="101"/>
+      <c r="P50" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q50" s="74"/>
-      <c r="R50" s="74"/>
-      <c r="S50" s="74"/>
-      <c r="T50" s="74"/>
-      <c r="U50" s="74"/>
-      <c r="V50" s="74"/>
-      <c r="W50" s="74"/>
+      <c r="Q50" s="90"/>
+      <c r="R50" s="90"/>
+      <c r="S50" s="90"/>
+      <c r="T50" s="90"/>
+      <c r="U50" s="90"/>
+      <c r="V50" s="90"/>
+      <c r="W50" s="90"/>
       <c r="X50" s="39"/>
-      <c r="Y50" s="70" t="s">
+      <c r="Y50" s="109" t="s">
         <v>140</v>
       </c>
-      <c r="Z50" s="71"/>
-      <c r="AA50" s="71"/>
-      <c r="AB50" s="72"/>
+      <c r="Z50" s="110"/>
+      <c r="AA50" s="110"/>
+      <c r="AB50" s="111"/>
     </row>
     <row r="51" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A51" s="53" t="s">
@@ -4911,10 +4911,10 @@
       <c r="D51" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E51" s="75" t="s">
+      <c r="E51" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F51" s="76"/>
+      <c r="F51" s="68"/>
       <c r="G51" s="39"/>
       <c r="H51" s="16">
         <v>1</v>
@@ -4928,29 +4928,29 @@
       <c r="K51" s="10">
         <v>1</v>
       </c>
-      <c r="L51" s="90" t="s">
+      <c r="L51" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M51" s="91"/>
-      <c r="N51" s="91"/>
-      <c r="O51" s="92"/>
-      <c r="P51" s="73" t="s">
+      <c r="M51" s="100"/>
+      <c r="N51" s="100"/>
+      <c r="O51" s="101"/>
+      <c r="P51" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q51" s="74"/>
-      <c r="R51" s="74"/>
-      <c r="S51" s="74"/>
-      <c r="T51" s="74"/>
-      <c r="U51" s="74"/>
-      <c r="V51" s="74"/>
-      <c r="W51" s="74"/>
+      <c r="Q51" s="90"/>
+      <c r="R51" s="90"/>
+      <c r="S51" s="90"/>
+      <c r="T51" s="90"/>
+      <c r="U51" s="90"/>
+      <c r="V51" s="90"/>
+      <c r="W51" s="90"/>
       <c r="X51" s="39"/>
-      <c r="Y51" s="67" t="s">
+      <c r="Y51" s="106" t="s">
         <v>141</v>
       </c>
-      <c r="Z51" s="68"/>
-      <c r="AA51" s="68"/>
-      <c r="AB51" s="69"/>
+      <c r="Z51" s="107"/>
+      <c r="AA51" s="107"/>
+      <c r="AB51" s="108"/>
     </row>
     <row r="52" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A52" s="51" t="s">
@@ -4963,10 +4963,10 @@
       <c r="D52" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E52" s="75" t="s">
+      <c r="E52" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F52" s="76"/>
+      <c r="F52" s="68"/>
       <c r="G52" s="39"/>
       <c r="H52" s="16">
         <v>1</v>
@@ -4980,29 +4980,29 @@
       <c r="K52" s="10">
         <v>1</v>
       </c>
-      <c r="L52" s="90" t="s">
+      <c r="L52" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M52" s="91"/>
-      <c r="N52" s="91"/>
-      <c r="O52" s="92"/>
-      <c r="P52" s="73" t="s">
+      <c r="M52" s="100"/>
+      <c r="N52" s="100"/>
+      <c r="O52" s="101"/>
+      <c r="P52" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q52" s="74"/>
-      <c r="R52" s="74"/>
-      <c r="S52" s="74"/>
-      <c r="T52" s="74"/>
-      <c r="U52" s="74"/>
-      <c r="V52" s="74"/>
-      <c r="W52" s="74"/>
+      <c r="Q52" s="90"/>
+      <c r="R52" s="90"/>
+      <c r="S52" s="90"/>
+      <c r="T52" s="90"/>
+      <c r="U52" s="90"/>
+      <c r="V52" s="90"/>
+      <c r="W52" s="90"/>
       <c r="X52" s="39"/>
-      <c r="Y52" s="70" t="s">
+      <c r="Y52" s="109" t="s">
         <v>142</v>
       </c>
-      <c r="Z52" s="71"/>
-      <c r="AA52" s="71"/>
-      <c r="AB52" s="72"/>
+      <c r="Z52" s="110"/>
+      <c r="AA52" s="110"/>
+      <c r="AB52" s="111"/>
     </row>
     <row r="53" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A53" s="53" t="s">
@@ -5015,10 +5015,10 @@
       <c r="D53" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E53" s="75" t="s">
+      <c r="E53" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F53" s="76"/>
+      <c r="F53" s="68"/>
       <c r="G53" s="39"/>
       <c r="H53" s="16">
         <v>1</v>
@@ -5032,22 +5032,22 @@
       <c r="K53" s="10">
         <v>1</v>
       </c>
-      <c r="L53" s="90" t="s">
+      <c r="L53" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="M53" s="91"/>
-      <c r="N53" s="91"/>
-      <c r="O53" s="92"/>
-      <c r="P53" s="73" t="s">
+      <c r="M53" s="100"/>
+      <c r="N53" s="100"/>
+      <c r="O53" s="101"/>
+      <c r="P53" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="Q53" s="74"/>
-      <c r="R53" s="74"/>
-      <c r="S53" s="74"/>
-      <c r="T53" s="74"/>
-      <c r="U53" s="74"/>
-      <c r="V53" s="74"/>
-      <c r="W53" s="74"/>
+      <c r="Q53" s="90"/>
+      <c r="R53" s="90"/>
+      <c r="S53" s="90"/>
+      <c r="T53" s="90"/>
+      <c r="U53" s="90"/>
+      <c r="V53" s="90"/>
+      <c r="W53" s="90"/>
       <c r="X53" s="39"/>
       <c r="Y53" s="37" t="b">
         <v>0</v>
@@ -5073,10 +5073,10 @@
       <c r="D54" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="E54" s="111" t="s">
+      <c r="E54" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="F54" s="112"/>
+      <c r="F54" s="70"/>
       <c r="G54" s="58"/>
       <c r="H54" s="60">
         <v>1</v>
@@ -5093,19 +5093,19 @@
       <c r="L54" s="23">
         <v>0</v>
       </c>
-      <c r="M54" s="78" t="s">
+      <c r="M54" s="113" t="s">
         <v>125</v>
       </c>
-      <c r="N54" s="79"/>
-      <c r="O54" s="79"/>
-      <c r="P54" s="79"/>
-      <c r="Q54" s="79"/>
-      <c r="R54" s="79"/>
-      <c r="S54" s="79"/>
-      <c r="T54" s="79"/>
-      <c r="U54" s="79"/>
-      <c r="V54" s="79"/>
-      <c r="W54" s="79"/>
+      <c r="N54" s="114"/>
+      <c r="O54" s="114"/>
+      <c r="P54" s="114"/>
+      <c r="Q54" s="114"/>
+      <c r="R54" s="114"/>
+      <c r="S54" s="114"/>
+      <c r="T54" s="114"/>
+      <c r="U54" s="114"/>
+      <c r="V54" s="114"/>
+      <c r="W54" s="114"/>
       <c r="X54" s="58"/>
       <c r="Y54" s="61" t="b">
         <v>0</v>
@@ -5122,6 +5122,152 @@
     </row>
   </sheetData>
   <mergeCells count="170">
+    <mergeCell ref="Y39:AB39"/>
+    <mergeCell ref="Y40:AB40"/>
+    <mergeCell ref="Y41:AB41"/>
+    <mergeCell ref="Y42:AB42"/>
+    <mergeCell ref="Y43:AB43"/>
+    <mergeCell ref="Y44:AB44"/>
+    <mergeCell ref="Y45:AB45"/>
+    <mergeCell ref="Y46:AB46"/>
+    <mergeCell ref="P39:W39"/>
+    <mergeCell ref="P40:W40"/>
+    <mergeCell ref="P41:W41"/>
+    <mergeCell ref="P42:W42"/>
+    <mergeCell ref="P43:W43"/>
+    <mergeCell ref="Y47:AB47"/>
+    <mergeCell ref="Y48:AB48"/>
+    <mergeCell ref="Y49:AB49"/>
+    <mergeCell ref="Y50:AB50"/>
+    <mergeCell ref="Y51:AB51"/>
+    <mergeCell ref="Y52:AB52"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="H1:W1"/>
+    <mergeCell ref="M54:W54"/>
+    <mergeCell ref="P33:W33"/>
+    <mergeCell ref="P34:W34"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="O6:W6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="R15:W15"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="O32:W32"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="P13:W13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="P14:W14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="L49:O49"/>
+    <mergeCell ref="L50:O50"/>
+    <mergeCell ref="L51:O51"/>
+    <mergeCell ref="L52:O52"/>
+    <mergeCell ref="P49:W49"/>
+    <mergeCell ref="P50:W50"/>
+    <mergeCell ref="P51:W51"/>
+    <mergeCell ref="P52:W52"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="P53:W53"/>
+    <mergeCell ref="L47:O47"/>
+    <mergeCell ref="L48:O48"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:O40"/>
+    <mergeCell ref="L41:O41"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="L43:O43"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="U28:W28"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="U29:W29"/>
+    <mergeCell ref="R30:T30"/>
+    <mergeCell ref="P44:W44"/>
+    <mergeCell ref="P45:W45"/>
+    <mergeCell ref="P46:W46"/>
+    <mergeCell ref="P47:W47"/>
+    <mergeCell ref="P48:W48"/>
+    <mergeCell ref="L38:O38"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="L45:O45"/>
+    <mergeCell ref="L46:O46"/>
+    <mergeCell ref="P12:W12"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="Q36:W36"/>
+    <mergeCell ref="Q37:W37"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="U30:W30"/>
+    <mergeCell ref="U27:W27"/>
+    <mergeCell ref="L35:R35"/>
+    <mergeCell ref="S35:W35"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="U25:W25"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="U26:W26"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="U20:W20"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="U21:W21"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:W11"/>
+    <mergeCell ref="M12:O12"/>
     <mergeCell ref="E51:F51"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="E53:F53"/>
@@ -5146,152 +5292,6 @@
     <mergeCell ref="M4:Q4"/>
     <mergeCell ref="M5:Q5"/>
     <mergeCell ref="R3:T3"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="U20:W20"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="U21:W21"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="U4:W4"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:W11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="P12:W12"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="Q36:W36"/>
-    <mergeCell ref="Q37:W37"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="U30:W30"/>
-    <mergeCell ref="U27:W27"/>
-    <mergeCell ref="L35:R35"/>
-    <mergeCell ref="S35:W35"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="U25:W25"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="U26:W26"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="L47:O47"/>
-    <mergeCell ref="L48:O48"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:O40"/>
-    <mergeCell ref="L41:O41"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="L43:O43"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="U28:W28"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="U29:W29"/>
-    <mergeCell ref="R30:T30"/>
-    <mergeCell ref="P44:W44"/>
-    <mergeCell ref="P45:W45"/>
-    <mergeCell ref="P46:W46"/>
-    <mergeCell ref="P47:W47"/>
-    <mergeCell ref="P48:W48"/>
-    <mergeCell ref="L38:O38"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="L45:O45"/>
-    <mergeCell ref="L46:O46"/>
-    <mergeCell ref="L49:O49"/>
-    <mergeCell ref="L50:O50"/>
-    <mergeCell ref="L51:O51"/>
-    <mergeCell ref="L52:O52"/>
-    <mergeCell ref="P49:W49"/>
-    <mergeCell ref="P50:W50"/>
-    <mergeCell ref="P51:W51"/>
-    <mergeCell ref="P52:W52"/>
-    <mergeCell ref="L53:O53"/>
-    <mergeCell ref="P53:W53"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P13:W13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="P14:W14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="Y47:AB47"/>
-    <mergeCell ref="Y48:AB48"/>
-    <mergeCell ref="Y49:AB49"/>
-    <mergeCell ref="Y50:AB50"/>
-    <mergeCell ref="Y51:AB51"/>
-    <mergeCell ref="Y52:AB52"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="H1:W1"/>
-    <mergeCell ref="M54:W54"/>
-    <mergeCell ref="P33:W33"/>
-    <mergeCell ref="P34:W34"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="O6:W6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="R15:W15"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="O32:W32"/>
-    <mergeCell ref="Y39:AB39"/>
-    <mergeCell ref="Y40:AB40"/>
-    <mergeCell ref="Y41:AB41"/>
-    <mergeCell ref="Y42:AB42"/>
-    <mergeCell ref="Y43:AB43"/>
-    <mergeCell ref="Y44:AB44"/>
-    <mergeCell ref="Y45:AB45"/>
-    <mergeCell ref="Y46:AB46"/>
-    <mergeCell ref="P39:W39"/>
-    <mergeCell ref="P40:W40"/>
-    <mergeCell ref="P41:W41"/>
-    <mergeCell ref="P42:W42"/>
-    <mergeCell ref="P43:W43"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5468,20 +5468,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b05417e1-eb89-4392-aea8-ecdaf8fc0423" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b05417e1-eb89-4392-aea8-ecdaf8fc0423" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5503,14 +5503,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEFCFB9-977F-4BC6-8CD6-7A1E4BA64254}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE327FA-98F8-4626-AE66-90F799A55F58}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5524,4 +5516,12 @@
     <ds:schemaRef ds:uri="b05417e1-eb89-4392-aea8-ecdaf8fc0423"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEFCFB9-977F-4BC6-8CD6-7A1E4BA64254}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: Rassemblement de l'assembleur pour générer un fichier .bin au format logisim avec la traduction comme attendu
</commit_message>
<xml_diff>
--- a/Encodage_PARM.xlsx
+++ b/Encodage_PARM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monsi\Desktop\Ecole\Polytech_Nice\Architecture\Projet-P-ARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AE8A59-CFD7-4022-B5A2-838A677C4960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A263F9FE-7037-439A-92B8-6476DCDC427E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1352,123 +1352,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
       <extLst>
@@ -1517,6 +1400,18 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1525,6 +1420,111 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1852,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="92" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1872,54 +1872,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="47"/>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="94"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="106"/>
       <c r="G1" s="48"/>
-      <c r="H1" s="112" t="s">
+      <c r="H1" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
-      <c r="W1" s="112"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
       <c r="X1" s="49"/>
-      <c r="Y1" s="71" t="s">
+      <c r="Y1" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="73"/>
+      <c r="Z1" s="105"/>
+      <c r="AA1" s="105"/>
+      <c r="AB1" s="113"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" s="93"/>
+      <c r="A2" s="103"/>
       <c r="B2" s="45"/>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="75"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="80"/>
       <c r="G2" s="38"/>
       <c r="H2" s="3">
         <v>15</v>
@@ -2016,23 +2016,23 @@
       <c r="L3" s="32">
         <v>0</v>
       </c>
-      <c r="M3" s="89" t="s">
+      <c r="M3" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="79" t="s">
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="110"/>
+      <c r="R3" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="S3" s="80"/>
-      <c r="T3" s="81"/>
-      <c r="U3" s="87" t="s">
+      <c r="S3" s="108"/>
+      <c r="T3" s="109"/>
+      <c r="U3" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="V3" s="88"/>
-      <c r="W3" s="88"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="86"/>
       <c r="X3" s="39"/>
       <c r="Y3" s="35" t="b">
         <v>1</v>
@@ -2080,23 +2080,23 @@
       <c r="L4" s="12">
         <v>1</v>
       </c>
-      <c r="M4" s="89" t="s">
+      <c r="M4" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="79" t="s">
+      <c r="N4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="110"/>
+      <c r="R4" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="S4" s="80"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="87" t="s">
+      <c r="S4" s="108"/>
+      <c r="T4" s="109"/>
+      <c r="U4" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="V4" s="88"/>
-      <c r="W4" s="88"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="86"/>
       <c r="X4" s="39"/>
       <c r="Y4" s="36" t="b">
         <v>1</v>
@@ -2144,23 +2144,23 @@
       <c r="L5" s="32">
         <v>0</v>
       </c>
-      <c r="M5" s="89" t="s">
+      <c r="M5" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="N5" s="90"/>
-      <c r="O5" s="90"/>
-      <c r="P5" s="90"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="79" t="s">
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="110"/>
+      <c r="R5" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="S5" s="80"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="87" t="s">
+      <c r="S5" s="108"/>
+      <c r="T5" s="109"/>
+      <c r="U5" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="V5" s="88"/>
-      <c r="W5" s="88"/>
+      <c r="V5" s="86"/>
+      <c r="W5" s="86"/>
       <c r="X5" s="39"/>
       <c r="Y5" s="35" t="b">
         <v>1</v>
@@ -2181,9 +2181,9 @@
       </c>
       <c r="B6" s="45"/>
       <c r="C6" s="34"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="75"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="80"/>
       <c r="G6" s="38"/>
       <c r="H6" s="3">
         <v>0</v>
@@ -2191,27 +2191,27 @@
       <c r="I6" s="1">
         <v>0</v>
       </c>
-      <c r="J6" s="75" t="s">
+      <c r="J6" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="78"/>
-      <c r="R6" s="78"/>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78"/>
-      <c r="U6" s="78"/>
-      <c r="V6" s="78"/>
-      <c r="W6" s="78"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="101"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="81"/>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="81"/>
+      <c r="U6" s="81"/>
+      <c r="V6" s="81"/>
+      <c r="W6" s="81"/>
       <c r="X6" s="38"/>
-      <c r="Y6" s="76"/>
-      <c r="Z6" s="74"/>
-      <c r="AA6" s="74"/>
-      <c r="AB6" s="77"/>
+      <c r="Y6" s="101"/>
+      <c r="Z6" s="82"/>
+      <c r="AA6" s="82"/>
+      <c r="AB6" s="114"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
@@ -2252,21 +2252,21 @@
       <c r="N7" s="32">
         <v>0</v>
       </c>
-      <c r="O7" s="82" t="s">
+      <c r="O7" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="P7" s="83"/>
-      <c r="Q7" s="84"/>
-      <c r="R7" s="79" t="s">
+      <c r="P7" s="84"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="S7" s="80"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="87" t="s">
+      <c r="S7" s="108"/>
+      <c r="T7" s="109"/>
+      <c r="U7" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="V7" s="88"/>
-      <c r="W7" s="88"/>
+      <c r="V7" s="86"/>
+      <c r="W7" s="86"/>
       <c r="X7" s="39"/>
       <c r="Y7" s="35" t="b">
         <v>1</v>
@@ -2320,21 +2320,21 @@
       <c r="N8" s="12">
         <v>1</v>
       </c>
-      <c r="O8" s="82" t="s">
+      <c r="O8" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="P8" s="83"/>
-      <c r="Q8" s="84"/>
-      <c r="R8" s="79" t="s">
+      <c r="P8" s="84"/>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="S8" s="80"/>
-      <c r="T8" s="81"/>
-      <c r="U8" s="87" t="s">
+      <c r="S8" s="108"/>
+      <c r="T8" s="109"/>
+      <c r="U8" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="V8" s="88"/>
-      <c r="W8" s="88"/>
+      <c r="V8" s="86"/>
+      <c r="W8" s="86"/>
       <c r="X8" s="39"/>
       <c r="Y8" s="36" t="b">
         <v>1</v>
@@ -2388,21 +2388,21 @@
       <c r="N9" s="32">
         <v>0</v>
       </c>
-      <c r="O9" s="89" t="s">
+      <c r="O9" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="P9" s="90"/>
-      <c r="Q9" s="91"/>
-      <c r="R9" s="79" t="s">
+      <c r="P9" s="74"/>
+      <c r="Q9" s="110"/>
+      <c r="R9" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="S9" s="80"/>
-      <c r="T9" s="81"/>
-      <c r="U9" s="87" t="s">
+      <c r="S9" s="108"/>
+      <c r="T9" s="109"/>
+      <c r="U9" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="V9" s="88"/>
-      <c r="W9" s="88"/>
+      <c r="V9" s="86"/>
+      <c r="W9" s="86"/>
       <c r="X9" s="39"/>
       <c r="Y9" s="35" t="b">
         <v>1</v>
@@ -2456,21 +2456,21 @@
       <c r="N10" s="12">
         <v>1</v>
       </c>
-      <c r="O10" s="89" t="s">
+      <c r="O10" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="P10" s="90"/>
-      <c r="Q10" s="91"/>
-      <c r="R10" s="79" t="s">
+      <c r="P10" s="74"/>
+      <c r="Q10" s="110"/>
+      <c r="R10" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="S10" s="80"/>
-      <c r="T10" s="81"/>
-      <c r="U10" s="87" t="s">
+      <c r="S10" s="108"/>
+      <c r="T10" s="109"/>
+      <c r="U10" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="V10" s="88"/>
-      <c r="W10" s="88"/>
+      <c r="V10" s="86"/>
+      <c r="W10" s="86"/>
       <c r="X10" s="39"/>
       <c r="Y10" s="36" t="b">
         <v>1</v>
@@ -2496,10 +2496,10 @@
       <c r="D11" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="89" t="s">
+      <c r="E11" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="F11" s="90"/>
+      <c r="F11" s="74"/>
       <c r="G11" s="39"/>
       <c r="H11" s="13">
         <v>0</v>
@@ -2516,21 +2516,21 @@
       <c r="L11" s="32">
         <v>0</v>
       </c>
-      <c r="M11" s="87" t="s">
+      <c r="M11" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="N11" s="88"/>
-      <c r="O11" s="95"/>
-      <c r="P11" s="89" t="s">
+      <c r="N11" s="86"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="90"/>
-      <c r="S11" s="90"/>
-      <c r="T11" s="90"/>
-      <c r="U11" s="90"/>
-      <c r="V11" s="90"/>
-      <c r="W11" s="90"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="74"/>
+      <c r="S11" s="74"/>
+      <c r="T11" s="74"/>
+      <c r="U11" s="74"/>
+      <c r="V11" s="74"/>
+      <c r="W11" s="74"/>
       <c r="X11" s="39"/>
       <c r="Y11" s="35" t="b">
         <v>0</v>
@@ -2556,10 +2556,10 @@
       <c r="D12" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="89" t="s">
+      <c r="E12" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="F12" s="90"/>
+      <c r="F12" s="74"/>
       <c r="G12" s="39"/>
       <c r="H12" s="13">
         <v>0</v>
@@ -2576,21 +2576,21 @@
       <c r="L12" s="12">
         <v>1</v>
       </c>
-      <c r="M12" s="87" t="s">
+      <c r="M12" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="N12" s="88"/>
-      <c r="O12" s="95"/>
-      <c r="P12" s="89" t="s">
+      <c r="N12" s="86"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
-      <c r="T12" s="90"/>
-      <c r="U12" s="90"/>
-      <c r="V12" s="90"/>
-      <c r="W12" s="90"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
+      <c r="S12" s="74"/>
+      <c r="T12" s="74"/>
+      <c r="U12" s="74"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="74"/>
       <c r="X12" s="39"/>
       <c r="Y12" s="36" t="b">
         <v>0</v>
@@ -2616,10 +2616,10 @@
       <c r="D13" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="89" t="s">
+      <c r="E13" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="F13" s="90"/>
+      <c r="F13" s="74"/>
       <c r="G13" s="39"/>
       <c r="H13" s="13">
         <v>0</v>
@@ -2636,21 +2636,21 @@
       <c r="L13" s="32">
         <v>0</v>
       </c>
-      <c r="M13" s="87" t="s">
+      <c r="M13" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="N13" s="88"/>
-      <c r="O13" s="95"/>
-      <c r="P13" s="89" t="s">
+      <c r="N13" s="86"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="Q13" s="90"/>
-      <c r="R13" s="90"/>
-      <c r="S13" s="90"/>
-      <c r="T13" s="90"/>
-      <c r="U13" s="90"/>
-      <c r="V13" s="90"/>
-      <c r="W13" s="90"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="74"/>
+      <c r="T13" s="74"/>
+      <c r="U13" s="74"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="74"/>
       <c r="X13" s="39"/>
       <c r="Y13" s="35" t="b">
         <v>1</v>
@@ -2676,10 +2676,10 @@
       <c r="D14" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="89" t="s">
+      <c r="E14" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="90"/>
+      <c r="F14" s="74"/>
       <c r="G14" s="39"/>
       <c r="H14" s="13">
         <v>0</v>
@@ -2696,21 +2696,21 @@
       <c r="L14" s="12">
         <v>1</v>
       </c>
-      <c r="M14" s="87" t="s">
+      <c r="M14" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="N14" s="88"/>
-      <c r="O14" s="95"/>
-      <c r="P14" s="89" t="s">
+      <c r="N14" s="86"/>
+      <c r="O14" s="87"/>
+      <c r="P14" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="90"/>
-      <c r="S14" s="90"/>
-      <c r="T14" s="90"/>
-      <c r="U14" s="90"/>
-      <c r="V14" s="90"/>
-      <c r="W14" s="90"/>
+      <c r="Q14" s="74"/>
+      <c r="R14" s="74"/>
+      <c r="S14" s="74"/>
+      <c r="T14" s="74"/>
+      <c r="U14" s="74"/>
+      <c r="V14" s="74"/>
+      <c r="W14" s="74"/>
       <c r="X14" s="39"/>
       <c r="Y14" s="36" t="b">
         <v>1</v>
@@ -2731,9 +2731,9 @@
       </c>
       <c r="B15" s="45"/>
       <c r="C15" s="34"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
       <c r="G15" s="38"/>
       <c r="H15" s="3">
         <v>0</v>
@@ -2753,18 +2753,18 @@
       <c r="M15" s="1">
         <v>0</v>
       </c>
-      <c r="N15" s="75" t="s">
+      <c r="N15" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="O15" s="78"/>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="74"/>
-      <c r="S15" s="74"/>
-      <c r="T15" s="74"/>
-      <c r="U15" s="74"/>
-      <c r="V15" s="74"/>
-      <c r="W15" s="74"/>
+      <c r="O15" s="81"/>
+      <c r="P15" s="81"/>
+      <c r="Q15" s="81"/>
+      <c r="R15" s="82"/>
+      <c r="S15" s="82"/>
+      <c r="T15" s="82"/>
+      <c r="U15" s="82"/>
+      <c r="V15" s="82"/>
+      <c r="W15" s="82"/>
       <c r="X15" s="38"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="1"/>
@@ -2782,10 +2782,10 @@
       <c r="D16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="82" t="s">
+      <c r="E16" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="83"/>
+      <c r="F16" s="84"/>
       <c r="G16" s="39"/>
       <c r="H16" s="13">
         <v>0</v>
@@ -2817,16 +2817,16 @@
       <c r="Q16" s="12">
         <v>0</v>
       </c>
-      <c r="R16" s="82" t="s">
+      <c r="R16" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S16" s="83"/>
-      <c r="T16" s="84"/>
-      <c r="U16" s="85" t="s">
+      <c r="S16" s="84"/>
+      <c r="T16" s="93"/>
+      <c r="U16" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="V16" s="86"/>
-      <c r="W16" s="86"/>
+      <c r="V16" s="95"/>
+      <c r="W16" s="95"/>
       <c r="X16" s="39"/>
       <c r="Y16" s="36" t="b">
         <v>1</v>
@@ -2852,10 +2852,10 @@
       <c r="D17" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="82" t="s">
+      <c r="E17" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="83"/>
+      <c r="F17" s="84"/>
       <c r="G17" s="39"/>
       <c r="H17" s="41">
         <v>0</v>
@@ -2887,16 +2887,16 @@
       <c r="Q17" s="32">
         <v>1</v>
       </c>
-      <c r="R17" s="82" t="s">
+      <c r="R17" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S17" s="83"/>
-      <c r="T17" s="84"/>
-      <c r="U17" s="85" t="s">
+      <c r="S17" s="84"/>
+      <c r="T17" s="93"/>
+      <c r="U17" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="V17" s="86"/>
-      <c r="W17" s="86"/>
+      <c r="V17" s="95"/>
+      <c r="W17" s="95"/>
       <c r="X17" s="39"/>
       <c r="Y17" s="35" t="b">
         <v>1</v>
@@ -2922,10 +2922,10 @@
       <c r="D18" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="82" t="s">
+      <c r="E18" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="83"/>
+      <c r="F18" s="84"/>
       <c r="G18" s="39"/>
       <c r="H18" s="13">
         <v>0</v>
@@ -2957,16 +2957,16 @@
       <c r="Q18" s="12">
         <v>0</v>
       </c>
-      <c r="R18" s="82" t="s">
+      <c r="R18" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S18" s="83"/>
-      <c r="T18" s="84"/>
-      <c r="U18" s="85" t="s">
+      <c r="S18" s="84"/>
+      <c r="T18" s="93"/>
+      <c r="U18" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="V18" s="86"/>
-      <c r="W18" s="86"/>
+      <c r="V18" s="95"/>
+      <c r="W18" s="95"/>
       <c r="X18" s="39"/>
       <c r="Y18" s="36" t="b">
         <v>1</v>
@@ -2992,10 +2992,10 @@
       <c r="D19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="82" t="s">
+      <c r="E19" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="83"/>
+      <c r="F19" s="84"/>
       <c r="G19" s="39"/>
       <c r="H19" s="41">
         <v>0</v>
@@ -3027,16 +3027,16 @@
       <c r="Q19" s="32">
         <v>1</v>
       </c>
-      <c r="R19" s="82" t="s">
+      <c r="R19" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S19" s="83"/>
-      <c r="T19" s="84"/>
-      <c r="U19" s="85" t="s">
+      <c r="S19" s="84"/>
+      <c r="T19" s="93"/>
+      <c r="U19" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="V19" s="86"/>
-      <c r="W19" s="86"/>
+      <c r="V19" s="95"/>
+      <c r="W19" s="95"/>
       <c r="X19" s="39"/>
       <c r="Y19" s="35" t="b">
         <v>1</v>
@@ -3062,10 +3062,10 @@
       <c r="D20" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="82" t="s">
+      <c r="E20" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="83"/>
+      <c r="F20" s="84"/>
       <c r="G20" s="39"/>
       <c r="H20" s="13">
         <v>0</v>
@@ -3097,16 +3097,16 @@
       <c r="Q20" s="12">
         <v>0</v>
       </c>
-      <c r="R20" s="82" t="s">
+      <c r="R20" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S20" s="83"/>
-      <c r="T20" s="84"/>
-      <c r="U20" s="85" t="s">
+      <c r="S20" s="84"/>
+      <c r="T20" s="93"/>
+      <c r="U20" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="V20" s="86"/>
-      <c r="W20" s="86"/>
+      <c r="V20" s="95"/>
+      <c r="W20" s="95"/>
       <c r="X20" s="39"/>
       <c r="Y20" s="36" t="b">
         <v>1</v>
@@ -3132,10 +3132,10 @@
       <c r="D21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="82" t="s">
+      <c r="E21" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="83"/>
+      <c r="F21" s="84"/>
       <c r="G21" s="39"/>
       <c r="H21" s="41">
         <v>0</v>
@@ -3167,16 +3167,16 @@
       <c r="Q21" s="32">
         <v>1</v>
       </c>
-      <c r="R21" s="82" t="s">
+      <c r="R21" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S21" s="83"/>
-      <c r="T21" s="84"/>
-      <c r="U21" s="85" t="s">
+      <c r="S21" s="84"/>
+      <c r="T21" s="93"/>
+      <c r="U21" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="V21" s="86"/>
-      <c r="W21" s="86"/>
+      <c r="V21" s="95"/>
+      <c r="W21" s="95"/>
       <c r="X21" s="39"/>
       <c r="Y21" s="35" t="b">
         <v>1</v>
@@ -3202,10 +3202,10 @@
       <c r="D22" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="82" t="s">
+      <c r="E22" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="83"/>
+      <c r="F22" s="84"/>
       <c r="G22" s="39"/>
       <c r="H22" s="13">
         <v>0</v>
@@ -3237,16 +3237,16 @@
       <c r="Q22" s="12">
         <v>0</v>
       </c>
-      <c r="R22" s="82" t="s">
+      <c r="R22" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S22" s="83"/>
-      <c r="T22" s="84"/>
-      <c r="U22" s="85" t="s">
+      <c r="S22" s="84"/>
+      <c r="T22" s="93"/>
+      <c r="U22" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="V22" s="86"/>
-      <c r="W22" s="86"/>
+      <c r="V22" s="95"/>
+      <c r="W22" s="95"/>
       <c r="X22" s="39"/>
       <c r="Y22" s="36" t="b">
         <v>1</v>
@@ -3272,10 +3272,10 @@
       <c r="D23" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="82" t="s">
+      <c r="E23" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="83"/>
+      <c r="F23" s="84"/>
       <c r="G23" s="39"/>
       <c r="H23" s="41">
         <v>0</v>
@@ -3307,16 +3307,16 @@
       <c r="Q23" s="32">
         <v>1</v>
       </c>
-      <c r="R23" s="82" t="s">
+      <c r="R23" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S23" s="83"/>
-      <c r="T23" s="84"/>
-      <c r="U23" s="85" t="s">
+      <c r="S23" s="84"/>
+      <c r="T23" s="93"/>
+      <c r="U23" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="V23" s="86"/>
-      <c r="W23" s="86"/>
+      <c r="V23" s="95"/>
+      <c r="W23" s="95"/>
       <c r="X23" s="39"/>
       <c r="Y23" s="35" t="b">
         <v>1</v>
@@ -3342,10 +3342,10 @@
       <c r="D24" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="82" t="s">
+      <c r="E24" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="83"/>
+      <c r="F24" s="84"/>
       <c r="G24" s="39"/>
       <c r="H24" s="13">
         <v>0</v>
@@ -3377,16 +3377,16 @@
       <c r="Q24" s="12">
         <v>0</v>
       </c>
-      <c r="R24" s="82" t="s">
+      <c r="R24" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S24" s="83"/>
-      <c r="T24" s="84"/>
-      <c r="U24" s="85" t="s">
+      <c r="S24" s="84"/>
+      <c r="T24" s="93"/>
+      <c r="U24" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="V24" s="86"/>
-      <c r="W24" s="86"/>
+      <c r="V24" s="95"/>
+      <c r="W24" s="95"/>
       <c r="X24" s="39"/>
       <c r="Y24" s="36" t="b">
         <v>1</v>
@@ -3449,16 +3449,16 @@
       <c r="Q25" s="32">
         <v>1</v>
       </c>
-      <c r="R25" s="82" t="s">
+      <c r="R25" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S25" s="83"/>
-      <c r="T25" s="84"/>
-      <c r="U25" s="85" t="s">
+      <c r="S25" s="84"/>
+      <c r="T25" s="93"/>
+      <c r="U25" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="V25" s="86"/>
-      <c r="W25" s="86"/>
+      <c r="V25" s="95"/>
+      <c r="W25" s="95"/>
       <c r="X25" s="39"/>
       <c r="Y25" s="35" t="b">
         <v>1</v>
@@ -3484,10 +3484,10 @@
       <c r="D26" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="82" t="s">
+      <c r="E26" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="83"/>
+      <c r="F26" s="84"/>
       <c r="G26" s="39"/>
       <c r="H26" s="13">
         <v>0</v>
@@ -3519,16 +3519,16 @@
       <c r="Q26" s="12">
         <v>0</v>
       </c>
-      <c r="R26" s="82" t="s">
+      <c r="R26" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S26" s="83"/>
-      <c r="T26" s="84"/>
-      <c r="U26" s="85" t="s">
+      <c r="S26" s="84"/>
+      <c r="T26" s="93"/>
+      <c r="U26" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="V26" s="86"/>
-      <c r="W26" s="86"/>
+      <c r="V26" s="95"/>
+      <c r="W26" s="95"/>
       <c r="X26" s="39"/>
       <c r="Y26" s="36" t="b">
         <v>1</v>
@@ -3554,10 +3554,10 @@
       <c r="D27" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="82" t="s">
+      <c r="E27" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="83"/>
+      <c r="F27" s="84"/>
       <c r="G27" s="39"/>
       <c r="H27" s="41">
         <v>0</v>
@@ -3589,16 +3589,16 @@
       <c r="Q27" s="32">
         <v>1</v>
       </c>
-      <c r="R27" s="82" t="s">
+      <c r="R27" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S27" s="83"/>
-      <c r="T27" s="84"/>
-      <c r="U27" s="85" t="s">
+      <c r="S27" s="84"/>
+      <c r="T27" s="93"/>
+      <c r="U27" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="V27" s="86"/>
-      <c r="W27" s="86"/>
+      <c r="V27" s="95"/>
+      <c r="W27" s="95"/>
       <c r="X27" s="39"/>
       <c r="Y27" s="35" t="b">
         <v>1</v>
@@ -3624,10 +3624,10 @@
       <c r="D28" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="82" t="s">
+      <c r="E28" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="83"/>
+      <c r="F28" s="84"/>
       <c r="G28" s="39"/>
       <c r="H28" s="13">
         <v>0</v>
@@ -3659,16 +3659,16 @@
       <c r="Q28" s="12">
         <v>0</v>
       </c>
-      <c r="R28" s="82" t="s">
+      <c r="R28" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S28" s="83"/>
-      <c r="T28" s="84"/>
-      <c r="U28" s="85" t="s">
+      <c r="S28" s="84"/>
+      <c r="T28" s="93"/>
+      <c r="U28" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="V28" s="86"/>
-      <c r="W28" s="86"/>
+      <c r="V28" s="95"/>
+      <c r="W28" s="95"/>
       <c r="X28" s="39"/>
       <c r="Y28" s="36" t="b">
         <v>1</v>
@@ -3731,16 +3731,16 @@
       <c r="Q29" s="32">
         <v>1</v>
       </c>
-      <c r="R29" s="82" t="s">
+      <c r="R29" s="83" t="s">
         <v>99</v>
       </c>
-      <c r="S29" s="83"/>
-      <c r="T29" s="84"/>
-      <c r="U29" s="102" t="s">
+      <c r="S29" s="84"/>
+      <c r="T29" s="93"/>
+      <c r="U29" s="96" t="s">
         <v>127</v>
       </c>
-      <c r="V29" s="103"/>
-      <c r="W29" s="103"/>
+      <c r="V29" s="97"/>
+      <c r="W29" s="97"/>
       <c r="X29" s="39"/>
       <c r="Y29" s="35" t="b">
         <v>0</v>
@@ -3766,10 +3766,10 @@
       <c r="D30" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="82" t="s">
+      <c r="E30" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="83"/>
+      <c r="F30" s="84"/>
       <c r="G30" s="39"/>
       <c r="H30" s="13">
         <v>0</v>
@@ -3801,16 +3801,16 @@
       <c r="Q30" s="12">
         <v>0</v>
       </c>
-      <c r="R30" s="82" t="s">
+      <c r="R30" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S30" s="83"/>
-      <c r="T30" s="84"/>
-      <c r="U30" s="85" t="s">
+      <c r="S30" s="84"/>
+      <c r="T30" s="93"/>
+      <c r="U30" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="V30" s="86"/>
-      <c r="W30" s="86"/>
+      <c r="V30" s="95"/>
+      <c r="W30" s="95"/>
       <c r="X30" s="39"/>
       <c r="Y30" s="36" t="b">
         <v>1</v>
@@ -3836,10 +3836,10 @@
       <c r="D31" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="82" t="s">
+      <c r="E31" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="83"/>
+      <c r="F31" s="84"/>
       <c r="G31" s="39"/>
       <c r="H31" s="41">
         <v>0</v>
@@ -3871,16 +3871,16 @@
       <c r="Q31" s="32">
         <v>1</v>
       </c>
-      <c r="R31" s="82" t="s">
+      <c r="R31" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="S31" s="83"/>
-      <c r="T31" s="84"/>
-      <c r="U31" s="85" t="s">
+      <c r="S31" s="84"/>
+      <c r="T31" s="93"/>
+      <c r="U31" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="V31" s="86"/>
-      <c r="W31" s="86"/>
+      <c r="V31" s="95"/>
+      <c r="W31" s="95"/>
       <c r="X31" s="39"/>
       <c r="Y31" s="35" t="b">
         <v>1</v>
@@ -3901,9 +3901,9 @@
       </c>
       <c r="B32" s="45"/>
       <c r="C32" s="34"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="81"/>
       <c r="G32" s="38"/>
       <c r="H32" s="15">
         <v>1</v>
@@ -3917,20 +3917,20 @@
       <c r="K32" s="4">
         <v>1</v>
       </c>
-      <c r="L32" s="75" t="s">
+      <c r="L32" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="M32" s="78"/>
-      <c r="N32" s="78"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="74"/>
-      <c r="R32" s="74"/>
-      <c r="S32" s="74"/>
-      <c r="T32" s="74"/>
-      <c r="U32" s="74"/>
-      <c r="V32" s="74"/>
-      <c r="W32" s="74"/>
+      <c r="M32" s="81"/>
+      <c r="N32" s="81"/>
+      <c r="O32" s="82"/>
+      <c r="P32" s="82"/>
+      <c r="Q32" s="82"/>
+      <c r="R32" s="82"/>
+      <c r="S32" s="82"/>
+      <c r="T32" s="82"/>
+      <c r="U32" s="82"/>
+      <c r="V32" s="82"/>
+      <c r="W32" s="82"/>
       <c r="X32" s="38"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="1"/>
@@ -3948,10 +3948,10 @@
       <c r="D33" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E33" s="89" t="s">
+      <c r="E33" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="F33" s="90"/>
+      <c r="F33" s="74"/>
       <c r="G33" s="39"/>
       <c r="H33" s="16">
         <v>1</v>
@@ -3968,21 +3968,21 @@
       <c r="L33" s="26">
         <v>0</v>
       </c>
-      <c r="M33" s="96" t="s">
+      <c r="M33" s="98" t="s">
         <v>104</v>
       </c>
-      <c r="N33" s="97"/>
-      <c r="O33" s="98"/>
-      <c r="P33" s="89" t="s">
+      <c r="N33" s="99"/>
+      <c r="O33" s="100"/>
+      <c r="P33" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q33" s="90"/>
-      <c r="R33" s="90"/>
-      <c r="S33" s="90"/>
-      <c r="T33" s="90"/>
-      <c r="U33" s="90"/>
-      <c r="V33" s="90"/>
-      <c r="W33" s="90"/>
+      <c r="Q33" s="74"/>
+      <c r="R33" s="74"/>
+      <c r="S33" s="74"/>
+      <c r="T33" s="74"/>
+      <c r="U33" s="74"/>
+      <c r="V33" s="74"/>
+      <c r="W33" s="74"/>
       <c r="X33" s="39"/>
       <c r="Y33" s="35" t="b">
         <v>0</v>
@@ -4008,10 +4008,10 @@
       <c r="D34" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E34" s="89" t="s">
+      <c r="E34" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="F34" s="90"/>
+      <c r="F34" s="74"/>
       <c r="G34" s="39"/>
       <c r="H34" s="16">
         <v>1</v>
@@ -4028,21 +4028,21 @@
       <c r="L34" s="5">
         <v>1</v>
       </c>
-      <c r="M34" s="96" t="s">
+      <c r="M34" s="98" t="s">
         <v>104</v>
       </c>
-      <c r="N34" s="97"/>
-      <c r="O34" s="98"/>
-      <c r="P34" s="89" t="s">
+      <c r="N34" s="99"/>
+      <c r="O34" s="100"/>
+      <c r="P34" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q34" s="90"/>
-      <c r="R34" s="90"/>
-      <c r="S34" s="90"/>
-      <c r="T34" s="90"/>
-      <c r="U34" s="90"/>
-      <c r="V34" s="90"/>
-      <c r="W34" s="90"/>
+      <c r="Q34" s="74"/>
+      <c r="R34" s="74"/>
+      <c r="S34" s="74"/>
+      <c r="T34" s="74"/>
+      <c r="U34" s="74"/>
+      <c r="V34" s="74"/>
+      <c r="W34" s="74"/>
       <c r="X34" s="39"/>
       <c r="Y34" s="36" t="b">
         <v>0</v>
@@ -4064,8 +4064,8 @@
       <c r="B35" s="45"/>
       <c r="C35" s="34"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="78"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="81"/>
       <c r="G35" s="38"/>
       <c r="H35" s="15">
         <v>1</v>
@@ -4079,20 +4079,20 @@
       <c r="K35" s="4">
         <v>1</v>
       </c>
-      <c r="L35" s="75" t="s">
+      <c r="L35" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="M35" s="78"/>
-      <c r="N35" s="78"/>
-      <c r="O35" s="78"/>
-      <c r="P35" s="78"/>
-      <c r="Q35" s="78"/>
-      <c r="R35" s="76"/>
-      <c r="S35" s="74"/>
-      <c r="T35" s="74"/>
-      <c r="U35" s="74"/>
-      <c r="V35" s="74"/>
-      <c r="W35" s="74"/>
+      <c r="M35" s="81"/>
+      <c r="N35" s="81"/>
+      <c r="O35" s="81"/>
+      <c r="P35" s="81"/>
+      <c r="Q35" s="81"/>
+      <c r="R35" s="101"/>
+      <c r="S35" s="82"/>
+      <c r="T35" s="82"/>
+      <c r="U35" s="82"/>
+      <c r="V35" s="82"/>
+      <c r="W35" s="82"/>
       <c r="X35" s="38"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="1"/>
@@ -4110,10 +4110,10 @@
       <c r="D36" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E36" s="104" t="s">
+      <c r="E36" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="F36" s="105"/>
+      <c r="F36" s="89"/>
       <c r="G36" s="39"/>
       <c r="H36" s="16">
         <v>1</v>
@@ -4142,15 +4142,15 @@
       <c r="P36" s="5">
         <v>0</v>
       </c>
-      <c r="Q36" s="89" t="s">
+      <c r="Q36" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="R36" s="90"/>
-      <c r="S36" s="90"/>
-      <c r="T36" s="90"/>
-      <c r="U36" s="90"/>
-      <c r="V36" s="90"/>
-      <c r="W36" s="90"/>
+      <c r="R36" s="74"/>
+      <c r="S36" s="74"/>
+      <c r="T36" s="74"/>
+      <c r="U36" s="74"/>
+      <c r="V36" s="74"/>
+      <c r="W36" s="74"/>
       <c r="X36" s="39"/>
       <c r="Y36" s="36" t="b">
         <v>0</v>
@@ -4176,10 +4176,10 @@
       <c r="D37" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E37" s="104" t="s">
+      <c r="E37" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="F37" s="105"/>
+      <c r="F37" s="89"/>
       <c r="G37" s="39"/>
       <c r="H37" s="16">
         <v>1</v>
@@ -4208,15 +4208,15 @@
       <c r="P37" s="26">
         <v>1</v>
       </c>
-      <c r="Q37" s="89" t="s">
+      <c r="Q37" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="R37" s="90"/>
-      <c r="S37" s="90"/>
-      <c r="T37" s="90"/>
-      <c r="U37" s="90"/>
-      <c r="V37" s="90"/>
-      <c r="W37" s="90"/>
+      <c r="R37" s="74"/>
+      <c r="S37" s="74"/>
+      <c r="T37" s="74"/>
+      <c r="U37" s="74"/>
+      <c r="V37" s="74"/>
+      <c r="W37" s="74"/>
       <c r="X37" s="39"/>
       <c r="Y37" s="35" t="b">
         <v>0</v>
@@ -4237,9 +4237,9 @@
       </c>
       <c r="B38" s="45"/>
       <c r="C38" s="34"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="78"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="81"/>
+      <c r="F38" s="81"/>
       <c r="G38" s="38"/>
       <c r="H38" s="42">
         <v>1</v>
@@ -4253,12 +4253,12 @@
       <c r="K38" s="21">
         <v>1</v>
       </c>
-      <c r="L38" s="74" t="s">
+      <c r="L38" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="M38" s="74"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="82"/>
+      <c r="O38" s="82"/>
       <c r="P38" s="66"/>
       <c r="Q38" s="66"/>
       <c r="R38" s="66"/>
@@ -4284,10 +4284,10 @@
       <c r="D39" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E39" s="67" t="s">
+      <c r="E39" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F39" s="68"/>
+      <c r="F39" s="76"/>
       <c r="G39" s="39"/>
       <c r="H39" s="16">
         <v>1</v>
@@ -4301,29 +4301,29 @@
       <c r="K39" s="10">
         <v>1</v>
       </c>
-      <c r="L39" s="99" t="s">
+      <c r="L39" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M39" s="100"/>
-      <c r="N39" s="100"/>
-      <c r="O39" s="101"/>
-      <c r="P39" s="89" t="s">
+      <c r="M39" s="91"/>
+      <c r="N39" s="91"/>
+      <c r="O39" s="92"/>
+      <c r="P39" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q39" s="90"/>
-      <c r="R39" s="90"/>
-      <c r="S39" s="90"/>
-      <c r="T39" s="90"/>
-      <c r="U39" s="90"/>
-      <c r="V39" s="90"/>
-      <c r="W39" s="90"/>
+      <c r="Q39" s="74"/>
+      <c r="R39" s="74"/>
+      <c r="S39" s="74"/>
+      <c r="T39" s="74"/>
+      <c r="U39" s="74"/>
+      <c r="V39" s="74"/>
+      <c r="W39" s="74"/>
       <c r="X39" s="39"/>
-      <c r="Y39" s="106" t="s">
+      <c r="Y39" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="Z39" s="107"/>
-      <c r="AA39" s="107"/>
-      <c r="AB39" s="108"/>
+      <c r="Z39" s="68"/>
+      <c r="AA39" s="68"/>
+      <c r="AB39" s="69"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" s="51" t="s">
@@ -4336,10 +4336,10 @@
       <c r="D40" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E40" s="67" t="s">
+      <c r="E40" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F40" s="68"/>
+      <c r="F40" s="76"/>
       <c r="G40" s="39"/>
       <c r="H40" s="16">
         <v>1</v>
@@ -4353,29 +4353,29 @@
       <c r="K40" s="10">
         <v>1</v>
       </c>
-      <c r="L40" s="99" t="s">
+      <c r="L40" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M40" s="100"/>
-      <c r="N40" s="100"/>
-      <c r="O40" s="101"/>
-      <c r="P40" s="89" t="s">
+      <c r="M40" s="91"/>
+      <c r="N40" s="91"/>
+      <c r="O40" s="92"/>
+      <c r="P40" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q40" s="90"/>
-      <c r="R40" s="90"/>
-      <c r="S40" s="90"/>
-      <c r="T40" s="90"/>
-      <c r="U40" s="90"/>
-      <c r="V40" s="90"/>
-      <c r="W40" s="90"/>
+      <c r="Q40" s="74"/>
+      <c r="R40" s="74"/>
+      <c r="S40" s="74"/>
+      <c r="T40" s="74"/>
+      <c r="U40" s="74"/>
+      <c r="V40" s="74"/>
+      <c r="W40" s="74"/>
       <c r="X40" s="39"/>
-      <c r="Y40" s="109" t="s">
+      <c r="Y40" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="Z40" s="110"/>
-      <c r="AA40" s="110"/>
-      <c r="AB40" s="111"/>
+      <c r="Z40" s="71"/>
+      <c r="AA40" s="71"/>
+      <c r="AB40" s="72"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" s="53" t="s">
@@ -4388,10 +4388,10 @@
       <c r="D41" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E41" s="67" t="s">
+      <c r="E41" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F41" s="68"/>
+      <c r="F41" s="76"/>
       <c r="G41" s="39"/>
       <c r="H41" s="16">
         <v>1</v>
@@ -4405,29 +4405,29 @@
       <c r="K41" s="10">
         <v>1</v>
       </c>
-      <c r="L41" s="99" t="s">
+      <c r="L41" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M41" s="100"/>
-      <c r="N41" s="100"/>
-      <c r="O41" s="101"/>
-      <c r="P41" s="89" t="s">
+      <c r="M41" s="91"/>
+      <c r="N41" s="91"/>
+      <c r="O41" s="92"/>
+      <c r="P41" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q41" s="90"/>
-      <c r="R41" s="90"/>
-      <c r="S41" s="90"/>
-      <c r="T41" s="90"/>
-      <c r="U41" s="90"/>
-      <c r="V41" s="90"/>
-      <c r="W41" s="90"/>
+      <c r="Q41" s="74"/>
+      <c r="R41" s="74"/>
+      <c r="S41" s="74"/>
+      <c r="T41" s="74"/>
+      <c r="U41" s="74"/>
+      <c r="V41" s="74"/>
+      <c r="W41" s="74"/>
       <c r="X41" s="39"/>
-      <c r="Y41" s="106" t="s">
+      <c r="Y41" s="67" t="s">
         <v>131</v>
       </c>
-      <c r="Z41" s="107"/>
-      <c r="AA41" s="107"/>
-      <c r="AB41" s="108"/>
+      <c r="Z41" s="68"/>
+      <c r="AA41" s="68"/>
+      <c r="AB41" s="69"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="51" t="s">
@@ -4440,10 +4440,10 @@
       <c r="D42" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E42" s="67" t="s">
+      <c r="E42" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F42" s="68"/>
+      <c r="F42" s="76"/>
       <c r="G42" s="39"/>
       <c r="H42" s="16">
         <v>1</v>
@@ -4457,29 +4457,29 @@
       <c r="K42" s="10">
         <v>1</v>
       </c>
-      <c r="L42" s="99" t="s">
+      <c r="L42" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M42" s="100"/>
-      <c r="N42" s="100"/>
-      <c r="O42" s="101"/>
-      <c r="P42" s="89" t="s">
+      <c r="M42" s="91"/>
+      <c r="N42" s="91"/>
+      <c r="O42" s="92"/>
+      <c r="P42" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q42" s="90"/>
-      <c r="R42" s="90"/>
-      <c r="S42" s="90"/>
-      <c r="T42" s="90"/>
-      <c r="U42" s="90"/>
-      <c r="V42" s="90"/>
-      <c r="W42" s="90"/>
+      <c r="Q42" s="74"/>
+      <c r="R42" s="74"/>
+      <c r="S42" s="74"/>
+      <c r="T42" s="74"/>
+      <c r="U42" s="74"/>
+      <c r="V42" s="74"/>
+      <c r="W42" s="74"/>
       <c r="X42" s="39"/>
-      <c r="Y42" s="109" t="s">
+      <c r="Y42" s="70" t="s">
         <v>132</v>
       </c>
-      <c r="Z42" s="110"/>
-      <c r="AA42" s="110"/>
-      <c r="AB42" s="111"/>
+      <c r="Z42" s="71"/>
+      <c r="AA42" s="71"/>
+      <c r="AB42" s="72"/>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" s="53" t="s">
@@ -4492,10 +4492,10 @@
       <c r="D43" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E43" s="67" t="s">
+      <c r="E43" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F43" s="68"/>
+      <c r="F43" s="76"/>
       <c r="G43" s="39"/>
       <c r="H43" s="16">
         <v>1</v>
@@ -4509,29 +4509,29 @@
       <c r="K43" s="10">
         <v>1</v>
       </c>
-      <c r="L43" s="99" t="s">
+      <c r="L43" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M43" s="100"/>
-      <c r="N43" s="100"/>
-      <c r="O43" s="101"/>
-      <c r="P43" s="89" t="s">
+      <c r="M43" s="91"/>
+      <c r="N43" s="91"/>
+      <c r="O43" s="92"/>
+      <c r="P43" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q43" s="90"/>
-      <c r="R43" s="90"/>
-      <c r="S43" s="90"/>
-      <c r="T43" s="90"/>
-      <c r="U43" s="90"/>
-      <c r="V43" s="90"/>
-      <c r="W43" s="90"/>
+      <c r="Q43" s="74"/>
+      <c r="R43" s="74"/>
+      <c r="S43" s="74"/>
+      <c r="T43" s="74"/>
+      <c r="U43" s="74"/>
+      <c r="V43" s="74"/>
+      <c r="W43" s="74"/>
       <c r="X43" s="39"/>
-      <c r="Y43" s="106" t="s">
+      <c r="Y43" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="Z43" s="107"/>
-      <c r="AA43" s="107"/>
-      <c r="AB43" s="108"/>
+      <c r="Z43" s="68"/>
+      <c r="AA43" s="68"/>
+      <c r="AB43" s="69"/>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" s="51" t="s">
@@ -4544,10 +4544,10 @@
       <c r="D44" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E44" s="67" t="s">
+      <c r="E44" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F44" s="68"/>
+      <c r="F44" s="76"/>
       <c r="G44" s="39"/>
       <c r="H44" s="16">
         <v>1</v>
@@ -4561,29 +4561,29 @@
       <c r="K44" s="10">
         <v>1</v>
       </c>
-      <c r="L44" s="99" t="s">
+      <c r="L44" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M44" s="100"/>
-      <c r="N44" s="100"/>
-      <c r="O44" s="101"/>
-      <c r="P44" s="89" t="s">
+      <c r="M44" s="91"/>
+      <c r="N44" s="91"/>
+      <c r="O44" s="92"/>
+      <c r="P44" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q44" s="90"/>
-      <c r="R44" s="90"/>
-      <c r="S44" s="90"/>
-      <c r="T44" s="90"/>
-      <c r="U44" s="90"/>
-      <c r="V44" s="90"/>
-      <c r="W44" s="90"/>
+      <c r="Q44" s="74"/>
+      <c r="R44" s="74"/>
+      <c r="S44" s="74"/>
+      <c r="T44" s="74"/>
+      <c r="U44" s="74"/>
+      <c r="V44" s="74"/>
+      <c r="W44" s="74"/>
       <c r="X44" s="39"/>
-      <c r="Y44" s="109" t="s">
+      <c r="Y44" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="Z44" s="110"/>
-      <c r="AA44" s="110"/>
-      <c r="AB44" s="111"/>
+      <c r="Z44" s="71"/>
+      <c r="AA44" s="71"/>
+      <c r="AB44" s="72"/>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" s="53" t="s">
@@ -4596,10 +4596,10 @@
       <c r="D45" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E45" s="67" t="s">
+      <c r="E45" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F45" s="68"/>
+      <c r="F45" s="76"/>
       <c r="G45" s="39"/>
       <c r="H45" s="16">
         <v>1</v>
@@ -4613,29 +4613,29 @@
       <c r="K45" s="10">
         <v>1</v>
       </c>
-      <c r="L45" s="99" t="s">
+      <c r="L45" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M45" s="100"/>
-      <c r="N45" s="100"/>
-      <c r="O45" s="101"/>
-      <c r="P45" s="89" t="s">
+      <c r="M45" s="91"/>
+      <c r="N45" s="91"/>
+      <c r="O45" s="92"/>
+      <c r="P45" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q45" s="90"/>
-      <c r="R45" s="90"/>
-      <c r="S45" s="90"/>
-      <c r="T45" s="90"/>
-      <c r="U45" s="90"/>
-      <c r="V45" s="90"/>
-      <c r="W45" s="90"/>
+      <c r="Q45" s="74"/>
+      <c r="R45" s="74"/>
+      <c r="S45" s="74"/>
+      <c r="T45" s="74"/>
+      <c r="U45" s="74"/>
+      <c r="V45" s="74"/>
+      <c r="W45" s="74"/>
       <c r="X45" s="39"/>
-      <c r="Y45" s="106" t="s">
+      <c r="Y45" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="Z45" s="107"/>
-      <c r="AA45" s="107"/>
-      <c r="AB45" s="108"/>
+      <c r="Z45" s="68"/>
+      <c r="AA45" s="68"/>
+      <c r="AB45" s="69"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" s="51" t="s">
@@ -4648,10 +4648,10 @@
       <c r="D46" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E46" s="67" t="s">
+      <c r="E46" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F46" s="68"/>
+      <c r="F46" s="76"/>
       <c r="G46" s="39"/>
       <c r="H46" s="16">
         <v>1</v>
@@ -4665,29 +4665,29 @@
       <c r="K46" s="10">
         <v>1</v>
       </c>
-      <c r="L46" s="99" t="s">
+      <c r="L46" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M46" s="100"/>
-      <c r="N46" s="100"/>
-      <c r="O46" s="101"/>
-      <c r="P46" s="89" t="s">
+      <c r="M46" s="91"/>
+      <c r="N46" s="91"/>
+      <c r="O46" s="92"/>
+      <c r="P46" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q46" s="90"/>
-      <c r="R46" s="90"/>
-      <c r="S46" s="90"/>
-      <c r="T46" s="90"/>
-      <c r="U46" s="90"/>
-      <c r="V46" s="90"/>
-      <c r="W46" s="90"/>
+      <c r="Q46" s="74"/>
+      <c r="R46" s="74"/>
+      <c r="S46" s="74"/>
+      <c r="T46" s="74"/>
+      <c r="U46" s="74"/>
+      <c r="V46" s="74"/>
+      <c r="W46" s="74"/>
       <c r="X46" s="39"/>
-      <c r="Y46" s="109" t="s">
+      <c r="Y46" s="70" t="s">
         <v>136</v>
       </c>
-      <c r="Z46" s="110"/>
-      <c r="AA46" s="110"/>
-      <c r="AB46" s="111"/>
+      <c r="Z46" s="71"/>
+      <c r="AA46" s="71"/>
+      <c r="AB46" s="72"/>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" s="53" t="s">
@@ -4700,10 +4700,10 @@
       <c r="D47" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E47" s="67" t="s">
+      <c r="E47" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F47" s="68"/>
+      <c r="F47" s="76"/>
       <c r="G47" s="39"/>
       <c r="H47" s="16">
         <v>1</v>
@@ -4717,29 +4717,29 @@
       <c r="K47" s="10">
         <v>1</v>
       </c>
-      <c r="L47" s="99" t="s">
+      <c r="L47" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M47" s="100"/>
-      <c r="N47" s="100"/>
-      <c r="O47" s="101"/>
-      <c r="P47" s="89" t="s">
+      <c r="M47" s="91"/>
+      <c r="N47" s="91"/>
+      <c r="O47" s="92"/>
+      <c r="P47" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q47" s="90"/>
-      <c r="R47" s="90"/>
-      <c r="S47" s="90"/>
-      <c r="T47" s="90"/>
-      <c r="U47" s="90"/>
-      <c r="V47" s="90"/>
-      <c r="W47" s="90"/>
+      <c r="Q47" s="74"/>
+      <c r="R47" s="74"/>
+      <c r="S47" s="74"/>
+      <c r="T47" s="74"/>
+      <c r="U47" s="74"/>
+      <c r="V47" s="74"/>
+      <c r="W47" s="74"/>
       <c r="X47" s="39"/>
-      <c r="Y47" s="106" t="s">
+      <c r="Y47" s="67" t="s">
         <v>137</v>
       </c>
-      <c r="Z47" s="107"/>
-      <c r="AA47" s="107"/>
-      <c r="AB47" s="108"/>
+      <c r="Z47" s="68"/>
+      <c r="AA47" s="68"/>
+      <c r="AB47" s="69"/>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A48" s="51" t="s">
@@ -4752,10 +4752,10 @@
       <c r="D48" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E48" s="67" t="s">
+      <c r="E48" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F48" s="68"/>
+      <c r="F48" s="76"/>
       <c r="G48" s="39"/>
       <c r="H48" s="16">
         <v>1</v>
@@ -4769,29 +4769,29 @@
       <c r="K48" s="10">
         <v>1</v>
       </c>
-      <c r="L48" s="99" t="s">
+      <c r="L48" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M48" s="100"/>
-      <c r="N48" s="100"/>
-      <c r="O48" s="101"/>
-      <c r="P48" s="89" t="s">
+      <c r="M48" s="91"/>
+      <c r="N48" s="91"/>
+      <c r="O48" s="92"/>
+      <c r="P48" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q48" s="90"/>
-      <c r="R48" s="90"/>
-      <c r="S48" s="90"/>
-      <c r="T48" s="90"/>
-      <c r="U48" s="90"/>
-      <c r="V48" s="90"/>
-      <c r="W48" s="90"/>
+      <c r="Q48" s="74"/>
+      <c r="R48" s="74"/>
+      <c r="S48" s="74"/>
+      <c r="T48" s="74"/>
+      <c r="U48" s="74"/>
+      <c r="V48" s="74"/>
+      <c r="W48" s="74"/>
       <c r="X48" s="39"/>
-      <c r="Y48" s="109" t="s">
+      <c r="Y48" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="Z48" s="110"/>
-      <c r="AA48" s="110"/>
-      <c r="AB48" s="111"/>
+      <c r="Z48" s="71"/>
+      <c r="AA48" s="71"/>
+      <c r="AB48" s="72"/>
     </row>
     <row r="49" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A49" s="53" t="s">
@@ -4804,10 +4804,10 @@
       <c r="D49" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E49" s="67" t="s">
+      <c r="E49" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F49" s="68"/>
+      <c r="F49" s="76"/>
       <c r="G49" s="39"/>
       <c r="H49" s="16">
         <v>1</v>
@@ -4821,29 +4821,29 @@
       <c r="K49" s="10">
         <v>1</v>
       </c>
-      <c r="L49" s="99" t="s">
+      <c r="L49" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M49" s="100"/>
-      <c r="N49" s="100"/>
-      <c r="O49" s="101"/>
-      <c r="P49" s="89" t="s">
+      <c r="M49" s="91"/>
+      <c r="N49" s="91"/>
+      <c r="O49" s="92"/>
+      <c r="P49" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q49" s="90"/>
-      <c r="R49" s="90"/>
-      <c r="S49" s="90"/>
-      <c r="T49" s="90"/>
-      <c r="U49" s="90"/>
-      <c r="V49" s="90"/>
-      <c r="W49" s="90"/>
+      <c r="Q49" s="74"/>
+      <c r="R49" s="74"/>
+      <c r="S49" s="74"/>
+      <c r="T49" s="74"/>
+      <c r="U49" s="74"/>
+      <c r="V49" s="74"/>
+      <c r="W49" s="74"/>
       <c r="X49" s="39"/>
-      <c r="Y49" s="106" t="s">
+      <c r="Y49" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="Z49" s="107"/>
-      <c r="AA49" s="107"/>
-      <c r="AB49" s="108"/>
+      <c r="Z49" s="68"/>
+      <c r="AA49" s="68"/>
+      <c r="AB49" s="69"/>
       <c r="AP49" s="9" t="s">
         <v>128</v>
       </c>
@@ -4859,10 +4859,10 @@
       <c r="D50" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E50" s="67" t="s">
+      <c r="E50" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F50" s="68"/>
+      <c r="F50" s="76"/>
       <c r="G50" s="39"/>
       <c r="H50" s="16">
         <v>1</v>
@@ -4876,29 +4876,29 @@
       <c r="K50" s="10">
         <v>1</v>
       </c>
-      <c r="L50" s="99" t="s">
+      <c r="L50" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M50" s="100"/>
-      <c r="N50" s="100"/>
-      <c r="O50" s="101"/>
-      <c r="P50" s="89" t="s">
+      <c r="M50" s="91"/>
+      <c r="N50" s="91"/>
+      <c r="O50" s="92"/>
+      <c r="P50" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q50" s="90"/>
-      <c r="R50" s="90"/>
-      <c r="S50" s="90"/>
-      <c r="T50" s="90"/>
-      <c r="U50" s="90"/>
-      <c r="V50" s="90"/>
-      <c r="W50" s="90"/>
+      <c r="Q50" s="74"/>
+      <c r="R50" s="74"/>
+      <c r="S50" s="74"/>
+      <c r="T50" s="74"/>
+      <c r="U50" s="74"/>
+      <c r="V50" s="74"/>
+      <c r="W50" s="74"/>
       <c r="X50" s="39"/>
-      <c r="Y50" s="109" t="s">
+      <c r="Y50" s="70" t="s">
         <v>140</v>
       </c>
-      <c r="Z50" s="110"/>
-      <c r="AA50" s="110"/>
-      <c r="AB50" s="111"/>
+      <c r="Z50" s="71"/>
+      <c r="AA50" s="71"/>
+      <c r="AB50" s="72"/>
     </row>
     <row r="51" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A51" s="53" t="s">
@@ -4911,10 +4911,10 @@
       <c r="D51" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E51" s="67" t="s">
+      <c r="E51" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F51" s="68"/>
+      <c r="F51" s="76"/>
       <c r="G51" s="39"/>
       <c r="H51" s="16">
         <v>1</v>
@@ -4928,29 +4928,29 @@
       <c r="K51" s="10">
         <v>1</v>
       </c>
-      <c r="L51" s="99" t="s">
+      <c r="L51" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M51" s="100"/>
-      <c r="N51" s="100"/>
-      <c r="O51" s="101"/>
-      <c r="P51" s="89" t="s">
+      <c r="M51" s="91"/>
+      <c r="N51" s="91"/>
+      <c r="O51" s="92"/>
+      <c r="P51" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q51" s="90"/>
-      <c r="R51" s="90"/>
-      <c r="S51" s="90"/>
-      <c r="T51" s="90"/>
-      <c r="U51" s="90"/>
-      <c r="V51" s="90"/>
-      <c r="W51" s="90"/>
+      <c r="Q51" s="74"/>
+      <c r="R51" s="74"/>
+      <c r="S51" s="74"/>
+      <c r="T51" s="74"/>
+      <c r="U51" s="74"/>
+      <c r="V51" s="74"/>
+      <c r="W51" s="74"/>
       <c r="X51" s="39"/>
-      <c r="Y51" s="106" t="s">
+      <c r="Y51" s="67" t="s">
         <v>141</v>
       </c>
-      <c r="Z51" s="107"/>
-      <c r="AA51" s="107"/>
-      <c r="AB51" s="108"/>
+      <c r="Z51" s="68"/>
+      <c r="AA51" s="68"/>
+      <c r="AB51" s="69"/>
     </row>
     <row r="52" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A52" s="51" t="s">
@@ -4963,10 +4963,10 @@
       <c r="D52" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E52" s="67" t="s">
+      <c r="E52" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F52" s="68"/>
+      <c r="F52" s="76"/>
       <c r="G52" s="39"/>
       <c r="H52" s="16">
         <v>1</v>
@@ -4980,29 +4980,29 @@
       <c r="K52" s="10">
         <v>1</v>
       </c>
-      <c r="L52" s="99" t="s">
+      <c r="L52" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M52" s="100"/>
-      <c r="N52" s="100"/>
-      <c r="O52" s="101"/>
-      <c r="P52" s="89" t="s">
+      <c r="M52" s="91"/>
+      <c r="N52" s="91"/>
+      <c r="O52" s="92"/>
+      <c r="P52" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q52" s="90"/>
-      <c r="R52" s="90"/>
-      <c r="S52" s="90"/>
-      <c r="T52" s="90"/>
-      <c r="U52" s="90"/>
-      <c r="V52" s="90"/>
-      <c r="W52" s="90"/>
+      <c r="Q52" s="74"/>
+      <c r="R52" s="74"/>
+      <c r="S52" s="74"/>
+      <c r="T52" s="74"/>
+      <c r="U52" s="74"/>
+      <c r="V52" s="74"/>
+      <c r="W52" s="74"/>
       <c r="X52" s="39"/>
-      <c r="Y52" s="109" t="s">
+      <c r="Y52" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="Z52" s="110"/>
-      <c r="AA52" s="110"/>
-      <c r="AB52" s="111"/>
+      <c r="Z52" s="71"/>
+      <c r="AA52" s="71"/>
+      <c r="AB52" s="72"/>
     </row>
     <row r="53" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A53" s="53" t="s">
@@ -5015,10 +5015,10 @@
       <c r="D53" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E53" s="67" t="s">
+      <c r="E53" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="F53" s="68"/>
+      <c r="F53" s="76"/>
       <c r="G53" s="39"/>
       <c r="H53" s="16">
         <v>1</v>
@@ -5032,22 +5032,22 @@
       <c r="K53" s="10">
         <v>1</v>
       </c>
-      <c r="L53" s="99" t="s">
+      <c r="L53" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="M53" s="100"/>
-      <c r="N53" s="100"/>
-      <c r="O53" s="101"/>
-      <c r="P53" s="89" t="s">
+      <c r="M53" s="91"/>
+      <c r="N53" s="91"/>
+      <c r="O53" s="92"/>
+      <c r="P53" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="Q53" s="90"/>
-      <c r="R53" s="90"/>
-      <c r="S53" s="90"/>
-      <c r="T53" s="90"/>
-      <c r="U53" s="90"/>
-      <c r="V53" s="90"/>
-      <c r="W53" s="90"/>
+      <c r="Q53" s="74"/>
+      <c r="R53" s="74"/>
+      <c r="S53" s="74"/>
+      <c r="T53" s="74"/>
+      <c r="U53" s="74"/>
+      <c r="V53" s="74"/>
+      <c r="W53" s="74"/>
       <c r="X53" s="39"/>
       <c r="Y53" s="37" t="b">
         <v>0</v>
@@ -5073,10 +5073,10 @@
       <c r="D54" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="E54" s="69" t="s">
+      <c r="E54" s="111" t="s">
         <v>121</v>
       </c>
-      <c r="F54" s="70"/>
+      <c r="F54" s="112"/>
       <c r="G54" s="58"/>
       <c r="H54" s="60">
         <v>1</v>
@@ -5093,19 +5093,19 @@
       <c r="L54" s="23">
         <v>0</v>
       </c>
-      <c r="M54" s="113" t="s">
+      <c r="M54" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="N54" s="114"/>
-      <c r="O54" s="114"/>
-      <c r="P54" s="114"/>
-      <c r="Q54" s="114"/>
-      <c r="R54" s="114"/>
-      <c r="S54" s="114"/>
-      <c r="T54" s="114"/>
-      <c r="U54" s="114"/>
-      <c r="V54" s="114"/>
-      <c r="W54" s="114"/>
+      <c r="N54" s="79"/>
+      <c r="O54" s="79"/>
+      <c r="P54" s="79"/>
+      <c r="Q54" s="79"/>
+      <c r="R54" s="79"/>
+      <c r="S54" s="79"/>
+      <c r="T54" s="79"/>
+      <c r="U54" s="79"/>
+      <c r="V54" s="79"/>
+      <c r="W54" s="79"/>
       <c r="X54" s="58"/>
       <c r="Y54" s="61" t="b">
         <v>0</v>
@@ -5122,19 +5122,139 @@
     </row>
   </sheetData>
   <mergeCells count="170">
-    <mergeCell ref="Y39:AB39"/>
-    <mergeCell ref="Y40:AB40"/>
-    <mergeCell ref="Y41:AB41"/>
-    <mergeCell ref="Y42:AB42"/>
-    <mergeCell ref="Y43:AB43"/>
-    <mergeCell ref="Y44:AB44"/>
-    <mergeCell ref="Y45:AB45"/>
-    <mergeCell ref="Y46:AB46"/>
-    <mergeCell ref="P39:W39"/>
-    <mergeCell ref="P40:W40"/>
-    <mergeCell ref="P41:W41"/>
-    <mergeCell ref="P42:W42"/>
-    <mergeCell ref="P43:W43"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="U7:W7"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="R31:T31"/>
+    <mergeCell ref="U31:W31"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="M4:Q4"/>
+    <mergeCell ref="M5:Q5"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="U20:W20"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="U21:W21"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:W11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="P12:W12"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="Q36:W36"/>
+    <mergeCell ref="Q37:W37"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="U30:W30"/>
+    <mergeCell ref="U27:W27"/>
+    <mergeCell ref="L35:R35"/>
+    <mergeCell ref="S35:W35"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="U25:W25"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="U26:W26"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="L47:O47"/>
+    <mergeCell ref="L48:O48"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:O40"/>
+    <mergeCell ref="L41:O41"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="L43:O43"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="U28:W28"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="U29:W29"/>
+    <mergeCell ref="R30:T30"/>
+    <mergeCell ref="P44:W44"/>
+    <mergeCell ref="P45:W45"/>
+    <mergeCell ref="P46:W46"/>
+    <mergeCell ref="P47:W47"/>
+    <mergeCell ref="P48:W48"/>
+    <mergeCell ref="L38:O38"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="L45:O45"/>
+    <mergeCell ref="L46:O46"/>
+    <mergeCell ref="L49:O49"/>
+    <mergeCell ref="L50:O50"/>
+    <mergeCell ref="L51:O51"/>
+    <mergeCell ref="L52:O52"/>
+    <mergeCell ref="P49:W49"/>
+    <mergeCell ref="P50:W50"/>
+    <mergeCell ref="P51:W51"/>
+    <mergeCell ref="P52:W52"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="P53:W53"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="P13:W13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="P14:W14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="Y47:AB47"/>
     <mergeCell ref="Y48:AB48"/>
     <mergeCell ref="Y49:AB49"/>
@@ -5159,139 +5279,19 @@
     <mergeCell ref="R15:W15"/>
     <mergeCell ref="L32:N32"/>
     <mergeCell ref="O32:W32"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P13:W13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="P14:W14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="L49:O49"/>
-    <mergeCell ref="L50:O50"/>
-    <mergeCell ref="L51:O51"/>
-    <mergeCell ref="L52:O52"/>
-    <mergeCell ref="P49:W49"/>
-    <mergeCell ref="P50:W50"/>
-    <mergeCell ref="P51:W51"/>
-    <mergeCell ref="P52:W52"/>
-    <mergeCell ref="L53:O53"/>
-    <mergeCell ref="P53:W53"/>
-    <mergeCell ref="L47:O47"/>
-    <mergeCell ref="L48:O48"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:O40"/>
-    <mergeCell ref="L41:O41"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="L43:O43"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="U28:W28"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="U29:W29"/>
-    <mergeCell ref="R30:T30"/>
-    <mergeCell ref="P44:W44"/>
-    <mergeCell ref="P45:W45"/>
-    <mergeCell ref="P46:W46"/>
-    <mergeCell ref="P47:W47"/>
-    <mergeCell ref="P48:W48"/>
-    <mergeCell ref="L38:O38"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="L45:O45"/>
-    <mergeCell ref="L46:O46"/>
-    <mergeCell ref="P12:W12"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="Q36:W36"/>
-    <mergeCell ref="Q37:W37"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="U30:W30"/>
-    <mergeCell ref="U27:W27"/>
-    <mergeCell ref="L35:R35"/>
-    <mergeCell ref="S35:W35"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="U25:W25"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="U26:W26"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="U20:W20"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="U21:W21"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="U4:W4"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:W11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="Y6:AB6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="U7:W7"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="U9:W9"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="R31:T31"/>
-    <mergeCell ref="U31:W31"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="M5:Q5"/>
-    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="Y39:AB39"/>
+    <mergeCell ref="Y40:AB40"/>
+    <mergeCell ref="Y41:AB41"/>
+    <mergeCell ref="Y42:AB42"/>
+    <mergeCell ref="Y43:AB43"/>
+    <mergeCell ref="Y44:AB44"/>
+    <mergeCell ref="Y45:AB45"/>
+    <mergeCell ref="Y46:AB46"/>
+    <mergeCell ref="P39:W39"/>
+    <mergeCell ref="P40:W40"/>
+    <mergeCell ref="P41:W41"/>
+    <mergeCell ref="P42:W42"/>
+    <mergeCell ref="P43:W43"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5468,20 +5468,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b05417e1-eb89-4392-aea8-ecdaf8fc0423" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b05417e1-eb89-4392-aea8-ecdaf8fc0423" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5503,6 +5503,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEFCFB9-977F-4BC6-8CD6-7A1E4BA64254}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE327FA-98F8-4626-AE66-90F799A55F58}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5516,12 +5524,4 @@
     <ds:schemaRef ds:uri="b05417e1-eb89-4392-aea8-ecdaf8fc0423"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEFCFB9-977F-4BC6-8CD6-7A1E4BA64254}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Le .bin se lance !
</commit_message>
<xml_diff>
--- a/Encodage_PARM.xlsx
+++ b/Encodage_PARM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monsi\Desktop\Ecole\Polytech_Nice\Architecture\Projet-P-ARM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\habib\PROJARCHI\Projet-P-ARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A263F9FE-7037-439A-92B8-6476DCDC427E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F20566-B01E-4588-922A-652592329052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15216" yWindow="0" windowWidth="7920" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encodage PARM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="147">
   <si>
     <t>Description</t>
   </si>
@@ -472,12 +472,6 @@
     <t>Rm</t>
   </si>
   <si>
-    <t>BCS</t>
-  </si>
-  <si>
-    <t>BCC</t>
-  </si>
-  <si>
     <t>BVS</t>
   </si>
   <si>
@@ -656,6 +650,21 @@
   </si>
   <si>
     <t>Sub 8-bit immediate</t>
+  </si>
+  <si>
+    <t>BCS OU BHS</t>
+  </si>
+  <si>
+    <t>BCC OU BLO</t>
+  </si>
+  <si>
+    <t>BVC</t>
+  </si>
+  <si>
+    <t>&lt;Rd&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Rn&gt;</t>
   </si>
 </sst>
 </file>
@@ -1346,11 +1355,125 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1400,18 +1523,6 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1421,110 +1532,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1852,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="92" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="F12" zoomScale="92" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1872,54 +1881,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="47"/>
-      <c r="C1" s="104" t="s">
+      <c r="C1" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="106"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="93"/>
       <c r="G1" s="48"/>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111"/>
       <c r="X1" s="49"/>
-      <c r="Y1" s="104" t="s">
+      <c r="Y1" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="105"/>
-      <c r="AA1" s="105"/>
-      <c r="AB1" s="113"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="71"/>
+      <c r="AB1" s="72"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" s="103"/>
+      <c r="A2" s="92"/>
       <c r="B2" s="45"/>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="82"/>
-      <c r="F2" s="80"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="74"/>
       <c r="G2" s="38"/>
       <c r="H2" s="3">
         <v>15</v>
@@ -1992,13 +2001,13 @@
         <v>64</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="41">
@@ -2016,23 +2025,23 @@
       <c r="L3" s="32">
         <v>0</v>
       </c>
-      <c r="M3" s="73" t="s">
-        <v>102</v>
-      </c>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="107" t="s">
+      <c r="M3" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="90"/>
+      <c r="R3" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="S3" s="79"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="S3" s="108"/>
-      <c r="T3" s="109"/>
-      <c r="U3" s="85" t="s">
-        <v>101</v>
-      </c>
-      <c r="V3" s="86"/>
-      <c r="W3" s="86"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="87"/>
       <c r="X3" s="39"/>
       <c r="Y3" s="35" t="b">
         <v>1</v>
@@ -2056,13 +2065,13 @@
         <v>65</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G4" s="39"/>
       <c r="H4" s="13">
@@ -2080,23 +2089,23 @@
       <c r="L4" s="12">
         <v>1</v>
       </c>
-      <c r="M4" s="73" t="s">
-        <v>102</v>
-      </c>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="110"/>
-      <c r="R4" s="107" t="s">
+      <c r="M4" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="S4" s="79"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="S4" s="108"/>
-      <c r="T4" s="109"/>
-      <c r="U4" s="85" t="s">
-        <v>101</v>
-      </c>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="87"/>
       <c r="X4" s="39"/>
       <c r="Y4" s="36" t="b">
         <v>1</v>
@@ -2120,13 +2129,13 @@
         <v>66</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G5" s="39"/>
       <c r="H5" s="41">
@@ -2144,23 +2153,23 @@
       <c r="L5" s="32">
         <v>0</v>
       </c>
-      <c r="M5" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="110"/>
-      <c r="R5" s="107" t="s">
+      <c r="M5" s="88" t="s">
+        <v>101</v>
+      </c>
+      <c r="N5" s="89"/>
+      <c r="O5" s="89"/>
+      <c r="P5" s="89"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="S5" s="79"/>
+      <c r="T5" s="80"/>
+      <c r="U5" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="S5" s="108"/>
-      <c r="T5" s="109"/>
-      <c r="U5" s="85" t="s">
-        <v>101</v>
-      </c>
-      <c r="V5" s="86"/>
-      <c r="W5" s="86"/>
+      <c r="V5" s="87"/>
+      <c r="W5" s="87"/>
       <c r="X5" s="39"/>
       <c r="Y5" s="35" t="b">
         <v>1</v>
@@ -2181,9 +2190,9 @@
       </c>
       <c r="B6" s="45"/>
       <c r="C6" s="34"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="80"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="74"/>
       <c r="G6" s="38"/>
       <c r="H6" s="3">
         <v>0</v>
@@ -2191,27 +2200,27 @@
       <c r="I6" s="1">
         <v>0</v>
       </c>
-      <c r="J6" s="80" t="s">
+      <c r="J6" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="81"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="77"/>
+      <c r="R6" s="77"/>
+      <c r="S6" s="77"/>
+      <c r="T6" s="77"/>
+      <c r="U6" s="77"/>
+      <c r="V6" s="77"/>
+      <c r="W6" s="77"/>
       <c r="X6" s="38"/>
-      <c r="Y6" s="101"/>
-      <c r="Z6" s="82"/>
-      <c r="AA6" s="82"/>
-      <c r="AB6" s="114"/>
+      <c r="Y6" s="75"/>
+      <c r="Z6" s="73"/>
+      <c r="AA6" s="73"/>
+      <c r="AB6" s="76"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
@@ -2222,10 +2231,10 @@
         <v>67</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>82</v>
@@ -2252,21 +2261,21 @@
       <c r="N7" s="32">
         <v>0</v>
       </c>
-      <c r="O7" s="83" t="s">
+      <c r="O7" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="P7" s="84"/>
-      <c r="Q7" s="93"/>
-      <c r="R7" s="107" t="s">
+      <c r="P7" s="82"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="S7" s="79"/>
+      <c r="T7" s="80"/>
+      <c r="U7" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="S7" s="108"/>
-      <c r="T7" s="109"/>
-      <c r="U7" s="85" t="s">
-        <v>101</v>
-      </c>
-      <c r="V7" s="86"/>
-      <c r="W7" s="86"/>
+      <c r="V7" s="87"/>
+      <c r="W7" s="87"/>
       <c r="X7" s="39"/>
       <c r="Y7" s="35" t="b">
         <v>1</v>
@@ -2290,10 +2299,10 @@
         <v>68</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>82</v>
@@ -2320,21 +2329,21 @@
       <c r="N8" s="12">
         <v>1</v>
       </c>
-      <c r="O8" s="83" t="s">
+      <c r="O8" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="P8" s="84"/>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="107" t="s">
+      <c r="P8" s="82"/>
+      <c r="Q8" s="83"/>
+      <c r="R8" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="S8" s="79"/>
+      <c r="T8" s="80"/>
+      <c r="U8" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="S8" s="108"/>
-      <c r="T8" s="109"/>
-      <c r="U8" s="85" t="s">
-        <v>101</v>
-      </c>
-      <c r="V8" s="86"/>
-      <c r="W8" s="86"/>
+      <c r="V8" s="87"/>
+      <c r="W8" s="87"/>
       <c r="X8" s="39"/>
       <c r="Y8" s="36" t="b">
         <v>1</v>
@@ -2358,13 +2367,13 @@
         <v>67</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G9" s="39"/>
       <c r="H9" s="14">
@@ -2388,21 +2397,21 @@
       <c r="N9" s="32">
         <v>0</v>
       </c>
-      <c r="O9" s="73" t="s">
-        <v>107</v>
-      </c>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="110"/>
-      <c r="R9" s="107" t="s">
+      <c r="O9" s="88" t="s">
+        <v>105</v>
+      </c>
+      <c r="P9" s="89"/>
+      <c r="Q9" s="90"/>
+      <c r="R9" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="S9" s="79"/>
+      <c r="T9" s="80"/>
+      <c r="U9" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="S9" s="108"/>
-      <c r="T9" s="109"/>
-      <c r="U9" s="85" t="s">
-        <v>101</v>
-      </c>
-      <c r="V9" s="86"/>
-      <c r="W9" s="86"/>
+      <c r="V9" s="87"/>
+      <c r="W9" s="87"/>
       <c r="X9" s="39"/>
       <c r="Y9" s="35" t="b">
         <v>1</v>
@@ -2426,13 +2435,13 @@
         <v>68</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G10" s="39"/>
       <c r="H10" s="14">
@@ -2456,21 +2465,21 @@
       <c r="N10" s="12">
         <v>1</v>
       </c>
-      <c r="O10" s="73" t="s">
-        <v>107</v>
-      </c>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="110"/>
-      <c r="R10" s="107" t="s">
+      <c r="O10" s="88" t="s">
+        <v>105</v>
+      </c>
+      <c r="P10" s="89"/>
+      <c r="Q10" s="90"/>
+      <c r="R10" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="S10" s="79"/>
+      <c r="T10" s="80"/>
+      <c r="U10" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="S10" s="108"/>
-      <c r="T10" s="109"/>
-      <c r="U10" s="85" t="s">
-        <v>101</v>
-      </c>
-      <c r="V10" s="86"/>
-      <c r="W10" s="86"/>
+      <c r="V10" s="87"/>
+      <c r="W10" s="87"/>
       <c r="X10" s="39"/>
       <c r="Y10" s="36" t="b">
         <v>1</v>
@@ -2494,12 +2503,12 @@
         <v>69</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="F11" s="74"/>
+        <v>96</v>
+      </c>
+      <c r="E11" s="88" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="89"/>
       <c r="G11" s="39"/>
       <c r="H11" s="13">
         <v>0</v>
@@ -2516,21 +2525,21 @@
       <c r="L11" s="32">
         <v>0</v>
       </c>
-      <c r="M11" s="85" t="s">
-        <v>101</v>
-      </c>
-      <c r="N11" s="86"/>
-      <c r="O11" s="87"/>
-      <c r="P11" s="73" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="74"/>
-      <c r="T11" s="74"/>
-      <c r="U11" s="74"/>
-      <c r="V11" s="74"/>
-      <c r="W11" s="74"/>
+      <c r="M11" s="86" t="s">
+        <v>99</v>
+      </c>
+      <c r="N11" s="87"/>
+      <c r="O11" s="94"/>
+      <c r="P11" s="88" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q11" s="89"/>
+      <c r="R11" s="89"/>
+      <c r="S11" s="89"/>
+      <c r="T11" s="89"/>
+      <c r="U11" s="89"/>
+      <c r="V11" s="89"/>
+      <c r="W11" s="89"/>
       <c r="X11" s="39"/>
       <c r="Y11" s="35" t="b">
         <v>0</v>
@@ -2547,19 +2556,19 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B12" s="39"/>
       <c r="C12" s="43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="74"/>
+        <v>96</v>
+      </c>
+      <c r="E12" s="88" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="89"/>
       <c r="G12" s="39"/>
       <c r="H12" s="13">
         <v>0</v>
@@ -2576,21 +2585,21 @@
       <c r="L12" s="12">
         <v>1</v>
       </c>
-      <c r="M12" s="85" t="s">
-        <v>101</v>
-      </c>
-      <c r="N12" s="86"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="73" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="74"/>
-      <c r="T12" s="74"/>
-      <c r="U12" s="74"/>
-      <c r="V12" s="74"/>
-      <c r="W12" s="74"/>
+      <c r="M12" s="86" t="s">
+        <v>99</v>
+      </c>
+      <c r="N12" s="87"/>
+      <c r="O12" s="94"/>
+      <c r="P12" s="88" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="89"/>
+      <c r="T12" s="89"/>
+      <c r="U12" s="89"/>
+      <c r="V12" s="89"/>
+      <c r="W12" s="89"/>
       <c r="X12" s="39"/>
       <c r="Y12" s="36" t="b">
         <v>0</v>
@@ -2607,19 +2616,19 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="51" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B13" s="46"/>
       <c r="C13" s="44" t="s">
         <v>67</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" s="74"/>
+        <v>96</v>
+      </c>
+      <c r="E13" s="88" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="89"/>
       <c r="G13" s="39"/>
       <c r="H13" s="13">
         <v>0</v>
@@ -2636,21 +2645,21 @@
       <c r="L13" s="32">
         <v>0</v>
       </c>
-      <c r="M13" s="85" t="s">
+      <c r="M13" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="N13" s="86"/>
-      <c r="O13" s="87"/>
-      <c r="P13" s="73" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="74"/>
-      <c r="S13" s="74"/>
-      <c r="T13" s="74"/>
-      <c r="U13" s="74"/>
-      <c r="V13" s="74"/>
-      <c r="W13" s="74"/>
+      <c r="N13" s="87"/>
+      <c r="O13" s="94"/>
+      <c r="P13" s="88" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q13" s="89"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="89"/>
+      <c r="T13" s="89"/>
+      <c r="U13" s="89"/>
+      <c r="V13" s="89"/>
+      <c r="W13" s="89"/>
       <c r="X13" s="39"/>
       <c r="Y13" s="35" t="b">
         <v>1</v>
@@ -2667,19 +2676,19 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="53" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="43" t="s">
         <v>68</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E14" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="74"/>
+        <v>96</v>
+      </c>
+      <c r="E14" s="88" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="89"/>
       <c r="G14" s="39"/>
       <c r="H14" s="13">
         <v>0</v>
@@ -2696,21 +2705,21 @@
       <c r="L14" s="12">
         <v>1</v>
       </c>
-      <c r="M14" s="85" t="s">
+      <c r="M14" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="N14" s="86"/>
-      <c r="O14" s="87"/>
-      <c r="P14" s="73" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="74"/>
-      <c r="S14" s="74"/>
-      <c r="T14" s="74"/>
-      <c r="U14" s="74"/>
-      <c r="V14" s="74"/>
-      <c r="W14" s="74"/>
+      <c r="N14" s="87"/>
+      <c r="O14" s="94"/>
+      <c r="P14" s="88" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q14" s="89"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="89"/>
+      <c r="T14" s="89"/>
+      <c r="U14" s="89"/>
+      <c r="V14" s="89"/>
+      <c r="W14" s="89"/>
       <c r="X14" s="39"/>
       <c r="Y14" s="36" t="b">
         <v>1</v>
@@ -2731,9 +2740,9 @@
       </c>
       <c r="B15" s="45"/>
       <c r="C15" s="34"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
       <c r="G15" s="38"/>
       <c r="H15" s="3">
         <v>0</v>
@@ -2753,18 +2762,18 @@
       <c r="M15" s="1">
         <v>0</v>
       </c>
-      <c r="N15" s="80" t="s">
+      <c r="N15" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="82"/>
-      <c r="S15" s="82"/>
-      <c r="T15" s="82"/>
-      <c r="U15" s="82"/>
-      <c r="V15" s="82"/>
-      <c r="W15" s="82"/>
+      <c r="O15" s="77"/>
+      <c r="P15" s="77"/>
+      <c r="Q15" s="77"/>
+      <c r="R15" s="73"/>
+      <c r="S15" s="73"/>
+      <c r="T15" s="73"/>
+      <c r="U15" s="73"/>
+      <c r="V15" s="73"/>
+      <c r="W15" s="73"/>
       <c r="X15" s="38"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="1"/>
@@ -2782,10 +2791,10 @@
       <c r="D16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="83" t="s">
+      <c r="E16" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="84"/>
+      <c r="F16" s="82"/>
       <c r="G16" s="39"/>
       <c r="H16" s="13">
         <v>0</v>
@@ -2817,16 +2826,16 @@
       <c r="Q16" s="12">
         <v>0</v>
       </c>
-      <c r="R16" s="83" t="s">
+      <c r="R16" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S16" s="84"/>
-      <c r="T16" s="93"/>
-      <c r="U16" s="94" t="s">
+      <c r="S16" s="82"/>
+      <c r="T16" s="83"/>
+      <c r="U16" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="V16" s="95"/>
-      <c r="W16" s="95"/>
+      <c r="V16" s="85"/>
+      <c r="W16" s="85"/>
       <c r="X16" s="39"/>
       <c r="Y16" s="36" t="b">
         <v>1</v>
@@ -2852,10 +2861,10 @@
       <c r="D17" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="83" t="s">
+      <c r="E17" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="84"/>
+      <c r="F17" s="82"/>
       <c r="G17" s="39"/>
       <c r="H17" s="41">
         <v>0</v>
@@ -2887,16 +2896,16 @@
       <c r="Q17" s="32">
         <v>1</v>
       </c>
-      <c r="R17" s="83" t="s">
+      <c r="R17" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S17" s="84"/>
-      <c r="T17" s="93"/>
-      <c r="U17" s="94" t="s">
+      <c r="S17" s="82"/>
+      <c r="T17" s="83"/>
+      <c r="U17" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="V17" s="95"/>
-      <c r="W17" s="95"/>
+      <c r="V17" s="85"/>
+      <c r="W17" s="85"/>
       <c r="X17" s="39"/>
       <c r="Y17" s="35" t="b">
         <v>1</v>
@@ -2922,10 +2931,10 @@
       <c r="D18" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="83" t="s">
+      <c r="E18" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="84"/>
+      <c r="F18" s="82"/>
       <c r="G18" s="39"/>
       <c r="H18" s="13">
         <v>0</v>
@@ -2957,16 +2966,16 @@
       <c r="Q18" s="12">
         <v>0</v>
       </c>
-      <c r="R18" s="83" t="s">
+      <c r="R18" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S18" s="84"/>
-      <c r="T18" s="93"/>
-      <c r="U18" s="94" t="s">
+      <c r="S18" s="82"/>
+      <c r="T18" s="83"/>
+      <c r="U18" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="V18" s="95"/>
-      <c r="W18" s="95"/>
+      <c r="V18" s="85"/>
+      <c r="W18" s="85"/>
       <c r="X18" s="39"/>
       <c r="Y18" s="36" t="b">
         <v>1</v>
@@ -2992,10 +3001,10 @@
       <c r="D19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="83" t="s">
+      <c r="E19" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="84"/>
+      <c r="F19" s="82"/>
       <c r="G19" s="39"/>
       <c r="H19" s="41">
         <v>0</v>
@@ -3027,16 +3036,16 @@
       <c r="Q19" s="32">
         <v>1</v>
       </c>
-      <c r="R19" s="83" t="s">
+      <c r="R19" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S19" s="84"/>
-      <c r="T19" s="93"/>
-      <c r="U19" s="94" t="s">
+      <c r="S19" s="82"/>
+      <c r="T19" s="83"/>
+      <c r="U19" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="V19" s="95"/>
-      <c r="W19" s="95"/>
+      <c r="V19" s="85"/>
+      <c r="W19" s="85"/>
       <c r="X19" s="39"/>
       <c r="Y19" s="35" t="b">
         <v>1</v>
@@ -3062,10 +3071,10 @@
       <c r="D20" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="83" t="s">
+      <c r="E20" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="84"/>
+      <c r="F20" s="82"/>
       <c r="G20" s="39"/>
       <c r="H20" s="13">
         <v>0</v>
@@ -3097,16 +3106,16 @@
       <c r="Q20" s="12">
         <v>0</v>
       </c>
-      <c r="R20" s="83" t="s">
+      <c r="R20" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S20" s="84"/>
-      <c r="T20" s="93"/>
-      <c r="U20" s="94" t="s">
+      <c r="S20" s="82"/>
+      <c r="T20" s="83"/>
+      <c r="U20" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="V20" s="95"/>
-      <c r="W20" s="95"/>
+      <c r="V20" s="85"/>
+      <c r="W20" s="85"/>
       <c r="X20" s="39"/>
       <c r="Y20" s="36" t="b">
         <v>1</v>
@@ -3132,10 +3141,10 @@
       <c r="D21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="83" t="s">
+      <c r="E21" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="84"/>
+      <c r="F21" s="82"/>
       <c r="G21" s="39"/>
       <c r="H21" s="41">
         <v>0</v>
@@ -3167,16 +3176,16 @@
       <c r="Q21" s="32">
         <v>1</v>
       </c>
-      <c r="R21" s="83" t="s">
+      <c r="R21" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S21" s="84"/>
-      <c r="T21" s="93"/>
-      <c r="U21" s="94" t="s">
+      <c r="S21" s="82"/>
+      <c r="T21" s="83"/>
+      <c r="U21" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="V21" s="95"/>
-      <c r="W21" s="95"/>
+      <c r="V21" s="85"/>
+      <c r="W21" s="85"/>
       <c r="X21" s="39"/>
       <c r="Y21" s="35" t="b">
         <v>1</v>
@@ -3202,10 +3211,10 @@
       <c r="D22" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="83" t="s">
+      <c r="E22" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="84"/>
+      <c r="F22" s="82"/>
       <c r="G22" s="39"/>
       <c r="H22" s="13">
         <v>0</v>
@@ -3237,16 +3246,16 @@
       <c r="Q22" s="12">
         <v>0</v>
       </c>
-      <c r="R22" s="83" t="s">
+      <c r="R22" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S22" s="84"/>
-      <c r="T22" s="93"/>
-      <c r="U22" s="94" t="s">
+      <c r="S22" s="82"/>
+      <c r="T22" s="83"/>
+      <c r="U22" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="V22" s="95"/>
-      <c r="W22" s="95"/>
+      <c r="V22" s="85"/>
+      <c r="W22" s="85"/>
       <c r="X22" s="39"/>
       <c r="Y22" s="36" t="b">
         <v>1</v>
@@ -3272,10 +3281,10 @@
       <c r="D23" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="83" t="s">
+      <c r="E23" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="84"/>
+      <c r="F23" s="82"/>
       <c r="G23" s="39"/>
       <c r="H23" s="41">
         <v>0</v>
@@ -3307,16 +3316,16 @@
       <c r="Q23" s="32">
         <v>1</v>
       </c>
-      <c r="R23" s="83" t="s">
+      <c r="R23" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S23" s="84"/>
-      <c r="T23" s="93"/>
-      <c r="U23" s="94" t="s">
+      <c r="S23" s="82"/>
+      <c r="T23" s="83"/>
+      <c r="U23" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="V23" s="95"/>
-      <c r="W23" s="95"/>
+      <c r="V23" s="85"/>
+      <c r="W23" s="85"/>
       <c r="X23" s="39"/>
       <c r="Y23" s="35" t="b">
         <v>1</v>
@@ -3340,12 +3349,12 @@
         <v>72</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" s="83" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="84"/>
+      <c r="F24" s="82"/>
       <c r="G24" s="39"/>
       <c r="H24" s="13">
         <v>0</v>
@@ -3377,16 +3386,16 @@
       <c r="Q24" s="12">
         <v>0</v>
       </c>
-      <c r="R24" s="83" t="s">
+      <c r="R24" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S24" s="84"/>
-      <c r="T24" s="93"/>
-      <c r="U24" s="94" t="s">
-        <v>99</v>
-      </c>
-      <c r="V24" s="95"/>
-      <c r="W24" s="95"/>
+      <c r="S24" s="82"/>
+      <c r="T24" s="83"/>
+      <c r="U24" s="84" t="s">
+        <v>97</v>
+      </c>
+      <c r="V24" s="85"/>
+      <c r="W24" s="85"/>
       <c r="X24" s="39"/>
       <c r="Y24" s="36" t="b">
         <v>1</v>
@@ -3410,13 +3419,13 @@
         <v>77</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="F25" s="40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G25" s="39"/>
       <c r="H25" s="41">
@@ -3449,16 +3458,16 @@
       <c r="Q25" s="32">
         <v>1</v>
       </c>
-      <c r="R25" s="83" t="s">
-        <v>85</v>
-      </c>
-      <c r="S25" s="84"/>
-      <c r="T25" s="93"/>
-      <c r="U25" s="94" t="s">
-        <v>84</v>
-      </c>
-      <c r="V25" s="95"/>
-      <c r="W25" s="95"/>
+      <c r="R25" s="81" t="s">
+        <v>97</v>
+      </c>
+      <c r="S25" s="82"/>
+      <c r="T25" s="83"/>
+      <c r="U25" s="84" t="s">
+        <v>98</v>
+      </c>
+      <c r="V25" s="85"/>
+      <c r="W25" s="85"/>
       <c r="X25" s="39"/>
       <c r="Y25" s="35" t="b">
         <v>1</v>
@@ -3484,10 +3493,10 @@
       <c r="D26" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="83" t="s">
+      <c r="E26" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="84"/>
+      <c r="F26" s="82"/>
       <c r="G26" s="39"/>
       <c r="H26" s="13">
         <v>0</v>
@@ -3519,16 +3528,16 @@
       <c r="Q26" s="12">
         <v>0</v>
       </c>
-      <c r="R26" s="83" t="s">
+      <c r="R26" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S26" s="84"/>
-      <c r="T26" s="93"/>
-      <c r="U26" s="94" t="s">
-        <v>99</v>
-      </c>
-      <c r="V26" s="95"/>
-      <c r="W26" s="95"/>
+      <c r="S26" s="82"/>
+      <c r="T26" s="83"/>
+      <c r="U26" s="84" t="s">
+        <v>97</v>
+      </c>
+      <c r="V26" s="85"/>
+      <c r="W26" s="85"/>
       <c r="X26" s="39"/>
       <c r="Y26" s="36" t="b">
         <v>1</v>
@@ -3554,10 +3563,10 @@
       <c r="D27" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="83" t="s">
+      <c r="E27" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="84"/>
+      <c r="F27" s="82"/>
       <c r="G27" s="39"/>
       <c r="H27" s="41">
         <v>0</v>
@@ -3589,16 +3598,16 @@
       <c r="Q27" s="32">
         <v>1</v>
       </c>
-      <c r="R27" s="83" t="s">
+      <c r="R27" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S27" s="84"/>
-      <c r="T27" s="93"/>
-      <c r="U27" s="94" t="s">
-        <v>99</v>
-      </c>
-      <c r="V27" s="95"/>
-      <c r="W27" s="95"/>
+      <c r="S27" s="82"/>
+      <c r="T27" s="83"/>
+      <c r="U27" s="84" t="s">
+        <v>97</v>
+      </c>
+      <c r="V27" s="85"/>
+      <c r="W27" s="85"/>
       <c r="X27" s="39"/>
       <c r="Y27" s="35" t="b">
         <v>1</v>
@@ -3624,10 +3633,10 @@
       <c r="D28" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="83" t="s">
+      <c r="E28" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="84"/>
+      <c r="F28" s="82"/>
       <c r="G28" s="39"/>
       <c r="H28" s="13">
         <v>0</v>
@@ -3659,16 +3668,16 @@
       <c r="Q28" s="12">
         <v>0</v>
       </c>
-      <c r="R28" s="83" t="s">
+      <c r="R28" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S28" s="84"/>
-      <c r="T28" s="93"/>
-      <c r="U28" s="94" t="s">
+      <c r="S28" s="82"/>
+      <c r="T28" s="83"/>
+      <c r="U28" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="V28" s="95"/>
-      <c r="W28" s="95"/>
+      <c r="V28" s="85"/>
+      <c r="W28" s="85"/>
       <c r="X28" s="39"/>
       <c r="Y28" s="36" t="b">
         <v>1</v>
@@ -3692,13 +3701,13 @@
         <v>75</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>82</v>
       </c>
       <c r="F29" s="40" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G29" s="39"/>
       <c r="H29" s="41">
@@ -3731,16 +3740,16 @@
       <c r="Q29" s="32">
         <v>1</v>
       </c>
-      <c r="R29" s="83" t="s">
-        <v>99</v>
-      </c>
-      <c r="S29" s="84"/>
-      <c r="T29" s="93"/>
-      <c r="U29" s="96" t="s">
-        <v>127</v>
-      </c>
-      <c r="V29" s="97"/>
-      <c r="W29" s="97"/>
+      <c r="R29" s="81" t="s">
+        <v>97</v>
+      </c>
+      <c r="S29" s="82"/>
+      <c r="T29" s="83"/>
+      <c r="U29" s="101" t="s">
+        <v>125</v>
+      </c>
+      <c r="V29" s="102"/>
+      <c r="W29" s="102"/>
       <c r="X29" s="39"/>
       <c r="Y29" s="35" t="b">
         <v>0</v>
@@ -3766,10 +3775,10 @@
       <c r="D30" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="83" t="s">
+      <c r="E30" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="84"/>
+      <c r="F30" s="82"/>
       <c r="G30" s="39"/>
       <c r="H30" s="13">
         <v>0</v>
@@ -3801,16 +3810,16 @@
       <c r="Q30" s="12">
         <v>0</v>
       </c>
-      <c r="R30" s="83" t="s">
+      <c r="R30" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S30" s="84"/>
-      <c r="T30" s="93"/>
-      <c r="U30" s="94" t="s">
+      <c r="S30" s="82"/>
+      <c r="T30" s="83"/>
+      <c r="U30" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="V30" s="95"/>
-      <c r="W30" s="95"/>
+      <c r="V30" s="85"/>
+      <c r="W30" s="85"/>
       <c r="X30" s="39"/>
       <c r="Y30" s="36" t="b">
         <v>1</v>
@@ -3834,12 +3843,12 @@
         <v>73</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="83" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="84"/>
+      <c r="F31" s="82"/>
       <c r="G31" s="39"/>
       <c r="H31" s="41">
         <v>0</v>
@@ -3871,16 +3880,16 @@
       <c r="Q31" s="32">
         <v>1</v>
       </c>
-      <c r="R31" s="83" t="s">
+      <c r="R31" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="S31" s="84"/>
-      <c r="T31" s="93"/>
-      <c r="U31" s="94" t="s">
-        <v>100</v>
-      </c>
-      <c r="V31" s="95"/>
-      <c r="W31" s="95"/>
+      <c r="S31" s="82"/>
+      <c r="T31" s="83"/>
+      <c r="U31" s="84" t="s">
+        <v>98</v>
+      </c>
+      <c r="V31" s="85"/>
+      <c r="W31" s="85"/>
       <c r="X31" s="39"/>
       <c r="Y31" s="35" t="b">
         <v>1</v>
@@ -3901,9 +3910,9 @@
       </c>
       <c r="B32" s="45"/>
       <c r="C32" s="34"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
       <c r="G32" s="38"/>
       <c r="H32" s="15">
         <v>1</v>
@@ -3917,20 +3926,20 @@
       <c r="K32" s="4">
         <v>1</v>
       </c>
-      <c r="L32" s="80" t="s">
+      <c r="L32" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="M32" s="81"/>
-      <c r="N32" s="81"/>
-      <c r="O32" s="82"/>
-      <c r="P32" s="82"/>
-      <c r="Q32" s="82"/>
-      <c r="R32" s="82"/>
-      <c r="S32" s="82"/>
-      <c r="T32" s="82"/>
-      <c r="U32" s="82"/>
-      <c r="V32" s="82"/>
-      <c r="W32" s="82"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
+      <c r="O32" s="73"/>
+      <c r="P32" s="73"/>
+      <c r="Q32" s="73"/>
+      <c r="R32" s="73"/>
+      <c r="S32" s="73"/>
+      <c r="T32" s="73"/>
+      <c r="U32" s="73"/>
+      <c r="V32" s="73"/>
+      <c r="W32" s="73"/>
       <c r="X32" s="38"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="1"/>
@@ -3946,12 +3955,12 @@
         <v>19</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="E33" s="73" t="s">
-        <v>117</v>
-      </c>
-      <c r="F33" s="74"/>
+        <v>118</v>
+      </c>
+      <c r="E33" s="88" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="89"/>
       <c r="G33" s="39"/>
       <c r="H33" s="16">
         <v>1</v>
@@ -3968,21 +3977,21 @@
       <c r="L33" s="26">
         <v>0</v>
       </c>
-      <c r="M33" s="98" t="s">
-        <v>104</v>
-      </c>
-      <c r="N33" s="99"/>
-      <c r="O33" s="100"/>
-      <c r="P33" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="74"/>
-      <c r="S33" s="74"/>
-      <c r="T33" s="74"/>
-      <c r="U33" s="74"/>
-      <c r="V33" s="74"/>
-      <c r="W33" s="74"/>
+      <c r="M33" s="95" t="s">
+        <v>102</v>
+      </c>
+      <c r="N33" s="96"/>
+      <c r="O33" s="97"/>
+      <c r="P33" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q33" s="89"/>
+      <c r="R33" s="89"/>
+      <c r="S33" s="89"/>
+      <c r="T33" s="89"/>
+      <c r="U33" s="89"/>
+      <c r="V33" s="89"/>
+      <c r="W33" s="89"/>
       <c r="X33" s="39"/>
       <c r="Y33" s="35" t="b">
         <v>0</v>
@@ -4006,12 +4015,12 @@
         <v>21</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="E34" s="73" t="s">
-        <v>117</v>
-      </c>
-      <c r="F34" s="74"/>
+        <v>118</v>
+      </c>
+      <c r="E34" s="88" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="89"/>
       <c r="G34" s="39"/>
       <c r="H34" s="16">
         <v>1</v>
@@ -4028,21 +4037,21 @@
       <c r="L34" s="5">
         <v>1</v>
       </c>
-      <c r="M34" s="98" t="s">
-        <v>104</v>
-      </c>
-      <c r="N34" s="99"/>
-      <c r="O34" s="100"/>
-      <c r="P34" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q34" s="74"/>
-      <c r="R34" s="74"/>
-      <c r="S34" s="74"/>
-      <c r="T34" s="74"/>
-      <c r="U34" s="74"/>
-      <c r="V34" s="74"/>
-      <c r="W34" s="74"/>
+      <c r="M34" s="95" t="s">
+        <v>102</v>
+      </c>
+      <c r="N34" s="96"/>
+      <c r="O34" s="97"/>
+      <c r="P34" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q34" s="89"/>
+      <c r="R34" s="89"/>
+      <c r="S34" s="89"/>
+      <c r="T34" s="89"/>
+      <c r="U34" s="89"/>
+      <c r="V34" s="89"/>
+      <c r="W34" s="89"/>
       <c r="X34" s="39"/>
       <c r="Y34" s="36" t="b">
         <v>0</v>
@@ -4064,8 +4073,8 @@
       <c r="B35" s="45"/>
       <c r="C35" s="34"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="80"/>
-      <c r="F35" s="81"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="77"/>
       <c r="G35" s="38"/>
       <c r="H35" s="15">
         <v>1</v>
@@ -4079,20 +4088,20 @@
       <c r="K35" s="4">
         <v>1</v>
       </c>
-      <c r="L35" s="80" t="s">
+      <c r="L35" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="M35" s="81"/>
-      <c r="N35" s="81"/>
-      <c r="O35" s="81"/>
-      <c r="P35" s="81"/>
-      <c r="Q35" s="81"/>
-      <c r="R35" s="101"/>
-      <c r="S35" s="82"/>
-      <c r="T35" s="82"/>
-      <c r="U35" s="82"/>
-      <c r="V35" s="82"/>
-      <c r="W35" s="82"/>
+      <c r="M35" s="77"/>
+      <c r="N35" s="77"/>
+      <c r="O35" s="77"/>
+      <c r="P35" s="77"/>
+      <c r="Q35" s="77"/>
+      <c r="R35" s="75"/>
+      <c r="S35" s="73"/>
+      <c r="T35" s="73"/>
+      <c r="U35" s="73"/>
+      <c r="V35" s="73"/>
+      <c r="W35" s="73"/>
       <c r="X35" s="38"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="1"/>
@@ -4108,12 +4117,12 @@
         <v>50</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E36" s="88" t="s">
-        <v>118</v>
-      </c>
-      <c r="F36" s="89"/>
+        <v>117</v>
+      </c>
+      <c r="E36" s="103" t="s">
+        <v>116</v>
+      </c>
+      <c r="F36" s="104"/>
       <c r="G36" s="39"/>
       <c r="H36" s="16">
         <v>1</v>
@@ -4142,15 +4151,15 @@
       <c r="P36" s="5">
         <v>0</v>
       </c>
-      <c r="Q36" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="R36" s="74"/>
-      <c r="S36" s="74"/>
-      <c r="T36" s="74"/>
-      <c r="U36" s="74"/>
-      <c r="V36" s="74"/>
-      <c r="W36" s="74"/>
+      <c r="Q36" s="88" t="s">
+        <v>106</v>
+      </c>
+      <c r="R36" s="89"/>
+      <c r="S36" s="89"/>
+      <c r="T36" s="89"/>
+      <c r="U36" s="89"/>
+      <c r="V36" s="89"/>
+      <c r="W36" s="89"/>
       <c r="X36" s="39"/>
       <c r="Y36" s="36" t="b">
         <v>0</v>
@@ -4174,12 +4183,12 @@
         <v>49</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" s="88" t="s">
-        <v>118</v>
-      </c>
-      <c r="F37" s="89"/>
+        <v>117</v>
+      </c>
+      <c r="E37" s="103" t="s">
+        <v>116</v>
+      </c>
+      <c r="F37" s="104"/>
       <c r="G37" s="39"/>
       <c r="H37" s="16">
         <v>1</v>
@@ -4208,15 +4217,15 @@
       <c r="P37" s="26">
         <v>1</v>
       </c>
-      <c r="Q37" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="R37" s="74"/>
-      <c r="S37" s="74"/>
-      <c r="T37" s="74"/>
-      <c r="U37" s="74"/>
-      <c r="V37" s="74"/>
-      <c r="W37" s="74"/>
+      <c r="Q37" s="88" t="s">
+        <v>106</v>
+      </c>
+      <c r="R37" s="89"/>
+      <c r="S37" s="89"/>
+      <c r="T37" s="89"/>
+      <c r="U37" s="89"/>
+      <c r="V37" s="89"/>
+      <c r="W37" s="89"/>
       <c r="X37" s="39"/>
       <c r="Y37" s="35" t="b">
         <v>0</v>
@@ -4233,13 +4242,13 @@
     </row>
     <row r="38" spans="1:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B38" s="45"/>
       <c r="C38" s="34"/>
-      <c r="D38" s="80"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
       <c r="G38" s="38"/>
       <c r="H38" s="42">
         <v>1</v>
@@ -4253,20 +4262,20 @@
       <c r="K38" s="21">
         <v>1</v>
       </c>
-      <c r="L38" s="82" t="s">
-        <v>111</v>
-      </c>
-      <c r="M38" s="82"/>
-      <c r="N38" s="82"/>
-      <c r="O38" s="82"/>
-      <c r="P38" s="66"/>
-      <c r="Q38" s="66"/>
-      <c r="R38" s="66"/>
-      <c r="S38" s="66"/>
-      <c r="T38" s="66"/>
-      <c r="U38" s="66"/>
-      <c r="V38" s="66"/>
-      <c r="W38" s="66"/>
+      <c r="L38" s="73" t="s">
+        <v>109</v>
+      </c>
+      <c r="M38" s="73"/>
+      <c r="N38" s="73"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="65"/>
+      <c r="Q38" s="65"/>
+      <c r="R38" s="65"/>
+      <c r="S38" s="65"/>
+      <c r="T38" s="65"/>
+      <c r="U38" s="65"/>
+      <c r="V38" s="65"/>
+      <c r="W38" s="65"/>
       <c r="X38" s="38"/>
       <c r="Y38" s="3"/>
       <c r="Z38" s="1"/>
@@ -4282,12 +4291,12 @@
         <v>23</v>
       </c>
       <c r="D39" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E39" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F39" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E39" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F39" s="69"/>
       <c r="G39" s="39"/>
       <c r="H39" s="16">
         <v>1</v>
@@ -4301,29 +4310,29 @@
       <c r="K39" s="10">
         <v>1</v>
       </c>
-      <c r="L39" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M39" s="91"/>
-      <c r="N39" s="91"/>
-      <c r="O39" s="92"/>
-      <c r="P39" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q39" s="74"/>
-      <c r="R39" s="74"/>
-      <c r="S39" s="74"/>
-      <c r="T39" s="74"/>
-      <c r="U39" s="74"/>
-      <c r="V39" s="74"/>
-      <c r="W39" s="74"/>
+      <c r="L39" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M39" s="99"/>
+      <c r="N39" s="99"/>
+      <c r="O39" s="100"/>
+      <c r="P39" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q39" s="89"/>
+      <c r="R39" s="89"/>
+      <c r="S39" s="89"/>
+      <c r="T39" s="89"/>
+      <c r="U39" s="89"/>
+      <c r="V39" s="89"/>
+      <c r="W39" s="89"/>
       <c r="X39" s="39"/>
-      <c r="Y39" s="67" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z39" s="68"/>
-      <c r="AA39" s="68"/>
-      <c r="AB39" s="69"/>
+      <c r="Y39" s="105" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z39" s="106"/>
+      <c r="AA39" s="106"/>
+      <c r="AB39" s="107"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" s="51" t="s">
@@ -4334,12 +4343,12 @@
         <v>25</v>
       </c>
       <c r="D40" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E40" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F40" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E40" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F40" s="69"/>
       <c r="G40" s="39"/>
       <c r="H40" s="16">
         <v>1</v>
@@ -4353,29 +4362,29 @@
       <c r="K40" s="10">
         <v>1</v>
       </c>
-      <c r="L40" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M40" s="91"/>
-      <c r="N40" s="91"/>
-      <c r="O40" s="92"/>
-      <c r="P40" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q40" s="74"/>
-      <c r="R40" s="74"/>
-      <c r="S40" s="74"/>
-      <c r="T40" s="74"/>
-      <c r="U40" s="74"/>
-      <c r="V40" s="74"/>
-      <c r="W40" s="74"/>
+      <c r="L40" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M40" s="99"/>
+      <c r="N40" s="99"/>
+      <c r="O40" s="100"/>
+      <c r="P40" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q40" s="89"/>
+      <c r="R40" s="89"/>
+      <c r="S40" s="89"/>
+      <c r="T40" s="89"/>
+      <c r="U40" s="89"/>
+      <c r="V40" s="89"/>
+      <c r="W40" s="89"/>
       <c r="X40" s="39"/>
-      <c r="Y40" s="70" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z40" s="71"/>
-      <c r="AA40" s="71"/>
-      <c r="AB40" s="72"/>
+      <c r="Y40" s="108" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z40" s="109"/>
+      <c r="AA40" s="109"/>
+      <c r="AB40" s="110"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" s="53" t="s">
@@ -4383,15 +4392,15 @@
       </c>
       <c r="B41" s="39"/>
       <c r="C41" s="43" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="D41" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E41" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F41" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E41" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F41" s="69"/>
       <c r="G41" s="39"/>
       <c r="H41" s="16">
         <v>1</v>
@@ -4405,29 +4414,29 @@
       <c r="K41" s="10">
         <v>1</v>
       </c>
-      <c r="L41" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M41" s="91"/>
-      <c r="N41" s="91"/>
-      <c r="O41" s="92"/>
-      <c r="P41" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q41" s="74"/>
-      <c r="R41" s="74"/>
-      <c r="S41" s="74"/>
-      <c r="T41" s="74"/>
-      <c r="U41" s="74"/>
-      <c r="V41" s="74"/>
-      <c r="W41" s="74"/>
+      <c r="L41" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M41" s="99"/>
+      <c r="N41" s="99"/>
+      <c r="O41" s="100"/>
+      <c r="P41" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q41" s="89"/>
+      <c r="R41" s="89"/>
+      <c r="S41" s="89"/>
+      <c r="T41" s="89"/>
+      <c r="U41" s="89"/>
+      <c r="V41" s="89"/>
+      <c r="W41" s="89"/>
       <c r="X41" s="39"/>
-      <c r="Y41" s="67" t="s">
-        <v>131</v>
-      </c>
-      <c r="Z41" s="68"/>
-      <c r="AA41" s="68"/>
-      <c r="AB41" s="69"/>
+      <c r="Y41" s="105" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z41" s="106"/>
+      <c r="AA41" s="106"/>
+      <c r="AB41" s="107"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="51" t="s">
@@ -4435,15 +4444,15 @@
       </c>
       <c r="B42" s="46"/>
       <c r="C42" s="44" t="s">
-        <v>87</v>
+        <v>143</v>
       </c>
       <c r="D42" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E42" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F42" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E42" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F42" s="69"/>
       <c r="G42" s="39"/>
       <c r="H42" s="16">
         <v>1</v>
@@ -4457,29 +4466,29 @@
       <c r="K42" s="10">
         <v>1</v>
       </c>
-      <c r="L42" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M42" s="91"/>
-      <c r="N42" s="91"/>
-      <c r="O42" s="92"/>
-      <c r="P42" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q42" s="74"/>
-      <c r="R42" s="74"/>
-      <c r="S42" s="74"/>
-      <c r="T42" s="74"/>
-      <c r="U42" s="74"/>
-      <c r="V42" s="74"/>
-      <c r="W42" s="74"/>
+      <c r="L42" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M42" s="99"/>
+      <c r="N42" s="99"/>
+      <c r="O42" s="100"/>
+      <c r="P42" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q42" s="89"/>
+      <c r="R42" s="89"/>
+      <c r="S42" s="89"/>
+      <c r="T42" s="89"/>
+      <c r="U42" s="89"/>
+      <c r="V42" s="89"/>
+      <c r="W42" s="89"/>
       <c r="X42" s="39"/>
-      <c r="Y42" s="70" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z42" s="71"/>
-      <c r="AA42" s="71"/>
-      <c r="AB42" s="72"/>
+      <c r="Y42" s="108" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z42" s="109"/>
+      <c r="AA42" s="109"/>
+      <c r="AB42" s="110"/>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" s="53" t="s">
@@ -4490,12 +4499,12 @@
         <v>27</v>
       </c>
       <c r="D43" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E43" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F43" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E43" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43" s="69"/>
       <c r="G43" s="39"/>
       <c r="H43" s="16">
         <v>1</v>
@@ -4509,29 +4518,29 @@
       <c r="K43" s="10">
         <v>1</v>
       </c>
-      <c r="L43" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M43" s="91"/>
-      <c r="N43" s="91"/>
-      <c r="O43" s="92"/>
-      <c r="P43" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q43" s="74"/>
-      <c r="R43" s="74"/>
-      <c r="S43" s="74"/>
-      <c r="T43" s="74"/>
-      <c r="U43" s="74"/>
-      <c r="V43" s="74"/>
-      <c r="W43" s="74"/>
+      <c r="L43" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M43" s="99"/>
+      <c r="N43" s="99"/>
+      <c r="O43" s="100"/>
+      <c r="P43" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q43" s="89"/>
+      <c r="R43" s="89"/>
+      <c r="S43" s="89"/>
+      <c r="T43" s="89"/>
+      <c r="U43" s="89"/>
+      <c r="V43" s="89"/>
+      <c r="W43" s="89"/>
       <c r="X43" s="39"/>
-      <c r="Y43" s="67" t="s">
-        <v>133</v>
-      </c>
-      <c r="Z43" s="68"/>
-      <c r="AA43" s="68"/>
-      <c r="AB43" s="69"/>
+      <c r="Y43" s="105" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z43" s="106"/>
+      <c r="AA43" s="106"/>
+      <c r="AB43" s="107"/>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" s="51" t="s">
@@ -4539,15 +4548,15 @@
       </c>
       <c r="B44" s="46"/>
       <c r="C44" s="44" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D44" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E44" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F44" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E44" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F44" s="69"/>
       <c r="G44" s="39"/>
       <c r="H44" s="16">
         <v>1</v>
@@ -4561,29 +4570,29 @@
       <c r="K44" s="10">
         <v>1</v>
       </c>
-      <c r="L44" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M44" s="91"/>
-      <c r="N44" s="91"/>
-      <c r="O44" s="92"/>
-      <c r="P44" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q44" s="74"/>
-      <c r="R44" s="74"/>
-      <c r="S44" s="74"/>
-      <c r="T44" s="74"/>
-      <c r="U44" s="74"/>
-      <c r="V44" s="74"/>
-      <c r="W44" s="74"/>
+      <c r="L44" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M44" s="99"/>
+      <c r="N44" s="99"/>
+      <c r="O44" s="100"/>
+      <c r="P44" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q44" s="89"/>
+      <c r="R44" s="89"/>
+      <c r="S44" s="89"/>
+      <c r="T44" s="89"/>
+      <c r="U44" s="89"/>
+      <c r="V44" s="89"/>
+      <c r="W44" s="89"/>
       <c r="X44" s="39"/>
-      <c r="Y44" s="70" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z44" s="71"/>
-      <c r="AA44" s="71"/>
-      <c r="AB44" s="72"/>
+      <c r="Y44" s="108" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z44" s="109"/>
+      <c r="AA44" s="109"/>
+      <c r="AB44" s="110"/>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" s="53" t="s">
@@ -4591,15 +4600,15 @@
       </c>
       <c r="B45" s="39"/>
       <c r="C45" s="43" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="D45" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E45" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F45" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E45" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F45" s="69"/>
       <c r="G45" s="39"/>
       <c r="H45" s="16">
         <v>1</v>
@@ -4613,29 +4622,29 @@
       <c r="K45" s="10">
         <v>1</v>
       </c>
-      <c r="L45" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M45" s="91"/>
-      <c r="N45" s="91"/>
-      <c r="O45" s="92"/>
-      <c r="P45" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q45" s="74"/>
-      <c r="R45" s="74"/>
-      <c r="S45" s="74"/>
-      <c r="T45" s="74"/>
-      <c r="U45" s="74"/>
-      <c r="V45" s="74"/>
-      <c r="W45" s="74"/>
+      <c r="L45" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M45" s="99"/>
+      <c r="N45" s="99"/>
+      <c r="O45" s="100"/>
+      <c r="P45" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q45" s="89"/>
+      <c r="R45" s="89"/>
+      <c r="S45" s="89"/>
+      <c r="T45" s="89"/>
+      <c r="U45" s="89"/>
+      <c r="V45" s="89"/>
+      <c r="W45" s="89"/>
       <c r="X45" s="39"/>
-      <c r="Y45" s="67" t="s">
-        <v>135</v>
-      </c>
-      <c r="Z45" s="68"/>
-      <c r="AA45" s="68"/>
-      <c r="AB45" s="69"/>
+      <c r="Y45" s="105" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z45" s="106"/>
+      <c r="AA45" s="106"/>
+      <c r="AB45" s="107"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" s="51" t="s">
@@ -4643,15 +4652,15 @@
       </c>
       <c r="B46" s="46"/>
       <c r="C46" s="44" t="s">
-        <v>88</v>
+        <v>144</v>
       </c>
       <c r="D46" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E46" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F46" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E46" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F46" s="69"/>
       <c r="G46" s="39"/>
       <c r="H46" s="16">
         <v>1</v>
@@ -4665,29 +4674,29 @@
       <c r="K46" s="10">
         <v>1</v>
       </c>
-      <c r="L46" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M46" s="91"/>
-      <c r="N46" s="91"/>
-      <c r="O46" s="92"/>
-      <c r="P46" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q46" s="74"/>
-      <c r="R46" s="74"/>
-      <c r="S46" s="74"/>
-      <c r="T46" s="74"/>
-      <c r="U46" s="74"/>
-      <c r="V46" s="74"/>
-      <c r="W46" s="74"/>
+      <c r="L46" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M46" s="99"/>
+      <c r="N46" s="99"/>
+      <c r="O46" s="100"/>
+      <c r="P46" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q46" s="89"/>
+      <c r="R46" s="89"/>
+      <c r="S46" s="89"/>
+      <c r="T46" s="89"/>
+      <c r="U46" s="89"/>
+      <c r="V46" s="89"/>
+      <c r="W46" s="89"/>
       <c r="X46" s="39"/>
-      <c r="Y46" s="70" t="s">
-        <v>136</v>
-      </c>
-      <c r="Z46" s="71"/>
-      <c r="AA46" s="71"/>
-      <c r="AB46" s="72"/>
+      <c r="Y46" s="108" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z46" s="109"/>
+      <c r="AA46" s="109"/>
+      <c r="AB46" s="110"/>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" s="53" t="s">
@@ -4695,15 +4704,15 @@
       </c>
       <c r="B47" s="39"/>
       <c r="C47" s="43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D47" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E47" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F47" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E47" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F47" s="69"/>
       <c r="G47" s="39"/>
       <c r="H47" s="16">
         <v>1</v>
@@ -4717,29 +4726,29 @@
       <c r="K47" s="10">
         <v>1</v>
       </c>
-      <c r="L47" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M47" s="91"/>
-      <c r="N47" s="91"/>
-      <c r="O47" s="92"/>
-      <c r="P47" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q47" s="74"/>
-      <c r="R47" s="74"/>
-      <c r="S47" s="74"/>
-      <c r="T47" s="74"/>
-      <c r="U47" s="74"/>
-      <c r="V47" s="74"/>
-      <c r="W47" s="74"/>
+      <c r="L47" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M47" s="99"/>
+      <c r="N47" s="99"/>
+      <c r="O47" s="100"/>
+      <c r="P47" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q47" s="89"/>
+      <c r="R47" s="89"/>
+      <c r="S47" s="89"/>
+      <c r="T47" s="89"/>
+      <c r="U47" s="89"/>
+      <c r="V47" s="89"/>
+      <c r="W47" s="89"/>
       <c r="X47" s="39"/>
-      <c r="Y47" s="67" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z47" s="68"/>
-      <c r="AA47" s="68"/>
-      <c r="AB47" s="69"/>
+      <c r="Y47" s="105" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z47" s="106"/>
+      <c r="AA47" s="106"/>
+      <c r="AB47" s="107"/>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A48" s="51" t="s">
@@ -4747,15 +4756,15 @@
       </c>
       <c r="B48" s="46"/>
       <c r="C48" s="44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D48" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E48" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F48" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E48" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F48" s="69"/>
       <c r="G48" s="39"/>
       <c r="H48" s="16">
         <v>1</v>
@@ -4769,29 +4778,29 @@
       <c r="K48" s="10">
         <v>1</v>
       </c>
-      <c r="L48" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M48" s="91"/>
-      <c r="N48" s="91"/>
-      <c r="O48" s="92"/>
-      <c r="P48" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q48" s="74"/>
-      <c r="R48" s="74"/>
-      <c r="S48" s="74"/>
-      <c r="T48" s="74"/>
-      <c r="U48" s="74"/>
-      <c r="V48" s="74"/>
-      <c r="W48" s="74"/>
+      <c r="L48" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M48" s="99"/>
+      <c r="N48" s="99"/>
+      <c r="O48" s="100"/>
+      <c r="P48" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q48" s="89"/>
+      <c r="R48" s="89"/>
+      <c r="S48" s="89"/>
+      <c r="T48" s="89"/>
+      <c r="U48" s="89"/>
+      <c r="V48" s="89"/>
+      <c r="W48" s="89"/>
       <c r="X48" s="39"/>
-      <c r="Y48" s="70" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z48" s="71"/>
-      <c r="AA48" s="71"/>
-      <c r="AB48" s="72"/>
+      <c r="Y48" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z48" s="109"/>
+      <c r="AA48" s="109"/>
+      <c r="AB48" s="110"/>
     </row>
     <row r="49" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A49" s="53" t="s">
@@ -4799,15 +4808,15 @@
       </c>
       <c r="B49" s="39"/>
       <c r="C49" s="43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D49" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E49" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F49" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E49" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F49" s="69"/>
       <c r="G49" s="39"/>
       <c r="H49" s="16">
         <v>1</v>
@@ -4821,31 +4830,31 @@
       <c r="K49" s="10">
         <v>1</v>
       </c>
-      <c r="L49" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M49" s="91"/>
-      <c r="N49" s="91"/>
-      <c r="O49" s="92"/>
-      <c r="P49" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q49" s="74"/>
-      <c r="R49" s="74"/>
-      <c r="S49" s="74"/>
-      <c r="T49" s="74"/>
-      <c r="U49" s="74"/>
-      <c r="V49" s="74"/>
-      <c r="W49" s="74"/>
+      <c r="L49" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M49" s="99"/>
+      <c r="N49" s="99"/>
+      <c r="O49" s="100"/>
+      <c r="P49" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q49" s="89"/>
+      <c r="R49" s="89"/>
+      <c r="S49" s="89"/>
+      <c r="T49" s="89"/>
+      <c r="U49" s="89"/>
+      <c r="V49" s="89"/>
+      <c r="W49" s="89"/>
       <c r="X49" s="39"/>
-      <c r="Y49" s="67" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z49" s="68"/>
-      <c r="AA49" s="68"/>
-      <c r="AB49" s="69"/>
+      <c r="Y49" s="105" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z49" s="106"/>
+      <c r="AA49" s="106"/>
+      <c r="AB49" s="107"/>
       <c r="AP49" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:42" x14ac:dyDescent="0.3">
@@ -4854,15 +4863,15 @@
       </c>
       <c r="B50" s="46"/>
       <c r="C50" s="44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D50" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E50" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F50" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E50" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F50" s="69"/>
       <c r="G50" s="39"/>
       <c r="H50" s="16">
         <v>1</v>
@@ -4876,29 +4885,29 @@
       <c r="K50" s="10">
         <v>1</v>
       </c>
-      <c r="L50" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M50" s="91"/>
-      <c r="N50" s="91"/>
-      <c r="O50" s="92"/>
-      <c r="P50" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q50" s="74"/>
-      <c r="R50" s="74"/>
-      <c r="S50" s="74"/>
-      <c r="T50" s="74"/>
-      <c r="U50" s="74"/>
-      <c r="V50" s="74"/>
-      <c r="W50" s="74"/>
+      <c r="L50" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M50" s="99"/>
+      <c r="N50" s="99"/>
+      <c r="O50" s="100"/>
+      <c r="P50" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q50" s="89"/>
+      <c r="R50" s="89"/>
+      <c r="S50" s="89"/>
+      <c r="T50" s="89"/>
+      <c r="U50" s="89"/>
+      <c r="V50" s="89"/>
+      <c r="W50" s="89"/>
       <c r="X50" s="39"/>
-      <c r="Y50" s="70" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z50" s="71"/>
-      <c r="AA50" s="71"/>
-      <c r="AB50" s="72"/>
+      <c r="Y50" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z50" s="109"/>
+      <c r="AA50" s="109"/>
+      <c r="AB50" s="110"/>
     </row>
     <row r="51" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A51" s="53" t="s">
@@ -4906,15 +4915,15 @@
       </c>
       <c r="B51" s="39"/>
       <c r="C51" s="43" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D51" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E51" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F51" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E51" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F51" s="69"/>
       <c r="G51" s="39"/>
       <c r="H51" s="16">
         <v>1</v>
@@ -4928,29 +4937,29 @@
       <c r="K51" s="10">
         <v>1</v>
       </c>
-      <c r="L51" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M51" s="91"/>
-      <c r="N51" s="91"/>
-      <c r="O51" s="92"/>
-      <c r="P51" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q51" s="74"/>
-      <c r="R51" s="74"/>
-      <c r="S51" s="74"/>
-      <c r="T51" s="74"/>
-      <c r="U51" s="74"/>
-      <c r="V51" s="74"/>
-      <c r="W51" s="74"/>
+      <c r="L51" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M51" s="99"/>
+      <c r="N51" s="99"/>
+      <c r="O51" s="100"/>
+      <c r="P51" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q51" s="89"/>
+      <c r="R51" s="89"/>
+      <c r="S51" s="89"/>
+      <c r="T51" s="89"/>
+      <c r="U51" s="89"/>
+      <c r="V51" s="89"/>
+      <c r="W51" s="89"/>
       <c r="X51" s="39"/>
-      <c r="Y51" s="67" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z51" s="68"/>
-      <c r="AA51" s="68"/>
-      <c r="AB51" s="69"/>
+      <c r="Y51" s="105" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z51" s="106"/>
+      <c r="AA51" s="106"/>
+      <c r="AB51" s="107"/>
     </row>
     <row r="52" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A52" s="51" t="s">
@@ -4958,15 +4967,15 @@
       </c>
       <c r="B52" s="46"/>
       <c r="C52" s="44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D52" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E52" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F52" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E52" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F52" s="69"/>
       <c r="G52" s="39"/>
       <c r="H52" s="16">
         <v>1</v>
@@ -4980,29 +4989,29 @@
       <c r="K52" s="10">
         <v>1</v>
       </c>
-      <c r="L52" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M52" s="91"/>
-      <c r="N52" s="91"/>
-      <c r="O52" s="92"/>
-      <c r="P52" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q52" s="74"/>
-      <c r="R52" s="74"/>
-      <c r="S52" s="74"/>
-      <c r="T52" s="74"/>
-      <c r="U52" s="74"/>
-      <c r="V52" s="74"/>
-      <c r="W52" s="74"/>
+      <c r="L52" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M52" s="99"/>
+      <c r="N52" s="99"/>
+      <c r="O52" s="100"/>
+      <c r="P52" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q52" s="89"/>
+      <c r="R52" s="89"/>
+      <c r="S52" s="89"/>
+      <c r="T52" s="89"/>
+      <c r="U52" s="89"/>
+      <c r="V52" s="89"/>
+      <c r="W52" s="89"/>
       <c r="X52" s="39"/>
-      <c r="Y52" s="70" t="s">
-        <v>142</v>
-      </c>
-      <c r="Z52" s="71"/>
-      <c r="AA52" s="71"/>
-      <c r="AB52" s="72"/>
+      <c r="Y52" s="108" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z52" s="109"/>
+      <c r="AA52" s="109"/>
+      <c r="AB52" s="110"/>
     </row>
     <row r="53" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A53" s="53" t="s">
@@ -5010,15 +5019,15 @@
       </c>
       <c r="B53" s="39"/>
       <c r="C53" s="43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D53" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="E53" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="F53" s="76"/>
+        <v>124</v>
+      </c>
+      <c r="E53" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="F53" s="69"/>
       <c r="G53" s="39"/>
       <c r="H53" s="16">
         <v>1</v>
@@ -5032,22 +5041,22 @@
       <c r="K53" s="10">
         <v>1</v>
       </c>
-      <c r="L53" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="M53" s="91"/>
-      <c r="N53" s="91"/>
-      <c r="O53" s="92"/>
-      <c r="P53" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q53" s="74"/>
-      <c r="R53" s="74"/>
-      <c r="S53" s="74"/>
-      <c r="T53" s="74"/>
-      <c r="U53" s="74"/>
-      <c r="V53" s="74"/>
-      <c r="W53" s="74"/>
+      <c r="L53" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="M53" s="99"/>
+      <c r="N53" s="99"/>
+      <c r="O53" s="100"/>
+      <c r="P53" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q53" s="89"/>
+      <c r="R53" s="89"/>
+      <c r="S53" s="89"/>
+      <c r="T53" s="89"/>
+      <c r="U53" s="89"/>
+      <c r="V53" s="89"/>
+      <c r="W53" s="89"/>
       <c r="X53" s="39"/>
       <c r="Y53" s="37" t="b">
         <v>0</v>
@@ -5064,19 +5073,17 @@
     </row>
     <row r="54" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="57" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B54" s="58"/>
       <c r="C54" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="D54" s="65" t="s">
-        <v>126</v>
-      </c>
-      <c r="E54" s="111" t="s">
-        <v>121</v>
-      </c>
-      <c r="F54" s="112"/>
+        <v>122</v>
+      </c>
+      <c r="D54" s="114"/>
+      <c r="E54" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="F54" s="67"/>
       <c r="G54" s="58"/>
       <c r="H54" s="60">
         <v>1</v>
@@ -5093,19 +5100,19 @@
       <c r="L54" s="23">
         <v>0</v>
       </c>
-      <c r="M54" s="78" t="s">
-        <v>125</v>
-      </c>
-      <c r="N54" s="79"/>
-      <c r="O54" s="79"/>
-      <c r="P54" s="79"/>
-      <c r="Q54" s="79"/>
-      <c r="R54" s="79"/>
-      <c r="S54" s="79"/>
-      <c r="T54" s="79"/>
-      <c r="U54" s="79"/>
-      <c r="V54" s="79"/>
-      <c r="W54" s="79"/>
+      <c r="M54" s="112" t="s">
+        <v>123</v>
+      </c>
+      <c r="N54" s="113"/>
+      <c r="O54" s="113"/>
+      <c r="P54" s="113"/>
+      <c r="Q54" s="113"/>
+      <c r="R54" s="113"/>
+      <c r="S54" s="113"/>
+      <c r="T54" s="113"/>
+      <c r="U54" s="113"/>
+      <c r="V54" s="113"/>
+      <c r="W54" s="113"/>
       <c r="X54" s="58"/>
       <c r="Y54" s="61" t="b">
         <v>0</v>
@@ -5121,31 +5128,129 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="170">
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="Y6:AB6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="U7:W7"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="U9:W9"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="R31:T31"/>
-    <mergeCell ref="U31:W31"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="M5:Q5"/>
-    <mergeCell ref="R3:T3"/>
+  <mergeCells count="169">
+    <mergeCell ref="Y39:AB39"/>
+    <mergeCell ref="Y40:AB40"/>
+    <mergeCell ref="Y41:AB41"/>
+    <mergeCell ref="Y42:AB42"/>
+    <mergeCell ref="Y43:AB43"/>
+    <mergeCell ref="Y44:AB44"/>
+    <mergeCell ref="Y45:AB45"/>
+    <mergeCell ref="Y46:AB46"/>
+    <mergeCell ref="P39:W39"/>
+    <mergeCell ref="P40:W40"/>
+    <mergeCell ref="P41:W41"/>
+    <mergeCell ref="P42:W42"/>
+    <mergeCell ref="P43:W43"/>
+    <mergeCell ref="Y47:AB47"/>
+    <mergeCell ref="Y48:AB48"/>
+    <mergeCell ref="Y49:AB49"/>
+    <mergeCell ref="Y50:AB50"/>
+    <mergeCell ref="Y51:AB51"/>
+    <mergeCell ref="Y52:AB52"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="H1:W1"/>
+    <mergeCell ref="M54:W54"/>
+    <mergeCell ref="P33:W33"/>
+    <mergeCell ref="P34:W34"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="O6:W6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="R15:W15"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="O32:W32"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="P13:W13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="P14:W14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="L49:O49"/>
+    <mergeCell ref="L50:O50"/>
+    <mergeCell ref="L51:O51"/>
+    <mergeCell ref="L52:O52"/>
+    <mergeCell ref="P49:W49"/>
+    <mergeCell ref="P50:W50"/>
+    <mergeCell ref="P51:W51"/>
+    <mergeCell ref="P52:W52"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="P53:W53"/>
+    <mergeCell ref="L47:O47"/>
+    <mergeCell ref="L48:O48"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:O40"/>
+    <mergeCell ref="L41:O41"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="L43:O43"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="U28:W28"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="U29:W29"/>
+    <mergeCell ref="R30:T30"/>
+    <mergeCell ref="P44:W44"/>
+    <mergeCell ref="P45:W45"/>
+    <mergeCell ref="P46:W46"/>
+    <mergeCell ref="P47:W47"/>
+    <mergeCell ref="P48:W48"/>
+    <mergeCell ref="L38:O38"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="L45:O45"/>
+    <mergeCell ref="L46:O46"/>
+    <mergeCell ref="P12:W12"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="Q36:W36"/>
+    <mergeCell ref="Q37:W37"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="U30:W30"/>
+    <mergeCell ref="U27:W27"/>
+    <mergeCell ref="L35:R35"/>
+    <mergeCell ref="S35:W35"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="U25:W25"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="U26:W26"/>
+    <mergeCell ref="R27:T27"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="R18:T18"/>
     <mergeCell ref="U18:W18"/>
@@ -5170,128 +5275,29 @@
     <mergeCell ref="M11:O11"/>
     <mergeCell ref="P11:W11"/>
     <mergeCell ref="M12:O12"/>
-    <mergeCell ref="P12:W12"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="Q36:W36"/>
-    <mergeCell ref="Q37:W37"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="U30:W30"/>
-    <mergeCell ref="U27:W27"/>
-    <mergeCell ref="L35:R35"/>
-    <mergeCell ref="S35:W35"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="U25:W25"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="U26:W26"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="L47:O47"/>
-    <mergeCell ref="L48:O48"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:O40"/>
-    <mergeCell ref="L41:O41"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="L43:O43"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="U28:W28"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="U29:W29"/>
-    <mergeCell ref="R30:T30"/>
-    <mergeCell ref="P44:W44"/>
-    <mergeCell ref="P45:W45"/>
-    <mergeCell ref="P46:W46"/>
-    <mergeCell ref="P47:W47"/>
-    <mergeCell ref="P48:W48"/>
-    <mergeCell ref="L38:O38"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="L45:O45"/>
-    <mergeCell ref="L46:O46"/>
-    <mergeCell ref="L49:O49"/>
-    <mergeCell ref="L50:O50"/>
-    <mergeCell ref="L51:O51"/>
-    <mergeCell ref="L52:O52"/>
-    <mergeCell ref="P49:W49"/>
-    <mergeCell ref="P50:W50"/>
-    <mergeCell ref="P51:W51"/>
-    <mergeCell ref="P52:W52"/>
-    <mergeCell ref="L53:O53"/>
-    <mergeCell ref="P53:W53"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P13:W13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="P14:W14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="Y47:AB47"/>
-    <mergeCell ref="Y48:AB48"/>
-    <mergeCell ref="Y49:AB49"/>
-    <mergeCell ref="Y50:AB50"/>
-    <mergeCell ref="Y51:AB51"/>
-    <mergeCell ref="Y52:AB52"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="H1:W1"/>
-    <mergeCell ref="M54:W54"/>
-    <mergeCell ref="P33:W33"/>
-    <mergeCell ref="P34:W34"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="O6:W6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="R15:W15"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="O32:W32"/>
-    <mergeCell ref="Y39:AB39"/>
-    <mergeCell ref="Y40:AB40"/>
-    <mergeCell ref="Y41:AB41"/>
-    <mergeCell ref="Y42:AB42"/>
-    <mergeCell ref="Y43:AB43"/>
-    <mergeCell ref="Y44:AB44"/>
-    <mergeCell ref="Y45:AB45"/>
-    <mergeCell ref="Y46:AB46"/>
-    <mergeCell ref="P39:W39"/>
-    <mergeCell ref="P40:W40"/>
-    <mergeCell ref="P41:W41"/>
-    <mergeCell ref="P42:W42"/>
-    <mergeCell ref="P43:W43"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="U7:W7"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="R31:T31"/>
+    <mergeCell ref="U31:W31"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="M4:Q4"/>
+    <mergeCell ref="M5:Q5"/>
+    <mergeCell ref="R3:T3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5468,20 +5474,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b05417e1-eb89-4392-aea8-ecdaf8fc0423" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b05417e1-eb89-4392-aea8-ecdaf8fc0423" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5503,14 +5509,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEFCFB9-977F-4BC6-8CD6-7A1E4BA64254}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE327FA-98F8-4626-AE66-90F799A55F58}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5524,4 +5522,12 @@
     <ds:schemaRef ds:uri="b05417e1-eb89-4392-aea8-ecdaf8fc0423"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEFCFB9-977F-4BC6-8CD6-7A1E4BA64254}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tests de Shift_Add_Sub_Mov bon !
</commit_message>
<xml_diff>
--- a/Encodage_PARM.xlsx
+++ b/Encodage_PARM.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\habib\PROJARCHI\Projet-P-ARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F20566-B01E-4588-922A-652592329052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D644A86B-F885-4828-AAD2-D65ADDCFED67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15216" yWindow="0" windowWidth="7920" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Encodage PARM" sheetId="1" r:id="rId1"/>
+    <sheet name="Graphique1" sheetId="2" r:id="rId1"/>
+    <sheet name="Encodage PARM" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="148">
   <si>
     <t>Description</t>
   </si>
@@ -665,6 +666,9 @@
   </si>
   <si>
     <t>&lt;Rn&gt;</t>
+  </si>
+  <si>
+    <t>xx</t>
   </si>
 </sst>
 </file>
@@ -1364,115 +1368,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1523,6 +1419,18 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1532,8 +1440,104 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1555,6 +1559,909 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Encodage PARM'!$F$7:$F$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>&lt;Rm&gt;</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&lt;Rm&gt;</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#&lt;imm3 &gt;</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#&lt;imm3 &gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Encodage PARM'!$C$11:$E$14</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>#&lt;imm8&gt;</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>#&lt;imm8&gt;</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>#&lt;imm8&gt;</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>#&lt;imm8&gt;</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>&lt;Rd &gt;</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>&lt;Rd &gt;</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>&lt;Rd &gt;</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>&lt;Rd &gt;</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>MOVS</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>CMPS</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>ADDS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>SUBS</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Encodage PARM'!$F$11:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7096-4ED6-9D9C-C7AB3EFD043B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1483583904"/>
+        <c:axId val="1483586784"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1483583904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1483586784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1483586784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1483583904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{15BEB18B-C54D-461E-8BB6-7CDA4B326474}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="112" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9286875" cy="6061982"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79BB590F-AE47-B055-1ED9-421D90E7A47D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1861,8 +2768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F12" zoomScale="92" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="92" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1881,54 +2788,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="47"/>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="93"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="108"/>
       <c r="G1" s="48"/>
-      <c r="H1" s="111" t="s">
+      <c r="H1" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
       <c r="X1" s="49"/>
-      <c r="Y1" s="70" t="s">
+      <c r="Y1" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="71"/>
-      <c r="AA1" s="71"/>
-      <c r="AB1" s="72"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="107"/>
+      <c r="AB1" s="113"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" s="92"/>
+      <c r="A2" s="105"/>
       <c r="B2" s="45"/>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="74"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="82"/>
       <c r="G2" s="38"/>
       <c r="H2" s="3">
         <v>15</v>
@@ -2025,23 +2932,23 @@
       <c r="L3" s="32">
         <v>0</v>
       </c>
-      <c r="M3" s="88" t="s">
+      <c r="M3" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="90"/>
-      <c r="R3" s="78" t="s">
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="112"/>
+      <c r="R3" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="S3" s="79"/>
-      <c r="T3" s="80"/>
-      <c r="U3" s="86" t="s">
+      <c r="S3" s="110"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="V3" s="87"/>
-      <c r="W3" s="87"/>
+      <c r="V3" s="88"/>
+      <c r="W3" s="88"/>
       <c r="X3" s="39"/>
       <c r="Y3" s="35" t="b">
         <v>1</v>
@@ -2089,23 +2996,23 @@
       <c r="L4" s="12">
         <v>1</v>
       </c>
-      <c r="M4" s="88" t="s">
+      <c r="M4" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="78" t="s">
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="112"/>
+      <c r="R4" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="S4" s="79"/>
-      <c r="T4" s="80"/>
-      <c r="U4" s="86" t="s">
+      <c r="S4" s="110"/>
+      <c r="T4" s="111"/>
+      <c r="U4" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="V4" s="87"/>
-      <c r="W4" s="87"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="88"/>
       <c r="X4" s="39"/>
       <c r="Y4" s="36" t="b">
         <v>1</v>
@@ -2153,23 +3060,23 @@
       <c r="L5" s="32">
         <v>0</v>
       </c>
-      <c r="M5" s="88" t="s">
+      <c r="M5" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="90"/>
-      <c r="R5" s="78" t="s">
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="112"/>
+      <c r="R5" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="S5" s="79"/>
-      <c r="T5" s="80"/>
-      <c r="U5" s="86" t="s">
+      <c r="S5" s="110"/>
+      <c r="T5" s="111"/>
+      <c r="U5" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="V5" s="87"/>
-      <c r="W5" s="87"/>
+      <c r="V5" s="88"/>
+      <c r="W5" s="88"/>
       <c r="X5" s="39"/>
       <c r="Y5" s="35" t="b">
         <v>1</v>
@@ -2190,9 +3097,9 @@
       </c>
       <c r="B6" s="45"/>
       <c r="C6" s="34"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="74"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="82"/>
       <c r="G6" s="38"/>
       <c r="H6" s="3">
         <v>0</v>
@@ -2200,27 +3107,27 @@
       <c r="I6" s="1">
         <v>0</v>
       </c>
-      <c r="J6" s="74" t="s">
+      <c r="J6" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="77"/>
-      <c r="R6" s="77"/>
-      <c r="S6" s="77"/>
-      <c r="T6" s="77"/>
-      <c r="U6" s="77"/>
-      <c r="V6" s="77"/>
-      <c r="W6" s="77"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="83"/>
+      <c r="M6" s="83"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="83"/>
+      <c r="Q6" s="83"/>
+      <c r="R6" s="83"/>
+      <c r="S6" s="83"/>
+      <c r="T6" s="83"/>
+      <c r="U6" s="83"/>
+      <c r="V6" s="83"/>
+      <c r="W6" s="83"/>
       <c r="X6" s="38"/>
-      <c r="Y6" s="75"/>
-      <c r="Z6" s="73"/>
-      <c r="AA6" s="73"/>
-      <c r="AB6" s="76"/>
+      <c r="Y6" s="103"/>
+      <c r="Z6" s="84"/>
+      <c r="AA6" s="84"/>
+      <c r="AB6" s="114"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
@@ -2261,21 +3168,21 @@
       <c r="N7" s="32">
         <v>0</v>
       </c>
-      <c r="O7" s="81" t="s">
+      <c r="O7" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="83"/>
-      <c r="R7" s="78" t="s">
+      <c r="P7" s="86"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="S7" s="79"/>
-      <c r="T7" s="80"/>
-      <c r="U7" s="86" t="s">
+      <c r="S7" s="110"/>
+      <c r="T7" s="111"/>
+      <c r="U7" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="V7" s="87"/>
-      <c r="W7" s="87"/>
+      <c r="V7" s="88"/>
+      <c r="W7" s="88"/>
       <c r="X7" s="39"/>
       <c r="Y7" s="35" t="b">
         <v>1</v>
@@ -2299,7 +3206,7 @@
         <v>68</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>95</v>
@@ -2329,21 +3236,21 @@
       <c r="N8" s="12">
         <v>1</v>
       </c>
-      <c r="O8" s="81" t="s">
+      <c r="O8" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="P8" s="82"/>
-      <c r="Q8" s="83"/>
-      <c r="R8" s="78" t="s">
+      <c r="P8" s="86"/>
+      <c r="Q8" s="95"/>
+      <c r="R8" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="S8" s="79"/>
-      <c r="T8" s="80"/>
-      <c r="U8" s="86" t="s">
+      <c r="S8" s="110"/>
+      <c r="T8" s="111"/>
+      <c r="U8" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="V8" s="87"/>
-      <c r="W8" s="87"/>
+      <c r="V8" s="88"/>
+      <c r="W8" s="88"/>
       <c r="X8" s="39"/>
       <c r="Y8" s="36" t="b">
         <v>1</v>
@@ -2397,21 +3304,21 @@
       <c r="N9" s="32">
         <v>0</v>
       </c>
-      <c r="O9" s="88" t="s">
+      <c r="O9" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="P9" s="89"/>
-      <c r="Q9" s="90"/>
-      <c r="R9" s="78" t="s">
+      <c r="P9" s="76"/>
+      <c r="Q9" s="112"/>
+      <c r="R9" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="S9" s="79"/>
-      <c r="T9" s="80"/>
-      <c r="U9" s="86" t="s">
+      <c r="S9" s="110"/>
+      <c r="T9" s="111"/>
+      <c r="U9" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="V9" s="87"/>
-      <c r="W9" s="87"/>
+      <c r="V9" s="88"/>
+      <c r="W9" s="88"/>
       <c r="X9" s="39"/>
       <c r="Y9" s="35" t="b">
         <v>1</v>
@@ -2465,21 +3372,21 @@
       <c r="N10" s="12">
         <v>1</v>
       </c>
-      <c r="O10" s="88" t="s">
+      <c r="O10" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="P10" s="89"/>
-      <c r="Q10" s="90"/>
-      <c r="R10" s="78" t="s">
+      <c r="P10" s="76"/>
+      <c r="Q10" s="112"/>
+      <c r="R10" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="S10" s="79"/>
-      <c r="T10" s="80"/>
-      <c r="U10" s="86" t="s">
+      <c r="S10" s="110"/>
+      <c r="T10" s="111"/>
+      <c r="U10" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="V10" s="87"/>
-      <c r="W10" s="87"/>
+      <c r="V10" s="88"/>
+      <c r="W10" s="88"/>
       <c r="X10" s="39"/>
       <c r="Y10" s="36" t="b">
         <v>1</v>
@@ -2505,10 +3412,10 @@
       <c r="D11" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="88" t="s">
+      <c r="E11" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="F11" s="89"/>
+      <c r="F11" s="76"/>
       <c r="G11" s="39"/>
       <c r="H11" s="13">
         <v>0</v>
@@ -2525,21 +3432,21 @@
       <c r="L11" s="32">
         <v>0</v>
       </c>
-      <c r="M11" s="86" t="s">
+      <c r="M11" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="N11" s="87"/>
-      <c r="O11" s="94"/>
-      <c r="P11" s="88" t="s">
+      <c r="N11" s="88"/>
+      <c r="O11" s="89"/>
+      <c r="P11" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="Q11" s="89"/>
-      <c r="R11" s="89"/>
-      <c r="S11" s="89"/>
-      <c r="T11" s="89"/>
-      <c r="U11" s="89"/>
-      <c r="V11" s="89"/>
-      <c r="W11" s="89"/>
+      <c r="Q11" s="76"/>
+      <c r="R11" s="76"/>
+      <c r="S11" s="76"/>
+      <c r="T11" s="76"/>
+      <c r="U11" s="76"/>
+      <c r="V11" s="76"/>
+      <c r="W11" s="76"/>
       <c r="X11" s="39"/>
       <c r="Y11" s="35" t="b">
         <v>0</v>
@@ -2565,10 +3472,10 @@
       <c r="D12" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="88" t="s">
+      <c r="E12" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="89"/>
+      <c r="F12" s="76"/>
       <c r="G12" s="39"/>
       <c r="H12" s="13">
         <v>0</v>
@@ -2585,21 +3492,21 @@
       <c r="L12" s="12">
         <v>1</v>
       </c>
-      <c r="M12" s="86" t="s">
+      <c r="M12" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="N12" s="87"/>
-      <c r="O12" s="94"/>
-      <c r="P12" s="88" t="s">
+      <c r="N12" s="88"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="89"/>
-      <c r="S12" s="89"/>
-      <c r="T12" s="89"/>
-      <c r="U12" s="89"/>
-      <c r="V12" s="89"/>
-      <c r="W12" s="89"/>
+      <c r="Q12" s="76"/>
+      <c r="R12" s="76"/>
+      <c r="S12" s="76"/>
+      <c r="T12" s="76"/>
+      <c r="U12" s="76"/>
+      <c r="V12" s="76"/>
+      <c r="W12" s="76"/>
       <c r="X12" s="39"/>
       <c r="Y12" s="36" t="b">
         <v>0</v>
@@ -2625,10 +3532,10 @@
       <c r="D13" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="88" t="s">
+      <c r="E13" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="F13" s="89"/>
+      <c r="F13" s="76"/>
       <c r="G13" s="39"/>
       <c r="H13" s="13">
         <v>0</v>
@@ -2645,21 +3552,21 @@
       <c r="L13" s="32">
         <v>0</v>
       </c>
-      <c r="M13" s="86" t="s">
+      <c r="M13" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="N13" s="87"/>
-      <c r="O13" s="94"/>
-      <c r="P13" s="88" t="s">
+      <c r="N13" s="88"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="89"/>
-      <c r="S13" s="89"/>
-      <c r="T13" s="89"/>
-      <c r="U13" s="89"/>
-      <c r="V13" s="89"/>
-      <c r="W13" s="89"/>
+      <c r="Q13" s="76"/>
+      <c r="R13" s="76"/>
+      <c r="S13" s="76"/>
+      <c r="T13" s="76"/>
+      <c r="U13" s="76"/>
+      <c r="V13" s="76"/>
+      <c r="W13" s="76"/>
       <c r="X13" s="39"/>
       <c r="Y13" s="35" t="b">
         <v>1</v>
@@ -2685,10 +3592,10 @@
       <c r="D14" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="88" t="s">
+      <c r="E14" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="F14" s="89"/>
+      <c r="F14" s="76"/>
       <c r="G14" s="39"/>
       <c r="H14" s="13">
         <v>0</v>
@@ -2705,21 +3612,21 @@
       <c r="L14" s="12">
         <v>1</v>
       </c>
-      <c r="M14" s="86" t="s">
+      <c r="M14" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="N14" s="87"/>
-      <c r="O14" s="94"/>
-      <c r="P14" s="88" t="s">
+      <c r="N14" s="88"/>
+      <c r="O14" s="89"/>
+      <c r="P14" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="Q14" s="89"/>
-      <c r="R14" s="89"/>
-      <c r="S14" s="89"/>
-      <c r="T14" s="89"/>
-      <c r="U14" s="89"/>
-      <c r="V14" s="89"/>
-      <c r="W14" s="89"/>
+      <c r="Q14" s="76"/>
+      <c r="R14" s="76"/>
+      <c r="S14" s="76"/>
+      <c r="T14" s="76"/>
+      <c r="U14" s="76"/>
+      <c r="V14" s="76"/>
+      <c r="W14" s="76"/>
       <c r="X14" s="39"/>
       <c r="Y14" s="36" t="b">
         <v>1</v>
@@ -2740,9 +3647,9 @@
       </c>
       <c r="B15" s="45"/>
       <c r="C15" s="34"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
       <c r="G15" s="38"/>
       <c r="H15" s="3">
         <v>0</v>
@@ -2762,18 +3669,18 @@
       <c r="M15" s="1">
         <v>0</v>
       </c>
-      <c r="N15" s="74" t="s">
+      <c r="N15" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="O15" s="77"/>
-      <c r="P15" s="77"/>
-      <c r="Q15" s="77"/>
-      <c r="R15" s="73"/>
-      <c r="S15" s="73"/>
-      <c r="T15" s="73"/>
-      <c r="U15" s="73"/>
-      <c r="V15" s="73"/>
-      <c r="W15" s="73"/>
+      <c r="O15" s="83"/>
+      <c r="P15" s="83"/>
+      <c r="Q15" s="83"/>
+      <c r="R15" s="84"/>
+      <c r="S15" s="84"/>
+      <c r="T15" s="84"/>
+      <c r="U15" s="84"/>
+      <c r="V15" s="84"/>
+      <c r="W15" s="84"/>
       <c r="X15" s="38"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="1"/>
@@ -2791,10 +3698,10 @@
       <c r="D16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="81" t="s">
+      <c r="E16" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="82"/>
+      <c r="F16" s="86"/>
       <c r="G16" s="39"/>
       <c r="H16" s="13">
         <v>0</v>
@@ -2826,16 +3733,16 @@
       <c r="Q16" s="12">
         <v>0</v>
       </c>
-      <c r="R16" s="81" t="s">
+      <c r="R16" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S16" s="82"/>
-      <c r="T16" s="83"/>
-      <c r="U16" s="84" t="s">
+      <c r="S16" s="86"/>
+      <c r="T16" s="95"/>
+      <c r="U16" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="V16" s="85"/>
-      <c r="W16" s="85"/>
+      <c r="V16" s="97"/>
+      <c r="W16" s="97"/>
       <c r="X16" s="39"/>
       <c r="Y16" s="36" t="b">
         <v>1</v>
@@ -2861,10 +3768,10 @@
       <c r="D17" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="81" t="s">
+      <c r="E17" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="82"/>
+      <c r="F17" s="86"/>
       <c r="G17" s="39"/>
       <c r="H17" s="41">
         <v>0</v>
@@ -2896,16 +3803,16 @@
       <c r="Q17" s="32">
         <v>1</v>
       </c>
-      <c r="R17" s="81" t="s">
+      <c r="R17" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S17" s="82"/>
-      <c r="T17" s="83"/>
-      <c r="U17" s="84" t="s">
+      <c r="S17" s="86"/>
+      <c r="T17" s="95"/>
+      <c r="U17" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="V17" s="85"/>
-      <c r="W17" s="85"/>
+      <c r="V17" s="97"/>
+      <c r="W17" s="97"/>
       <c r="X17" s="39"/>
       <c r="Y17" s="35" t="b">
         <v>1</v>
@@ -2931,10 +3838,10 @@
       <c r="D18" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="81" t="s">
+      <c r="E18" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="82"/>
+      <c r="F18" s="86"/>
       <c r="G18" s="39"/>
       <c r="H18" s="13">
         <v>0</v>
@@ -2966,16 +3873,16 @@
       <c r="Q18" s="12">
         <v>0</v>
       </c>
-      <c r="R18" s="81" t="s">
+      <c r="R18" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S18" s="82"/>
-      <c r="T18" s="83"/>
-      <c r="U18" s="84" t="s">
+      <c r="S18" s="86"/>
+      <c r="T18" s="95"/>
+      <c r="U18" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="V18" s="85"/>
-      <c r="W18" s="85"/>
+      <c r="V18" s="97"/>
+      <c r="W18" s="97"/>
       <c r="X18" s="39"/>
       <c r="Y18" s="36" t="b">
         <v>1</v>
@@ -3001,10 +3908,10 @@
       <c r="D19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="81" t="s">
+      <c r="E19" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="82"/>
+      <c r="F19" s="86"/>
       <c r="G19" s="39"/>
       <c r="H19" s="41">
         <v>0</v>
@@ -3036,16 +3943,16 @@
       <c r="Q19" s="32">
         <v>1</v>
       </c>
-      <c r="R19" s="81" t="s">
+      <c r="R19" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S19" s="82"/>
-      <c r="T19" s="83"/>
-      <c r="U19" s="84" t="s">
+      <c r="S19" s="86"/>
+      <c r="T19" s="95"/>
+      <c r="U19" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="V19" s="85"/>
-      <c r="W19" s="85"/>
+      <c r="V19" s="97"/>
+      <c r="W19" s="97"/>
       <c r="X19" s="39"/>
       <c r="Y19" s="35" t="b">
         <v>1</v>
@@ -3071,10 +3978,10 @@
       <c r="D20" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="81" t="s">
+      <c r="E20" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="82"/>
+      <c r="F20" s="86"/>
       <c r="G20" s="39"/>
       <c r="H20" s="13">
         <v>0</v>
@@ -3106,16 +4013,16 @@
       <c r="Q20" s="12">
         <v>0</v>
       </c>
-      <c r="R20" s="81" t="s">
+      <c r="R20" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S20" s="82"/>
-      <c r="T20" s="83"/>
-      <c r="U20" s="84" t="s">
+      <c r="S20" s="86"/>
+      <c r="T20" s="95"/>
+      <c r="U20" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="V20" s="85"/>
-      <c r="W20" s="85"/>
+      <c r="V20" s="97"/>
+      <c r="W20" s="97"/>
       <c r="X20" s="39"/>
       <c r="Y20" s="36" t="b">
         <v>1</v>
@@ -3141,10 +4048,10 @@
       <c r="D21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="81" t="s">
+      <c r="E21" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="82"/>
+      <c r="F21" s="86"/>
       <c r="G21" s="39"/>
       <c r="H21" s="41">
         <v>0</v>
@@ -3176,16 +4083,16 @@
       <c r="Q21" s="32">
         <v>1</v>
       </c>
-      <c r="R21" s="81" t="s">
+      <c r="R21" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S21" s="82"/>
-      <c r="T21" s="83"/>
-      <c r="U21" s="84" t="s">
+      <c r="S21" s="86"/>
+      <c r="T21" s="95"/>
+      <c r="U21" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="V21" s="85"/>
-      <c r="W21" s="85"/>
+      <c r="V21" s="97"/>
+      <c r="W21" s="97"/>
       <c r="X21" s="39"/>
       <c r="Y21" s="35" t="b">
         <v>1</v>
@@ -3211,10 +4118,10 @@
       <c r="D22" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="81" t="s">
+      <c r="E22" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="82"/>
+      <c r="F22" s="86"/>
       <c r="G22" s="39"/>
       <c r="H22" s="13">
         <v>0</v>
@@ -3246,16 +4153,16 @@
       <c r="Q22" s="12">
         <v>0</v>
       </c>
-      <c r="R22" s="81" t="s">
+      <c r="R22" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S22" s="82"/>
-      <c r="T22" s="83"/>
-      <c r="U22" s="84" t="s">
+      <c r="S22" s="86"/>
+      <c r="T22" s="95"/>
+      <c r="U22" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="V22" s="85"/>
-      <c r="W22" s="85"/>
+      <c r="V22" s="97"/>
+      <c r="W22" s="97"/>
       <c r="X22" s="39"/>
       <c r="Y22" s="36" t="b">
         <v>1</v>
@@ -3281,10 +4188,10 @@
       <c r="D23" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="81" t="s">
+      <c r="E23" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="82"/>
+      <c r="F23" s="86"/>
       <c r="G23" s="39"/>
       <c r="H23" s="41">
         <v>0</v>
@@ -3316,16 +4223,16 @@
       <c r="Q23" s="32">
         <v>1</v>
       </c>
-      <c r="R23" s="81" t="s">
+      <c r="R23" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S23" s="82"/>
-      <c r="T23" s="83"/>
-      <c r="U23" s="84" t="s">
+      <c r="S23" s="86"/>
+      <c r="T23" s="95"/>
+      <c r="U23" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="V23" s="85"/>
-      <c r="W23" s="85"/>
+      <c r="V23" s="97"/>
+      <c r="W23" s="97"/>
       <c r="X23" s="39"/>
       <c r="Y23" s="35" t="b">
         <v>1</v>
@@ -3351,10 +4258,10 @@
       <c r="D24" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E24" s="81" t="s">
+      <c r="E24" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="82"/>
+      <c r="F24" s="86"/>
       <c r="G24" s="39"/>
       <c r="H24" s="13">
         <v>0</v>
@@ -3386,16 +4293,16 @@
       <c r="Q24" s="12">
         <v>0</v>
       </c>
-      <c r="R24" s="81" t="s">
+      <c r="R24" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S24" s="82"/>
-      <c r="T24" s="83"/>
-      <c r="U24" s="84" t="s">
+      <c r="S24" s="86"/>
+      <c r="T24" s="95"/>
+      <c r="U24" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="V24" s="85"/>
-      <c r="W24" s="85"/>
+      <c r="V24" s="97"/>
+      <c r="W24" s="97"/>
       <c r="X24" s="39"/>
       <c r="Y24" s="36" t="b">
         <v>1</v>
@@ -3458,16 +4365,16 @@
       <c r="Q25" s="32">
         <v>1</v>
       </c>
-      <c r="R25" s="81" t="s">
+      <c r="R25" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="S25" s="82"/>
-      <c r="T25" s="83"/>
-      <c r="U25" s="84" t="s">
+      <c r="S25" s="86"/>
+      <c r="T25" s="95"/>
+      <c r="U25" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="V25" s="85"/>
-      <c r="W25" s="85"/>
+      <c r="V25" s="97"/>
+      <c r="W25" s="97"/>
       <c r="X25" s="39"/>
       <c r="Y25" s="35" t="b">
         <v>1</v>
@@ -3493,10 +4400,10 @@
       <c r="D26" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="81" t="s">
+      <c r="E26" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="82"/>
+      <c r="F26" s="86"/>
       <c r="G26" s="39"/>
       <c r="H26" s="13">
         <v>0</v>
@@ -3528,16 +4435,16 @@
       <c r="Q26" s="12">
         <v>0</v>
       </c>
-      <c r="R26" s="81" t="s">
+      <c r="R26" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S26" s="82"/>
-      <c r="T26" s="83"/>
-      <c r="U26" s="84" t="s">
+      <c r="S26" s="86"/>
+      <c r="T26" s="95"/>
+      <c r="U26" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="V26" s="85"/>
-      <c r="W26" s="85"/>
+      <c r="V26" s="97"/>
+      <c r="W26" s="97"/>
       <c r="X26" s="39"/>
       <c r="Y26" s="36" t="b">
         <v>1</v>
@@ -3563,10 +4470,10 @@
       <c r="D27" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="81" t="s">
+      <c r="E27" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="82"/>
+      <c r="F27" s="86"/>
       <c r="G27" s="39"/>
       <c r="H27" s="41">
         <v>0</v>
@@ -3598,16 +4505,16 @@
       <c r="Q27" s="32">
         <v>1</v>
       </c>
-      <c r="R27" s="81" t="s">
+      <c r="R27" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S27" s="82"/>
-      <c r="T27" s="83"/>
-      <c r="U27" s="84" t="s">
+      <c r="S27" s="86"/>
+      <c r="T27" s="95"/>
+      <c r="U27" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="V27" s="85"/>
-      <c r="W27" s="85"/>
+      <c r="V27" s="97"/>
+      <c r="W27" s="97"/>
       <c r="X27" s="39"/>
       <c r="Y27" s="35" t="b">
         <v>1</v>
@@ -3633,10 +4540,10 @@
       <c r="D28" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="81" t="s">
+      <c r="E28" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="82"/>
+      <c r="F28" s="86"/>
       <c r="G28" s="39"/>
       <c r="H28" s="13">
         <v>0</v>
@@ -3668,16 +4575,16 @@
       <c r="Q28" s="12">
         <v>0</v>
       </c>
-      <c r="R28" s="81" t="s">
+      <c r="R28" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S28" s="82"/>
-      <c r="T28" s="83"/>
-      <c r="U28" s="84" t="s">
+      <c r="S28" s="86"/>
+      <c r="T28" s="95"/>
+      <c r="U28" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="V28" s="85"/>
-      <c r="W28" s="85"/>
+      <c r="V28" s="97"/>
+      <c r="W28" s="97"/>
       <c r="X28" s="39"/>
       <c r="Y28" s="36" t="b">
         <v>1</v>
@@ -3740,16 +4647,16 @@
       <c r="Q29" s="32">
         <v>1</v>
       </c>
-      <c r="R29" s="81" t="s">
+      <c r="R29" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="S29" s="82"/>
-      <c r="T29" s="83"/>
-      <c r="U29" s="101" t="s">
+      <c r="S29" s="86"/>
+      <c r="T29" s="95"/>
+      <c r="U29" s="98" t="s">
         <v>125</v>
       </c>
-      <c r="V29" s="102"/>
-      <c r="W29" s="102"/>
+      <c r="V29" s="99"/>
+      <c r="W29" s="99"/>
       <c r="X29" s="39"/>
       <c r="Y29" s="35" t="b">
         <v>0</v>
@@ -3775,10 +4682,10 @@
       <c r="D30" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="81" t="s">
+      <c r="E30" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="82"/>
+      <c r="F30" s="86"/>
       <c r="G30" s="39"/>
       <c r="H30" s="13">
         <v>0</v>
@@ -3810,16 +4717,16 @@
       <c r="Q30" s="12">
         <v>0</v>
       </c>
-      <c r="R30" s="81" t="s">
+      <c r="R30" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S30" s="82"/>
-      <c r="T30" s="83"/>
-      <c r="U30" s="84" t="s">
+      <c r="S30" s="86"/>
+      <c r="T30" s="95"/>
+      <c r="U30" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="V30" s="85"/>
-      <c r="W30" s="85"/>
+      <c r="V30" s="97"/>
+      <c r="W30" s="97"/>
       <c r="X30" s="39"/>
       <c r="Y30" s="36" t="b">
         <v>1</v>
@@ -3845,10 +4752,10 @@
       <c r="D31" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="E31" s="81" t="s">
+      <c r="E31" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="82"/>
+      <c r="F31" s="86"/>
       <c r="G31" s="39"/>
       <c r="H31" s="41">
         <v>0</v>
@@ -3880,16 +4787,16 @@
       <c r="Q31" s="32">
         <v>1</v>
       </c>
-      <c r="R31" s="81" t="s">
+      <c r="R31" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="S31" s="82"/>
-      <c r="T31" s="83"/>
-      <c r="U31" s="84" t="s">
+      <c r="S31" s="86"/>
+      <c r="T31" s="95"/>
+      <c r="U31" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="V31" s="85"/>
-      <c r="W31" s="85"/>
+      <c r="V31" s="97"/>
+      <c r="W31" s="97"/>
       <c r="X31" s="39"/>
       <c r="Y31" s="35" t="b">
         <v>1</v>
@@ -3910,9 +4817,9 @@
       </c>
       <c r="B32" s="45"/>
       <c r="C32" s="34"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="77"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
       <c r="G32" s="38"/>
       <c r="H32" s="15">
         <v>1</v>
@@ -3926,20 +4833,20 @@
       <c r="K32" s="4">
         <v>1</v>
       </c>
-      <c r="L32" s="74" t="s">
+      <c r="L32" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="M32" s="77"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="73"/>
-      <c r="P32" s="73"/>
-      <c r="Q32" s="73"/>
-      <c r="R32" s="73"/>
-      <c r="S32" s="73"/>
-      <c r="T32" s="73"/>
-      <c r="U32" s="73"/>
-      <c r="V32" s="73"/>
-      <c r="W32" s="73"/>
+      <c r="M32" s="83"/>
+      <c r="N32" s="83"/>
+      <c r="O32" s="84"/>
+      <c r="P32" s="84"/>
+      <c r="Q32" s="84"/>
+      <c r="R32" s="84"/>
+      <c r="S32" s="84"/>
+      <c r="T32" s="84"/>
+      <c r="U32" s="84"/>
+      <c r="V32" s="84"/>
+      <c r="W32" s="84"/>
       <c r="X32" s="38"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="1"/>
@@ -3957,10 +4864,10 @@
       <c r="D33" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="88" t="s">
+      <c r="E33" s="75" t="s">
         <v>115</v>
       </c>
-      <c r="F33" s="89"/>
+      <c r="F33" s="76"/>
       <c r="G33" s="39"/>
       <c r="H33" s="16">
         <v>1</v>
@@ -3977,21 +4884,21 @@
       <c r="L33" s="26">
         <v>0</v>
       </c>
-      <c r="M33" s="95" t="s">
+      <c r="M33" s="100" t="s">
         <v>102</v>
       </c>
-      <c r="N33" s="96"/>
-      <c r="O33" s="97"/>
-      <c r="P33" s="88" t="s">
+      <c r="N33" s="101"/>
+      <c r="O33" s="102"/>
+      <c r="P33" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q33" s="89"/>
-      <c r="R33" s="89"/>
-      <c r="S33" s="89"/>
-      <c r="T33" s="89"/>
-      <c r="U33" s="89"/>
-      <c r="V33" s="89"/>
-      <c r="W33" s="89"/>
+      <c r="Q33" s="76"/>
+      <c r="R33" s="76"/>
+      <c r="S33" s="76"/>
+      <c r="T33" s="76"/>
+      <c r="U33" s="76"/>
+      <c r="V33" s="76"/>
+      <c r="W33" s="76"/>
       <c r="X33" s="39"/>
       <c r="Y33" s="35" t="b">
         <v>0</v>
@@ -4017,10 +4924,10 @@
       <c r="D34" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="E34" s="88" t="s">
+      <c r="E34" s="75" t="s">
         <v>115</v>
       </c>
-      <c r="F34" s="89"/>
+      <c r="F34" s="76"/>
       <c r="G34" s="39"/>
       <c r="H34" s="16">
         <v>1</v>
@@ -4037,21 +4944,21 @@
       <c r="L34" s="5">
         <v>1</v>
       </c>
-      <c r="M34" s="95" t="s">
+      <c r="M34" s="100" t="s">
         <v>102</v>
       </c>
-      <c r="N34" s="96"/>
-      <c r="O34" s="97"/>
-      <c r="P34" s="88" t="s">
+      <c r="N34" s="101"/>
+      <c r="O34" s="102"/>
+      <c r="P34" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q34" s="89"/>
-      <c r="R34" s="89"/>
-      <c r="S34" s="89"/>
-      <c r="T34" s="89"/>
-      <c r="U34" s="89"/>
-      <c r="V34" s="89"/>
-      <c r="W34" s="89"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="76"/>
+      <c r="S34" s="76"/>
+      <c r="T34" s="76"/>
+      <c r="U34" s="76"/>
+      <c r="V34" s="76"/>
+      <c r="W34" s="76"/>
       <c r="X34" s="39"/>
       <c r="Y34" s="36" t="b">
         <v>0</v>
@@ -4073,8 +4980,8 @@
       <c r="B35" s="45"/>
       <c r="C35" s="34"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="74"/>
-      <c r="F35" s="77"/>
+      <c r="E35" s="82"/>
+      <c r="F35" s="83"/>
       <c r="G35" s="38"/>
       <c r="H35" s="15">
         <v>1</v>
@@ -4088,20 +4995,20 @@
       <c r="K35" s="4">
         <v>1</v>
       </c>
-      <c r="L35" s="74" t="s">
+      <c r="L35" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="M35" s="77"/>
-      <c r="N35" s="77"/>
-      <c r="O35" s="77"/>
-      <c r="P35" s="77"/>
-      <c r="Q35" s="77"/>
-      <c r="R35" s="75"/>
-      <c r="S35" s="73"/>
-      <c r="T35" s="73"/>
-      <c r="U35" s="73"/>
-      <c r="V35" s="73"/>
-      <c r="W35" s="73"/>
+      <c r="M35" s="83"/>
+      <c r="N35" s="83"/>
+      <c r="O35" s="83"/>
+      <c r="P35" s="83"/>
+      <c r="Q35" s="83"/>
+      <c r="R35" s="103"/>
+      <c r="S35" s="84"/>
+      <c r="T35" s="84"/>
+      <c r="U35" s="84"/>
+      <c r="V35" s="84"/>
+      <c r="W35" s="84"/>
       <c r="X35" s="38"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="1"/>
@@ -4119,10 +5026,10 @@
       <c r="D36" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="103" t="s">
+      <c r="E36" s="90" t="s">
         <v>116</v>
       </c>
-      <c r="F36" s="104"/>
+      <c r="F36" s="91"/>
       <c r="G36" s="39"/>
       <c r="H36" s="16">
         <v>1</v>
@@ -4151,15 +5058,15 @@
       <c r="P36" s="5">
         <v>0</v>
       </c>
-      <c r="Q36" s="88" t="s">
+      <c r="Q36" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="R36" s="89"/>
-      <c r="S36" s="89"/>
-      <c r="T36" s="89"/>
-      <c r="U36" s="89"/>
-      <c r="V36" s="89"/>
-      <c r="W36" s="89"/>
+      <c r="R36" s="76"/>
+      <c r="S36" s="76"/>
+      <c r="T36" s="76"/>
+      <c r="U36" s="76"/>
+      <c r="V36" s="76"/>
+      <c r="W36" s="76"/>
       <c r="X36" s="39"/>
       <c r="Y36" s="36" t="b">
         <v>0</v>
@@ -4185,10 +5092,10 @@
       <c r="D37" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E37" s="103" t="s">
+      <c r="E37" s="90" t="s">
         <v>116</v>
       </c>
-      <c r="F37" s="104"/>
+      <c r="F37" s="91"/>
       <c r="G37" s="39"/>
       <c r="H37" s="16">
         <v>1</v>
@@ -4217,15 +5124,15 @@
       <c r="P37" s="26">
         <v>1</v>
       </c>
-      <c r="Q37" s="88" t="s">
+      <c r="Q37" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="R37" s="89"/>
-      <c r="S37" s="89"/>
-      <c r="T37" s="89"/>
-      <c r="U37" s="89"/>
-      <c r="V37" s="89"/>
-      <c r="W37" s="89"/>
+      <c r="R37" s="76"/>
+      <c r="S37" s="76"/>
+      <c r="T37" s="76"/>
+      <c r="U37" s="76"/>
+      <c r="V37" s="76"/>
+      <c r="W37" s="76"/>
       <c r="X37" s="39"/>
       <c r="Y37" s="35" t="b">
         <v>0</v>
@@ -4246,9 +5153,9 @@
       </c>
       <c r="B38" s="45"/>
       <c r="C38" s="34"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="77"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="83"/>
       <c r="G38" s="38"/>
       <c r="H38" s="42">
         <v>1</v>
@@ -4262,12 +5169,12 @@
       <c r="K38" s="21">
         <v>1</v>
       </c>
-      <c r="L38" s="73" t="s">
+      <c r="L38" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="M38" s="73"/>
-      <c r="N38" s="73"/>
-      <c r="O38" s="73"/>
+      <c r="M38" s="84"/>
+      <c r="N38" s="84"/>
+      <c r="O38" s="84"/>
       <c r="P38" s="65"/>
       <c r="Q38" s="65"/>
       <c r="R38" s="65"/>
@@ -4293,10 +5200,10 @@
       <c r="D39" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E39" s="68" t="s">
+      <c r="E39" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F39" s="69"/>
+      <c r="F39" s="78"/>
       <c r="G39" s="39"/>
       <c r="H39" s="16">
         <v>1</v>
@@ -4310,29 +5217,29 @@
       <c r="K39" s="10">
         <v>1</v>
       </c>
-      <c r="L39" s="98" t="s">
+      <c r="L39" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M39" s="99"/>
-      <c r="N39" s="99"/>
-      <c r="O39" s="100"/>
-      <c r="P39" s="88" t="s">
+      <c r="M39" s="93"/>
+      <c r="N39" s="93"/>
+      <c r="O39" s="94"/>
+      <c r="P39" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q39" s="89"/>
-      <c r="R39" s="89"/>
-      <c r="S39" s="89"/>
-      <c r="T39" s="89"/>
-      <c r="U39" s="89"/>
-      <c r="V39" s="89"/>
-      <c r="W39" s="89"/>
+      <c r="Q39" s="76"/>
+      <c r="R39" s="76"/>
+      <c r="S39" s="76"/>
+      <c r="T39" s="76"/>
+      <c r="U39" s="76"/>
+      <c r="V39" s="76"/>
+      <c r="W39" s="76"/>
       <c r="X39" s="39"/>
-      <c r="Y39" s="105" t="s">
+      <c r="Y39" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="Z39" s="106"/>
-      <c r="AA39" s="106"/>
-      <c r="AB39" s="107"/>
+      <c r="Z39" s="70"/>
+      <c r="AA39" s="70"/>
+      <c r="AB39" s="71"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" s="51" t="s">
@@ -4345,10 +5252,10 @@
       <c r="D40" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E40" s="68" t="s">
+      <c r="E40" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F40" s="69"/>
+      <c r="F40" s="78"/>
       <c r="G40" s="39"/>
       <c r="H40" s="16">
         <v>1</v>
@@ -4362,29 +5269,29 @@
       <c r="K40" s="10">
         <v>1</v>
       </c>
-      <c r="L40" s="98" t="s">
+      <c r="L40" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M40" s="99"/>
-      <c r="N40" s="99"/>
-      <c r="O40" s="100"/>
-      <c r="P40" s="88" t="s">
+      <c r="M40" s="93"/>
+      <c r="N40" s="93"/>
+      <c r="O40" s="94"/>
+      <c r="P40" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q40" s="89"/>
-      <c r="R40" s="89"/>
-      <c r="S40" s="89"/>
-      <c r="T40" s="89"/>
-      <c r="U40" s="89"/>
-      <c r="V40" s="89"/>
-      <c r="W40" s="89"/>
+      <c r="Q40" s="76"/>
+      <c r="R40" s="76"/>
+      <c r="S40" s="76"/>
+      <c r="T40" s="76"/>
+      <c r="U40" s="76"/>
+      <c r="V40" s="76"/>
+      <c r="W40" s="76"/>
       <c r="X40" s="39"/>
-      <c r="Y40" s="108" t="s">
+      <c r="Y40" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="Z40" s="109"/>
-      <c r="AA40" s="109"/>
-      <c r="AB40" s="110"/>
+      <c r="Z40" s="73"/>
+      <c r="AA40" s="73"/>
+      <c r="AB40" s="74"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" s="53" t="s">
@@ -4397,10 +5304,10 @@
       <c r="D41" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E41" s="68" t="s">
+      <c r="E41" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F41" s="69"/>
+      <c r="F41" s="78"/>
       <c r="G41" s="39"/>
       <c r="H41" s="16">
         <v>1</v>
@@ -4414,29 +5321,29 @@
       <c r="K41" s="10">
         <v>1</v>
       </c>
-      <c r="L41" s="98" t="s">
+      <c r="L41" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M41" s="99"/>
-      <c r="N41" s="99"/>
-      <c r="O41" s="100"/>
-      <c r="P41" s="88" t="s">
+      <c r="M41" s="93"/>
+      <c r="N41" s="93"/>
+      <c r="O41" s="94"/>
+      <c r="P41" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q41" s="89"/>
-      <c r="R41" s="89"/>
-      <c r="S41" s="89"/>
-      <c r="T41" s="89"/>
-      <c r="U41" s="89"/>
-      <c r="V41" s="89"/>
-      <c r="W41" s="89"/>
+      <c r="Q41" s="76"/>
+      <c r="R41" s="76"/>
+      <c r="S41" s="76"/>
+      <c r="T41" s="76"/>
+      <c r="U41" s="76"/>
+      <c r="V41" s="76"/>
+      <c r="W41" s="76"/>
       <c r="X41" s="39"/>
-      <c r="Y41" s="105" t="s">
+      <c r="Y41" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="Z41" s="106"/>
-      <c r="AA41" s="106"/>
-      <c r="AB41" s="107"/>
+      <c r="Z41" s="70"/>
+      <c r="AA41" s="70"/>
+      <c r="AB41" s="71"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="51" t="s">
@@ -4449,10 +5356,10 @@
       <c r="D42" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E42" s="68" t="s">
+      <c r="E42" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F42" s="69"/>
+      <c r="F42" s="78"/>
       <c r="G42" s="39"/>
       <c r="H42" s="16">
         <v>1</v>
@@ -4466,29 +5373,29 @@
       <c r="K42" s="10">
         <v>1</v>
       </c>
-      <c r="L42" s="98" t="s">
+      <c r="L42" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M42" s="99"/>
-      <c r="N42" s="99"/>
-      <c r="O42" s="100"/>
-      <c r="P42" s="88" t="s">
+      <c r="M42" s="93"/>
+      <c r="N42" s="93"/>
+      <c r="O42" s="94"/>
+      <c r="P42" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q42" s="89"/>
-      <c r="R42" s="89"/>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
-      <c r="V42" s="89"/>
-      <c r="W42" s="89"/>
+      <c r="Q42" s="76"/>
+      <c r="R42" s="76"/>
+      <c r="S42" s="76"/>
+      <c r="T42" s="76"/>
+      <c r="U42" s="76"/>
+      <c r="V42" s="76"/>
+      <c r="W42" s="76"/>
       <c r="X42" s="39"/>
-      <c r="Y42" s="108" t="s">
+      <c r="Y42" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="Z42" s="109"/>
-      <c r="AA42" s="109"/>
-      <c r="AB42" s="110"/>
+      <c r="Z42" s="73"/>
+      <c r="AA42" s="73"/>
+      <c r="AB42" s="74"/>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" s="53" t="s">
@@ -4501,10 +5408,10 @@
       <c r="D43" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E43" s="68" t="s">
+      <c r="E43" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F43" s="69"/>
+      <c r="F43" s="78"/>
       <c r="G43" s="39"/>
       <c r="H43" s="16">
         <v>1</v>
@@ -4518,29 +5425,29 @@
       <c r="K43" s="10">
         <v>1</v>
       </c>
-      <c r="L43" s="98" t="s">
+      <c r="L43" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M43" s="99"/>
-      <c r="N43" s="99"/>
-      <c r="O43" s="100"/>
-      <c r="P43" s="88" t="s">
+      <c r="M43" s="93"/>
+      <c r="N43" s="93"/>
+      <c r="O43" s="94"/>
+      <c r="P43" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q43" s="89"/>
-      <c r="R43" s="89"/>
-      <c r="S43" s="89"/>
-      <c r="T43" s="89"/>
-      <c r="U43" s="89"/>
-      <c r="V43" s="89"/>
-      <c r="W43" s="89"/>
+      <c r="Q43" s="76"/>
+      <c r="R43" s="76"/>
+      <c r="S43" s="76"/>
+      <c r="T43" s="76"/>
+      <c r="U43" s="76"/>
+      <c r="V43" s="76"/>
+      <c r="W43" s="76"/>
       <c r="X43" s="39"/>
-      <c r="Y43" s="105" t="s">
+      <c r="Y43" s="69" t="s">
         <v>131</v>
       </c>
-      <c r="Z43" s="106"/>
-      <c r="AA43" s="106"/>
-      <c r="AB43" s="107"/>
+      <c r="Z43" s="70"/>
+      <c r="AA43" s="70"/>
+      <c r="AB43" s="71"/>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" s="51" t="s">
@@ -4553,10 +5460,10 @@
       <c r="D44" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E44" s="68" t="s">
+      <c r="E44" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F44" s="69"/>
+      <c r="F44" s="78"/>
       <c r="G44" s="39"/>
       <c r="H44" s="16">
         <v>1</v>
@@ -4570,29 +5477,29 @@
       <c r="K44" s="10">
         <v>1</v>
       </c>
-      <c r="L44" s="98" t="s">
+      <c r="L44" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M44" s="99"/>
-      <c r="N44" s="99"/>
-      <c r="O44" s="100"/>
-      <c r="P44" s="88" t="s">
+      <c r="M44" s="93"/>
+      <c r="N44" s="93"/>
+      <c r="O44" s="94"/>
+      <c r="P44" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q44" s="89"/>
-      <c r="R44" s="89"/>
-      <c r="S44" s="89"/>
-      <c r="T44" s="89"/>
-      <c r="U44" s="89"/>
-      <c r="V44" s="89"/>
-      <c r="W44" s="89"/>
+      <c r="Q44" s="76"/>
+      <c r="R44" s="76"/>
+      <c r="S44" s="76"/>
+      <c r="T44" s="76"/>
+      <c r="U44" s="76"/>
+      <c r="V44" s="76"/>
+      <c r="W44" s="76"/>
       <c r="X44" s="39"/>
-      <c r="Y44" s="108" t="s">
+      <c r="Y44" s="72" t="s">
         <v>132</v>
       </c>
-      <c r="Z44" s="109"/>
-      <c r="AA44" s="109"/>
-      <c r="AB44" s="110"/>
+      <c r="Z44" s="73"/>
+      <c r="AA44" s="73"/>
+      <c r="AB44" s="74"/>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" s="53" t="s">
@@ -4605,10 +5512,10 @@
       <c r="D45" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E45" s="68" t="s">
+      <c r="E45" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F45" s="69"/>
+      <c r="F45" s="78"/>
       <c r="G45" s="39"/>
       <c r="H45" s="16">
         <v>1</v>
@@ -4622,29 +5529,29 @@
       <c r="K45" s="10">
         <v>1</v>
       </c>
-      <c r="L45" s="98" t="s">
+      <c r="L45" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M45" s="99"/>
-      <c r="N45" s="99"/>
-      <c r="O45" s="100"/>
-      <c r="P45" s="88" t="s">
+      <c r="M45" s="93"/>
+      <c r="N45" s="93"/>
+      <c r="O45" s="94"/>
+      <c r="P45" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q45" s="89"/>
-      <c r="R45" s="89"/>
-      <c r="S45" s="89"/>
-      <c r="T45" s="89"/>
-      <c r="U45" s="89"/>
-      <c r="V45" s="89"/>
-      <c r="W45" s="89"/>
+      <c r="Q45" s="76"/>
+      <c r="R45" s="76"/>
+      <c r="S45" s="76"/>
+      <c r="T45" s="76"/>
+      <c r="U45" s="76"/>
+      <c r="V45" s="76"/>
+      <c r="W45" s="76"/>
       <c r="X45" s="39"/>
-      <c r="Y45" s="105" t="s">
+      <c r="Y45" s="69" t="s">
         <v>133</v>
       </c>
-      <c r="Z45" s="106"/>
-      <c r="AA45" s="106"/>
-      <c r="AB45" s="107"/>
+      <c r="Z45" s="70"/>
+      <c r="AA45" s="70"/>
+      <c r="AB45" s="71"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" s="51" t="s">
@@ -4657,10 +5564,10 @@
       <c r="D46" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E46" s="68" t="s">
+      <c r="E46" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F46" s="69"/>
+      <c r="F46" s="78"/>
       <c r="G46" s="39"/>
       <c r="H46" s="16">
         <v>1</v>
@@ -4674,29 +5581,29 @@
       <c r="K46" s="10">
         <v>1</v>
       </c>
-      <c r="L46" s="98" t="s">
+      <c r="L46" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M46" s="99"/>
-      <c r="N46" s="99"/>
-      <c r="O46" s="100"/>
-      <c r="P46" s="88" t="s">
+      <c r="M46" s="93"/>
+      <c r="N46" s="93"/>
+      <c r="O46" s="94"/>
+      <c r="P46" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q46" s="89"/>
-      <c r="R46" s="89"/>
-      <c r="S46" s="89"/>
-      <c r="T46" s="89"/>
-      <c r="U46" s="89"/>
-      <c r="V46" s="89"/>
-      <c r="W46" s="89"/>
+      <c r="Q46" s="76"/>
+      <c r="R46" s="76"/>
+      <c r="S46" s="76"/>
+      <c r="T46" s="76"/>
+      <c r="U46" s="76"/>
+      <c r="V46" s="76"/>
+      <c r="W46" s="76"/>
       <c r="X46" s="39"/>
-      <c r="Y46" s="108" t="s">
+      <c r="Y46" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="Z46" s="109"/>
-      <c r="AA46" s="109"/>
-      <c r="AB46" s="110"/>
+      <c r="Z46" s="73"/>
+      <c r="AA46" s="73"/>
+      <c r="AB46" s="74"/>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" s="53" t="s">
@@ -4709,10 +5616,10 @@
       <c r="D47" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E47" s="68" t="s">
+      <c r="E47" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F47" s="69"/>
+      <c r="F47" s="78"/>
       <c r="G47" s="39"/>
       <c r="H47" s="16">
         <v>1</v>
@@ -4726,29 +5633,29 @@
       <c r="K47" s="10">
         <v>1</v>
       </c>
-      <c r="L47" s="98" t="s">
+      <c r="L47" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M47" s="99"/>
-      <c r="N47" s="99"/>
-      <c r="O47" s="100"/>
-      <c r="P47" s="88" t="s">
+      <c r="M47" s="93"/>
+      <c r="N47" s="93"/>
+      <c r="O47" s="94"/>
+      <c r="P47" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q47" s="89"/>
-      <c r="R47" s="89"/>
-      <c r="S47" s="89"/>
-      <c r="T47" s="89"/>
-      <c r="U47" s="89"/>
-      <c r="V47" s="89"/>
-      <c r="W47" s="89"/>
+      <c r="Q47" s="76"/>
+      <c r="R47" s="76"/>
+      <c r="S47" s="76"/>
+      <c r="T47" s="76"/>
+      <c r="U47" s="76"/>
+      <c r="V47" s="76"/>
+      <c r="W47" s="76"/>
       <c r="X47" s="39"/>
-      <c r="Y47" s="105" t="s">
+      <c r="Y47" s="69" t="s">
         <v>135</v>
       </c>
-      <c r="Z47" s="106"/>
-      <c r="AA47" s="106"/>
-      <c r="AB47" s="107"/>
+      <c r="Z47" s="70"/>
+      <c r="AA47" s="70"/>
+      <c r="AB47" s="71"/>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A48" s="51" t="s">
@@ -4761,10 +5668,10 @@
       <c r="D48" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E48" s="68" t="s">
+      <c r="E48" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F48" s="69"/>
+      <c r="F48" s="78"/>
       <c r="G48" s="39"/>
       <c r="H48" s="16">
         <v>1</v>
@@ -4778,29 +5685,29 @@
       <c r="K48" s="10">
         <v>1</v>
       </c>
-      <c r="L48" s="98" t="s">
+      <c r="L48" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M48" s="99"/>
-      <c r="N48" s="99"/>
-      <c r="O48" s="100"/>
-      <c r="P48" s="88" t="s">
+      <c r="M48" s="93"/>
+      <c r="N48" s="93"/>
+      <c r="O48" s="94"/>
+      <c r="P48" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q48" s="89"/>
-      <c r="R48" s="89"/>
-      <c r="S48" s="89"/>
-      <c r="T48" s="89"/>
-      <c r="U48" s="89"/>
-      <c r="V48" s="89"/>
-      <c r="W48" s="89"/>
+      <c r="Q48" s="76"/>
+      <c r="R48" s="76"/>
+      <c r="S48" s="76"/>
+      <c r="T48" s="76"/>
+      <c r="U48" s="76"/>
+      <c r="V48" s="76"/>
+      <c r="W48" s="76"/>
       <c r="X48" s="39"/>
-      <c r="Y48" s="108" t="s">
+      <c r="Y48" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="Z48" s="109"/>
-      <c r="AA48" s="109"/>
-      <c r="AB48" s="110"/>
+      <c r="Z48" s="73"/>
+      <c r="AA48" s="73"/>
+      <c r="AB48" s="74"/>
     </row>
     <row r="49" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A49" s="53" t="s">
@@ -4813,10 +5720,10 @@
       <c r="D49" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E49" s="68" t="s">
+      <c r="E49" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F49" s="69"/>
+      <c r="F49" s="78"/>
       <c r="G49" s="39"/>
       <c r="H49" s="16">
         <v>1</v>
@@ -4830,29 +5737,29 @@
       <c r="K49" s="10">
         <v>1</v>
       </c>
-      <c r="L49" s="98" t="s">
+      <c r="L49" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M49" s="99"/>
-      <c r="N49" s="99"/>
-      <c r="O49" s="100"/>
-      <c r="P49" s="88" t="s">
+      <c r="M49" s="93"/>
+      <c r="N49" s="93"/>
+      <c r="O49" s="94"/>
+      <c r="P49" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q49" s="89"/>
-      <c r="R49" s="89"/>
-      <c r="S49" s="89"/>
-      <c r="T49" s="89"/>
-      <c r="U49" s="89"/>
-      <c r="V49" s="89"/>
-      <c r="W49" s="89"/>
+      <c r="Q49" s="76"/>
+      <c r="R49" s="76"/>
+      <c r="S49" s="76"/>
+      <c r="T49" s="76"/>
+      <c r="U49" s="76"/>
+      <c r="V49" s="76"/>
+      <c r="W49" s="76"/>
       <c r="X49" s="39"/>
-      <c r="Y49" s="105" t="s">
+      <c r="Y49" s="69" t="s">
         <v>137</v>
       </c>
-      <c r="Z49" s="106"/>
-      <c r="AA49" s="106"/>
-      <c r="AB49" s="107"/>
+      <c r="Z49" s="70"/>
+      <c r="AA49" s="70"/>
+      <c r="AB49" s="71"/>
       <c r="AP49" s="9" t="s">
         <v>126</v>
       </c>
@@ -4868,10 +5775,10 @@
       <c r="D50" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E50" s="68" t="s">
+      <c r="E50" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F50" s="69"/>
+      <c r="F50" s="78"/>
       <c r="G50" s="39"/>
       <c r="H50" s="16">
         <v>1</v>
@@ -4885,29 +5792,29 @@
       <c r="K50" s="10">
         <v>1</v>
       </c>
-      <c r="L50" s="98" t="s">
+      <c r="L50" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M50" s="99"/>
-      <c r="N50" s="99"/>
-      <c r="O50" s="100"/>
-      <c r="P50" s="88" t="s">
+      <c r="M50" s="93"/>
+      <c r="N50" s="93"/>
+      <c r="O50" s="94"/>
+      <c r="P50" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q50" s="89"/>
-      <c r="R50" s="89"/>
-      <c r="S50" s="89"/>
-      <c r="T50" s="89"/>
-      <c r="U50" s="89"/>
-      <c r="V50" s="89"/>
-      <c r="W50" s="89"/>
+      <c r="Q50" s="76"/>
+      <c r="R50" s="76"/>
+      <c r="S50" s="76"/>
+      <c r="T50" s="76"/>
+      <c r="U50" s="76"/>
+      <c r="V50" s="76"/>
+      <c r="W50" s="76"/>
       <c r="X50" s="39"/>
-      <c r="Y50" s="108" t="s">
+      <c r="Y50" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="Z50" s="109"/>
-      <c r="AA50" s="109"/>
-      <c r="AB50" s="110"/>
+      <c r="Z50" s="73"/>
+      <c r="AA50" s="73"/>
+      <c r="AB50" s="74"/>
     </row>
     <row r="51" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A51" s="53" t="s">
@@ -4920,10 +5827,10 @@
       <c r="D51" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E51" s="68" t="s">
+      <c r="E51" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F51" s="69"/>
+      <c r="F51" s="78"/>
       <c r="G51" s="39"/>
       <c r="H51" s="16">
         <v>1</v>
@@ -4937,29 +5844,29 @@
       <c r="K51" s="10">
         <v>1</v>
       </c>
-      <c r="L51" s="98" t="s">
+      <c r="L51" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M51" s="99"/>
-      <c r="N51" s="99"/>
-      <c r="O51" s="100"/>
-      <c r="P51" s="88" t="s">
+      <c r="M51" s="93"/>
+      <c r="N51" s="93"/>
+      <c r="O51" s="94"/>
+      <c r="P51" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q51" s="89"/>
-      <c r="R51" s="89"/>
-      <c r="S51" s="89"/>
-      <c r="T51" s="89"/>
-      <c r="U51" s="89"/>
-      <c r="V51" s="89"/>
-      <c r="W51" s="89"/>
+      <c r="Q51" s="76"/>
+      <c r="R51" s="76"/>
+      <c r="S51" s="76"/>
+      <c r="T51" s="76"/>
+      <c r="U51" s="76"/>
+      <c r="V51" s="76"/>
+      <c r="W51" s="76"/>
       <c r="X51" s="39"/>
-      <c r="Y51" s="105" t="s">
+      <c r="Y51" s="69" t="s">
         <v>139</v>
       </c>
-      <c r="Z51" s="106"/>
-      <c r="AA51" s="106"/>
-      <c r="AB51" s="107"/>
+      <c r="Z51" s="70"/>
+      <c r="AA51" s="70"/>
+      <c r="AB51" s="71"/>
     </row>
     <row r="52" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A52" s="51" t="s">
@@ -4972,10 +5879,10 @@
       <c r="D52" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E52" s="68" t="s">
+      <c r="E52" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F52" s="69"/>
+      <c r="F52" s="78"/>
       <c r="G52" s="39"/>
       <c r="H52" s="16">
         <v>1</v>
@@ -4989,29 +5896,29 @@
       <c r="K52" s="10">
         <v>1</v>
       </c>
-      <c r="L52" s="98" t="s">
+      <c r="L52" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M52" s="99"/>
-      <c r="N52" s="99"/>
-      <c r="O52" s="100"/>
-      <c r="P52" s="88" t="s">
+      <c r="M52" s="93"/>
+      <c r="N52" s="93"/>
+      <c r="O52" s="94"/>
+      <c r="P52" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q52" s="89"/>
-      <c r="R52" s="89"/>
-      <c r="S52" s="89"/>
-      <c r="T52" s="89"/>
-      <c r="U52" s="89"/>
-      <c r="V52" s="89"/>
-      <c r="W52" s="89"/>
+      <c r="Q52" s="76"/>
+      <c r="R52" s="76"/>
+      <c r="S52" s="76"/>
+      <c r="T52" s="76"/>
+      <c r="U52" s="76"/>
+      <c r="V52" s="76"/>
+      <c r="W52" s="76"/>
       <c r="X52" s="39"/>
-      <c r="Y52" s="108" t="s">
+      <c r="Y52" s="72" t="s">
         <v>140</v>
       </c>
-      <c r="Z52" s="109"/>
-      <c r="AA52" s="109"/>
-      <c r="AB52" s="110"/>
+      <c r="Z52" s="73"/>
+      <c r="AA52" s="73"/>
+      <c r="AB52" s="74"/>
     </row>
     <row r="53" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A53" s="53" t="s">
@@ -5024,10 +5931,10 @@
       <c r="D53" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E53" s="68" t="s">
+      <c r="E53" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F53" s="69"/>
+      <c r="F53" s="78"/>
       <c r="G53" s="39"/>
       <c r="H53" s="16">
         <v>1</v>
@@ -5041,22 +5948,22 @@
       <c r="K53" s="10">
         <v>1</v>
       </c>
-      <c r="L53" s="98" t="s">
+      <c r="L53" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="M53" s="99"/>
-      <c r="N53" s="99"/>
-      <c r="O53" s="100"/>
-      <c r="P53" s="88" t="s">
+      <c r="M53" s="93"/>
+      <c r="N53" s="93"/>
+      <c r="O53" s="94"/>
+      <c r="P53" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="Q53" s="89"/>
-      <c r="R53" s="89"/>
-      <c r="S53" s="89"/>
-      <c r="T53" s="89"/>
-      <c r="U53" s="89"/>
-      <c r="V53" s="89"/>
-      <c r="W53" s="89"/>
+      <c r="Q53" s="76"/>
+      <c r="R53" s="76"/>
+      <c r="S53" s="76"/>
+      <c r="T53" s="76"/>
+      <c r="U53" s="76"/>
+      <c r="V53" s="76"/>
+      <c r="W53" s="76"/>
       <c r="X53" s="39"/>
       <c r="Y53" s="37" t="b">
         <v>0</v>
@@ -5079,7 +5986,7 @@
       <c r="C54" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="D54" s="114"/>
+      <c r="D54" s="68"/>
       <c r="E54" s="66" t="s">
         <v>119</v>
       </c>
@@ -5100,19 +6007,19 @@
       <c r="L54" s="23">
         <v>0</v>
       </c>
-      <c r="M54" s="112" t="s">
+      <c r="M54" s="80" t="s">
         <v>123</v>
       </c>
-      <c r="N54" s="113"/>
-      <c r="O54" s="113"/>
-      <c r="P54" s="113"/>
-      <c r="Q54" s="113"/>
-      <c r="R54" s="113"/>
-      <c r="S54" s="113"/>
-      <c r="T54" s="113"/>
-      <c r="U54" s="113"/>
-      <c r="V54" s="113"/>
-      <c r="W54" s="113"/>
+      <c r="N54" s="81"/>
+      <c r="O54" s="81"/>
+      <c r="P54" s="81"/>
+      <c r="Q54" s="81"/>
+      <c r="R54" s="81"/>
+      <c r="S54" s="81"/>
+      <c r="T54" s="81"/>
+      <c r="U54" s="81"/>
+      <c r="V54" s="81"/>
+      <c r="W54" s="81"/>
       <c r="X54" s="58"/>
       <c r="Y54" s="61" t="b">
         <v>0</v>
@@ -5129,19 +6036,138 @@
     </row>
   </sheetData>
   <mergeCells count="169">
-    <mergeCell ref="Y39:AB39"/>
-    <mergeCell ref="Y40:AB40"/>
-    <mergeCell ref="Y41:AB41"/>
-    <mergeCell ref="Y42:AB42"/>
-    <mergeCell ref="Y43:AB43"/>
-    <mergeCell ref="Y44:AB44"/>
-    <mergeCell ref="Y45:AB45"/>
-    <mergeCell ref="Y46:AB46"/>
-    <mergeCell ref="P39:W39"/>
-    <mergeCell ref="P40:W40"/>
-    <mergeCell ref="P41:W41"/>
-    <mergeCell ref="P42:W42"/>
-    <mergeCell ref="P43:W43"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="U7:W7"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="R31:T31"/>
+    <mergeCell ref="U31:W31"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="M4:Q4"/>
+    <mergeCell ref="M5:Q5"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="U20:W20"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="U21:W21"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:W11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="P12:W12"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="Q36:W36"/>
+    <mergeCell ref="Q37:W37"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="U30:W30"/>
+    <mergeCell ref="U27:W27"/>
+    <mergeCell ref="L35:R35"/>
+    <mergeCell ref="S35:W35"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="U25:W25"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="U26:W26"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="L47:O47"/>
+    <mergeCell ref="L48:O48"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:O40"/>
+    <mergeCell ref="L41:O41"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="L43:O43"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="U28:W28"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="U29:W29"/>
+    <mergeCell ref="R30:T30"/>
+    <mergeCell ref="P44:W44"/>
+    <mergeCell ref="P45:W45"/>
+    <mergeCell ref="P46:W46"/>
+    <mergeCell ref="P47:W47"/>
+    <mergeCell ref="P48:W48"/>
+    <mergeCell ref="L38:O38"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="L45:O45"/>
+    <mergeCell ref="L46:O46"/>
+    <mergeCell ref="L49:O49"/>
+    <mergeCell ref="L50:O50"/>
+    <mergeCell ref="L51:O51"/>
+    <mergeCell ref="L52:O52"/>
+    <mergeCell ref="P49:W49"/>
+    <mergeCell ref="P50:W50"/>
+    <mergeCell ref="P51:W51"/>
+    <mergeCell ref="P52:W52"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="P53:W53"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="P13:W13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="P14:W14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="Y47:AB47"/>
     <mergeCell ref="Y48:AB48"/>
     <mergeCell ref="Y49:AB49"/>
@@ -5166,138 +6192,19 @@
     <mergeCell ref="R15:W15"/>
     <mergeCell ref="L32:N32"/>
     <mergeCell ref="O32:W32"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P13:W13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="P14:W14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="L49:O49"/>
-    <mergeCell ref="L50:O50"/>
-    <mergeCell ref="L51:O51"/>
-    <mergeCell ref="L52:O52"/>
-    <mergeCell ref="P49:W49"/>
-    <mergeCell ref="P50:W50"/>
-    <mergeCell ref="P51:W51"/>
-    <mergeCell ref="P52:W52"/>
-    <mergeCell ref="L53:O53"/>
-    <mergeCell ref="P53:W53"/>
-    <mergeCell ref="L47:O47"/>
-    <mergeCell ref="L48:O48"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:O40"/>
-    <mergeCell ref="L41:O41"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="L43:O43"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="U28:W28"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="U29:W29"/>
-    <mergeCell ref="R30:T30"/>
-    <mergeCell ref="P44:W44"/>
-    <mergeCell ref="P45:W45"/>
-    <mergeCell ref="P46:W46"/>
-    <mergeCell ref="P47:W47"/>
-    <mergeCell ref="P48:W48"/>
-    <mergeCell ref="L38:O38"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="L45:O45"/>
-    <mergeCell ref="L46:O46"/>
-    <mergeCell ref="P12:W12"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="Q36:W36"/>
-    <mergeCell ref="Q37:W37"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="U30:W30"/>
-    <mergeCell ref="U27:W27"/>
-    <mergeCell ref="L35:R35"/>
-    <mergeCell ref="S35:W35"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="U25:W25"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="U26:W26"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="U20:W20"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="U21:W21"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="U4:W4"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:W11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="Y6:AB6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="U7:W7"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="U9:W9"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="R31:T31"/>
-    <mergeCell ref="U31:W31"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="M5:Q5"/>
-    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="Y39:AB39"/>
+    <mergeCell ref="Y40:AB40"/>
+    <mergeCell ref="Y41:AB41"/>
+    <mergeCell ref="Y42:AB42"/>
+    <mergeCell ref="Y43:AB43"/>
+    <mergeCell ref="Y44:AB44"/>
+    <mergeCell ref="Y45:AB45"/>
+    <mergeCell ref="Y46:AB46"/>
+    <mergeCell ref="P39:W39"/>
+    <mergeCell ref="P40:W40"/>
+    <mergeCell ref="P41:W41"/>
+    <mergeCell ref="P42:W42"/>
+    <mergeCell ref="P43:W43"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5474,20 +6381,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b05417e1-eb89-4392-aea8-ecdaf8fc0423" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b05417e1-eb89-4392-aea8-ecdaf8fc0423" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5509,6 +6416,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEFCFB9-977F-4BC6-8CD6-7A1E4BA64254}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE327FA-98F8-4626-AE66-90F799A55F58}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5522,12 +6437,4 @@
     <ds:schemaRef ds:uri="b05417e1-eb89-4392-aea8-ecdaf8fc0423"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEFCFB9-977F-4BC6-8CD6-7A1E4BA64254}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>